<commit_message>
moved incrementing logic into the PC module
</commit_message>
<xml_diff>
--- a/doc/decoding.xlsx
+++ b/doc/decoding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\SystemVerilog\FRiscV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A81521F-CDC0-43E7-A5D8-FD26F9A9A4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B6E9F7-0074-4CCE-B152-90B9D0EA0C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29835" yWindow="735" windowWidth="20805" windowHeight="11835" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
+    <workbookView xWindow="2085" yWindow="1785" windowWidth="25965" windowHeight="13860" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
     <t>R-TYPE</t>
   </si>
@@ -222,6 +222,24 @@
   </si>
   <si>
     <t>JAL</t>
+  </si>
+  <si>
+    <t>pcSrc</t>
+  </si>
+  <si>
+    <t>regWr</t>
+  </si>
+  <si>
+    <t>memWr</t>
+  </si>
+  <si>
+    <t>resSrc</t>
+  </si>
+  <si>
+    <t>Main Control Signals</t>
+  </si>
+  <si>
+    <t>aluSrc</t>
   </si>
 </sst>
 </file>
@@ -321,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -530,11 +548,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,39 +584,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -623,86 +623,126 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1019,10 +1059,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA95D64-5055-4174-A4D5-0BDBECB18FB0}">
-  <dimension ref="D2:AU33"/>
+  <dimension ref="D2:BA33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11:T11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="7" ySplit="19" topLeftCell="P24" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A5" sqref="A5"/>
+      <selection pane="topRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="AW32" sqref="AW32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1033,52 +1077,58 @@
     <col min="20" max="20" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="21" max="32" width="4.7109375" style="3"/>
     <col min="33" max="33" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="4.7109375" style="3"/>
+    <col min="34" max="48" width="4.7109375" style="3"/>
+    <col min="49" max="49" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="4.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP2" s="45" t="s">
+      <c r="AP2" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="AQ2" s="46"/>
-      <c r="AR2" s="46"/>
-      <c r="AS2" s="46"/>
-      <c r="AT2" s="46"/>
-      <c r="AU2" s="47"/>
+      <c r="AQ2" s="41"/>
+      <c r="AR2" s="41"/>
+      <c r="AS2" s="41"/>
+      <c r="AT2" s="41"/>
+      <c r="AU2" s="42"/>
     </row>
     <row r="3" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP3" s="35" t="s">
+      <c r="AP3" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="36"/>
-      <c r="AR3" s="41">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="41">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="41">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="42">
+      <c r="AQ3" s="48"/>
+      <c r="AR3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP4" s="37" t="s">
+      <c r="AP4" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="AQ4" s="38"/>
-      <c r="AR4" s="41">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="41">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="41">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="42">
+      <c r="AQ4" s="46"/>
+      <c r="AR4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="21">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1179,20 +1229,20 @@
       <c r="AN5" s="2">
         <v>0</v>
       </c>
-      <c r="AP5" s="37" t="s">
+      <c r="AP5" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="AQ5" s="38"/>
-      <c r="AR5" s="41">
-        <v>0</v>
-      </c>
-      <c r="AS5" s="41">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="41">
-        <v>1</v>
-      </c>
-      <c r="AU5" s="42">
+      <c r="AQ5" s="46"/>
+      <c r="AR5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="21">
+        <v>1</v>
+      </c>
+      <c r="AU5" s="22">
         <v>0</v>
       </c>
     </row>
@@ -1229,20 +1279,20 @@
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
-      <c r="AP6" s="37" t="s">
+      <c r="AP6" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="AQ6" s="38"/>
-      <c r="AR6" s="41">
-        <v>0</v>
-      </c>
-      <c r="AS6" s="41">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="41">
-        <v>1</v>
-      </c>
-      <c r="AU6" s="42">
+      <c r="AQ6" s="46"/>
+      <c r="AR6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="21">
+        <v>1</v>
+      </c>
+      <c r="AU6" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1283,88 +1333,88 @@
       <c r="AN7" s="3">
         <v>0</v>
       </c>
-      <c r="AP7" s="37" t="s">
+      <c r="AP7" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="AQ7" s="38"/>
-      <c r="AR7" s="41">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="41">
-        <v>1</v>
-      </c>
-      <c r="AT7" s="41">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="42">
+      <c r="AQ7" s="46"/>
+      <c r="AR7" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="21">
+        <v>1</v>
+      </c>
+      <c r="AT7" s="21">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="I8" s="7" t="s">
+      <c r="D8" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="I8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="10" t="s">
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="10" t="s">
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="10" t="s">
+      <c r="V8" s="36"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="37"/>
+      <c r="Z8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="10" t="s">
+      <c r="AA8" s="36"/>
+      <c r="AB8" s="37"/>
+      <c r="AC8" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="10" t="s">
+      <c r="AD8" s="36"/>
+      <c r="AE8" s="36"/>
+      <c r="AF8" s="36"/>
+      <c r="AG8" s="37"/>
+      <c r="AH8" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="8"/>
-      <c r="AN8" s="11"/>
-      <c r="AP8" s="37" t="s">
+      <c r="AI8" s="36"/>
+      <c r="AJ8" s="36"/>
+      <c r="AK8" s="36"/>
+      <c r="AL8" s="36"/>
+      <c r="AM8" s="36"/>
+      <c r="AN8" s="49"/>
+      <c r="AP8" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="AQ8" s="38"/>
-      <c r="AR8" s="41">
-        <v>0</v>
-      </c>
-      <c r="AS8" s="41">
-        <v>1</v>
-      </c>
-      <c r="AT8" s="41">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="42">
+      <c r="AQ8" s="46"/>
+      <c r="AR8" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="21">
+        <v>1</v>
+      </c>
+      <c r="AT8" s="21">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="22">
         <v>1</v>
       </c>
     </row>
@@ -1405,20 +1455,20 @@
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
-      <c r="AP9" s="37" t="s">
+      <c r="AP9" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="AQ9" s="38"/>
-      <c r="AR9" s="41">
-        <v>0</v>
-      </c>
-      <c r="AS9" s="41">
-        <v>1</v>
-      </c>
-      <c r="AT9" s="41">
-        <v>1</v>
-      </c>
-      <c r="AU9" s="42">
+      <c r="AQ9" s="46"/>
+      <c r="AR9" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AT9" s="21">
+        <v>1</v>
+      </c>
+      <c r="AU9" s="22">
         <v>0</v>
       </c>
     </row>
@@ -1457,86 +1507,86 @@
       <c r="AN10" s="3">
         <v>0</v>
       </c>
-      <c r="AP10" s="37" t="s">
+      <c r="AP10" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="AQ10" s="38"/>
-      <c r="AR10" s="41">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="41">
-        <v>1</v>
-      </c>
-      <c r="AT10" s="41">
-        <v>1</v>
-      </c>
-      <c r="AU10" s="42">
+      <c r="AQ10" s="46"/>
+      <c r="AR10" s="21">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AT10" s="21">
+        <v>1</v>
+      </c>
+      <c r="AU10" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="I11" s="7" t="s">
+      <c r="D11" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="I11" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="10" t="s">
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="10" t="s">
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="36"/>
+      <c r="Y11" s="37"/>
+      <c r="Z11" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AA11" s="8"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="10" t="s">
+      <c r="AA11" s="36"/>
+      <c r="AB11" s="37"/>
+      <c r="AC11" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AD11" s="8"/>
-      <c r="AE11" s="8"/>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="9"/>
-      <c r="AH11" s="10" t="s">
+      <c r="AD11" s="36"/>
+      <c r="AE11" s="36"/>
+      <c r="AF11" s="36"/>
+      <c r="AG11" s="37"/>
+      <c r="AH11" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AI11" s="8"/>
-      <c r="AJ11" s="8"/>
-      <c r="AK11" s="8"/>
-      <c r="AL11" s="8"/>
-      <c r="AM11" s="8"/>
-      <c r="AN11" s="11"/>
-      <c r="AP11" s="39" t="s">
+      <c r="AI11" s="36"/>
+      <c r="AJ11" s="36"/>
+      <c r="AK11" s="36"/>
+      <c r="AL11" s="36"/>
+      <c r="AM11" s="36"/>
+      <c r="AN11" s="49"/>
+      <c r="AP11" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="AQ11" s="40"/>
-      <c r="AR11" s="43">
-        <v>1</v>
-      </c>
-      <c r="AS11" s="43">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="43">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="44">
+      <c r="AQ11" s="44"/>
+      <c r="AR11" s="23">
+        <v>1</v>
+      </c>
+      <c r="AS11" s="23">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="23">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="24">
         <v>0</v>
       </c>
     </row>
@@ -1621,56 +1671,56 @@
       </c>
     </row>
     <row r="14" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="I14" s="7" t="s">
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="I14" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="10" t="s">
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="10" t="s">
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="10" t="s">
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="37"/>
+      <c r="Z14" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="10" t="s">
+      <c r="AA14" s="36"/>
+      <c r="AB14" s="37"/>
+      <c r="AC14" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-      <c r="AF14" s="8"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="10" t="s">
+      <c r="AD14" s="36"/>
+      <c r="AE14" s="36"/>
+      <c r="AF14" s="36"/>
+      <c r="AG14" s="37"/>
+      <c r="AH14" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AI14" s="8"/>
-      <c r="AJ14" s="8"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="8"/>
-      <c r="AM14" s="8"/>
-      <c r="AN14" s="11"/>
+      <c r="AI14" s="36"/>
+      <c r="AJ14" s="36"/>
+      <c r="AK14" s="36"/>
+      <c r="AL14" s="36"/>
+      <c r="AM14" s="36"/>
+      <c r="AN14" s="49"/>
     </row>
     <row r="15" spans="4:47" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
@@ -1755,63 +1805,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="14" t="s">
+    <row r="17" spans="4:53" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="I17" s="32" t="s">
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="I17" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="10" t="s">
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="10" t="s">
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="10" t="s">
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="37"/>
+      <c r="Z17" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="10" t="s">
+      <c r="AA17" s="36"/>
+      <c r="AB17" s="37"/>
+      <c r="AC17" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="AD17" s="8"/>
-      <c r="AE17" s="8"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="22" t="s">
+      <c r="AD17" s="36"/>
+      <c r="AE17" s="36"/>
+      <c r="AF17" s="37"/>
+      <c r="AG17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AH17" s="10" t="s">
+      <c r="AH17" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AI17" s="8"/>
-      <c r="AJ17" s="8"/>
-      <c r="AK17" s="8"/>
-      <c r="AL17" s="8"/>
-      <c r="AM17" s="8"/>
-      <c r="AN17" s="11"/>
-    </row>
-    <row r="18" spans="4:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="AI17" s="36"/>
+      <c r="AJ17" s="36"/>
+      <c r="AK17" s="36"/>
+      <c r="AL17" s="36"/>
+      <c r="AM17" s="36"/>
+      <c r="AN17" s="49"/>
+    </row>
+    <row r="18" spans="4:53" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1849,7 +1899,7 @@
       <c r="AM18" s="4"/>
       <c r="AN18" s="4"/>
     </row>
-    <row r="19" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1873,53 +1923,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="15" t="s">
+    <row r="20" spans="4:53" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="I20" s="7" t="s">
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="I20" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="8"/>
-      <c r="AA20" s="8"/>
-      <c r="AB20" s="9"/>
-      <c r="AC20" s="10" t="s">
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="36"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36"/>
+      <c r="Y20" s="36"/>
+      <c r="Z20" s="36"/>
+      <c r="AA20" s="36"/>
+      <c r="AB20" s="37"/>
+      <c r="AC20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AD20" s="8"/>
-      <c r="AE20" s="8"/>
-      <c r="AF20" s="8"/>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="10" t="s">
+      <c r="AD20" s="36"/>
+      <c r="AE20" s="36"/>
+      <c r="AF20" s="36"/>
+      <c r="AG20" s="37"/>
+      <c r="AH20" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AI20" s="8"/>
-      <c r="AJ20" s="8"/>
-      <c r="AK20" s="8"/>
-      <c r="AL20" s="8"/>
-      <c r="AM20" s="8"/>
-      <c r="AN20" s="11"/>
-    </row>
-    <row r="21" spans="4:47" ht="15" x14ac:dyDescent="0.25">
+      <c r="AI20" s="36"/>
+      <c r="AJ20" s="36"/>
+      <c r="AK20" s="36"/>
+      <c r="AL20" s="36"/>
+      <c r="AM20" s="36"/>
+      <c r="AN20" s="49"/>
+    </row>
+    <row r="21" spans="4:53" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1957,7 +2007,7 @@
       <c r="AM21" s="4"/>
       <c r="AN21" s="4"/>
     </row>
-    <row r="22" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1993,702 +2043,839 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="16" t="s">
+    <row r="23" spans="4:53" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="I23" s="17" t="s">
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="I23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="J23" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="18" t="s">
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U23" s="10" t="s">
+      <c r="U23" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
-      <c r="AA23" s="8"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="10" t="s">
+      <c r="V23" s="36"/>
+      <c r="W23" s="36"/>
+      <c r="X23" s="36"/>
+      <c r="Y23" s="36"/>
+      <c r="Z23" s="36"/>
+      <c r="AA23" s="36"/>
+      <c r="AB23" s="37"/>
+      <c r="AC23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AD23" s="8"/>
-      <c r="AE23" s="8"/>
-      <c r="AF23" s="8"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="10" t="s">
+      <c r="AD23" s="36"/>
+      <c r="AE23" s="36"/>
+      <c r="AF23" s="36"/>
+      <c r="AG23" s="37"/>
+      <c r="AH23" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="AI23" s="8"/>
-      <c r="AJ23" s="8"/>
-      <c r="AK23" s="8"/>
-      <c r="AL23" s="8"/>
-      <c r="AM23" s="8"/>
-      <c r="AN23" s="11"/>
-    </row>
-    <row r="26" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AP26" s="49" t="s">
+      <c r="AI23" s="36"/>
+      <c r="AJ23" s="36"/>
+      <c r="AK23" s="36"/>
+      <c r="AL23" s="36"/>
+      <c r="AM23" s="36"/>
+      <c r="AN23" s="49"/>
+    </row>
+    <row r="25" spans="4:53" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW25" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX25" s="60"/>
+      <c r="AY25" s="60"/>
+      <c r="AZ25" s="60"/>
+      <c r="BA25" s="60"/>
+    </row>
+    <row r="26" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AP26" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="AQ26" s="49"/>
-      <c r="AR26" s="49"/>
-      <c r="AS26" s="49"/>
-      <c r="AT26" s="48"/>
-      <c r="AU26" s="48"/>
-    </row>
-    <row r="27" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="30" t="s">
+      <c r="AQ26" s="39"/>
+      <c r="AR26" s="39"/>
+      <c r="AS26" s="39"/>
+      <c r="AT26" s="25"/>
+      <c r="AU26" s="25"/>
+      <c r="AW26" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX26" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY26" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ26" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA26" s="59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31" t="s">
+      <c r="E27" s="34"/>
+      <c r="F27" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I27" s="25">
-        <v>0</v>
-      </c>
-      <c r="J27" s="20">
-        <v>0</v>
-      </c>
-      <c r="K27" s="20">
-        <v>0</v>
-      </c>
-      <c r="L27" s="20">
-        <v>0</v>
-      </c>
-      <c r="M27" s="20">
-        <v>0</v>
-      </c>
-      <c r="N27" s="20">
-        <v>0</v>
-      </c>
-      <c r="O27" s="21">
-        <v>0</v>
-      </c>
-      <c r="P27" s="10" t="s">
+      <c r="I27" s="14">
+        <v>0</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0</v>
+      </c>
+      <c r="N27" s="9">
+        <v>0</v>
+      </c>
+      <c r="O27" s="10">
+        <v>0</v>
+      </c>
+      <c r="P27" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="10" t="s">
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="27">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="28">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="29">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="10" t="s">
+      <c r="V27" s="36"/>
+      <c r="W27" s="36"/>
+      <c r="X27" s="36"/>
+      <c r="Y27" s="37"/>
+      <c r="Z27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AD27" s="8"/>
-      <c r="AE27" s="8"/>
-      <c r="AF27" s="8"/>
-      <c r="AG27" s="9"/>
-      <c r="AH27" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI27" s="20">
-        <v>1</v>
-      </c>
-      <c r="AJ27" s="20">
-        <v>1</v>
-      </c>
-      <c r="AK27" s="20">
-        <v>0</v>
-      </c>
-      <c r="AL27" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM27" s="20">
-        <v>1</v>
-      </c>
-      <c r="AN27" s="26">
-        <v>1</v>
-      </c>
-      <c r="AP27" s="50">
-        <v>0</v>
-      </c>
-      <c r="AQ27" s="51">
-        <v>0</v>
-      </c>
-      <c r="AR27" s="51">
-        <v>1</v>
-      </c>
-      <c r="AS27" s="52">
-        <v>1</v>
-      </c>
-      <c r="AT27" s="34" t="s">
+      <c r="AD27" s="36"/>
+      <c r="AE27" s="36"/>
+      <c r="AF27" s="36"/>
+      <c r="AG27" s="37"/>
+      <c r="AH27" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AK27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM27" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN27" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP27" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="AU27" s="33"/>
-    </row>
-    <row r="28" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="30" t="s">
+      <c r="AQ27" s="56"/>
+      <c r="AR27" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS27" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT27" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU27" s="28">
+        <v>1</v>
+      </c>
+      <c r="AW27" s="57">
+        <v>1</v>
+      </c>
+      <c r="AX27" s="57">
+        <v>1</v>
+      </c>
+      <c r="AY27" s="57">
+        <v>0</v>
+      </c>
+      <c r="AZ27" s="57">
+        <v>0</v>
+      </c>
+      <c r="BA27" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31" t="s">
+      <c r="E28" s="34"/>
+      <c r="F28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="25">
-        <v>0</v>
-      </c>
-      <c r="J28" s="20">
-        <v>1</v>
-      </c>
-      <c r="K28" s="20">
-        <v>0</v>
-      </c>
-      <c r="L28" s="20">
-        <v>0</v>
-      </c>
-      <c r="M28" s="20">
-        <v>0</v>
-      </c>
-      <c r="N28" s="20">
-        <v>0</v>
-      </c>
-      <c r="O28" s="21">
-        <v>0</v>
-      </c>
-      <c r="P28" s="10" t="s">
+      <c r="I28" s="14">
+        <v>0</v>
+      </c>
+      <c r="J28" s="9">
+        <v>1</v>
+      </c>
+      <c r="K28" s="9">
+        <v>0</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0</v>
+      </c>
+      <c r="N28" s="9">
+        <v>0</v>
+      </c>
+      <c r="O28" s="10">
+        <v>0</v>
+      </c>
+      <c r="P28" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="10" t="s">
+      <c r="Q28" s="36"/>
+      <c r="R28" s="36"/>
+      <c r="S28" s="36"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="9"/>
-      <c r="Z28" s="27">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="28">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="29">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="10" t="s">
+      <c r="V28" s="36"/>
+      <c r="W28" s="36"/>
+      <c r="X28" s="36"/>
+      <c r="Y28" s="37"/>
+      <c r="Z28" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AD28" s="8"/>
-      <c r="AE28" s="8"/>
-      <c r="AF28" s="8"/>
-      <c r="AG28" s="9"/>
-      <c r="AH28" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI28" s="20">
-        <v>1</v>
-      </c>
-      <c r="AJ28" s="20">
-        <v>1</v>
-      </c>
-      <c r="AK28" s="20">
-        <v>0</v>
-      </c>
-      <c r="AL28" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM28" s="20">
-        <v>1</v>
-      </c>
-      <c r="AN28" s="26">
-        <v>1</v>
-      </c>
-      <c r="AP28" s="53">
-        <v>0</v>
-      </c>
-      <c r="AQ28" s="54">
-        <v>1</v>
-      </c>
-      <c r="AR28" s="54">
-        <v>0</v>
-      </c>
-      <c r="AS28" s="55">
-        <v>0</v>
-      </c>
-      <c r="AT28" s="34" t="s">
+      <c r="AD28" s="36"/>
+      <c r="AE28" s="36"/>
+      <c r="AF28" s="36"/>
+      <c r="AG28" s="37"/>
+      <c r="AH28" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ28" s="9">
+        <v>1</v>
+      </c>
+      <c r="AK28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM28" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN28" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP28" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="AU28" s="33"/>
-    </row>
-    <row r="29" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="30" t="s">
+      <c r="AQ28" s="56"/>
+      <c r="AR28" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS28" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT28" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU28" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW28" s="57">
+        <v>1</v>
+      </c>
+      <c r="AX28" s="57">
+        <v>1</v>
+      </c>
+      <c r="AY28" s="57">
+        <v>0</v>
+      </c>
+      <c r="AZ28" s="57">
+        <v>0</v>
+      </c>
+      <c r="BA28" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="23" t="s">
+      <c r="E29" s="34"/>
+      <c r="F29" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="10" t="s">
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="9"/>
-      <c r="Z29" s="27">
-        <v>0</v>
-      </c>
-      <c r="AA29" s="28">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="29">
-        <v>0</v>
-      </c>
-      <c r="AC29" s="10" t="s">
+      <c r="V29" s="36"/>
+      <c r="W29" s="36"/>
+      <c r="X29" s="36"/>
+      <c r="Y29" s="37"/>
+      <c r="Z29" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AD29" s="8"/>
-      <c r="AE29" s="8"/>
-      <c r="AF29" s="8"/>
-      <c r="AG29" s="9"/>
-      <c r="AH29" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI29" s="20">
-        <v>0</v>
-      </c>
-      <c r="AJ29" s="20">
-        <v>1</v>
-      </c>
-      <c r="AK29" s="20">
-        <v>0</v>
-      </c>
-      <c r="AL29" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM29" s="20">
-        <v>1</v>
-      </c>
-      <c r="AN29" s="26">
-        <v>1</v>
-      </c>
-      <c r="AP29" s="53">
-        <v>0</v>
-      </c>
-      <c r="AQ29" s="54">
-        <v>0</v>
-      </c>
-      <c r="AR29" s="54">
-        <v>1</v>
-      </c>
-      <c r="AS29" s="55">
-        <v>1</v>
-      </c>
-      <c r="AT29" s="34" t="s">
+      <c r="AD29" s="36"/>
+      <c r="AE29" s="36"/>
+      <c r="AF29" s="36"/>
+      <c r="AG29" s="37"/>
+      <c r="AH29" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ29" s="9">
+        <v>1</v>
+      </c>
+      <c r="AK29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN29" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP29" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="AU29" s="33"/>
-    </row>
-    <row r="30" spans="4:47" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="30" t="s">
+      <c r="AQ29" s="56"/>
+      <c r="AR29" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS29" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT29" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU29" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW29" s="57">
+        <v>1</v>
+      </c>
+      <c r="AX29" s="57">
+        <v>1</v>
+      </c>
+      <c r="AY29" s="57">
+        <v>1</v>
+      </c>
+      <c r="AZ29" s="57">
+        <v>0</v>
+      </c>
+      <c r="BA29" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="4:53" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="30"/>
-      <c r="F30" s="23" t="s">
+      <c r="E30" s="34"/>
+      <c r="F30" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="7" t="s">
+      <c r="I30" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="10" t="s">
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="37"/>
+      <c r="U30" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="9"/>
-      <c r="Z30" s="27">
-        <v>0</v>
-      </c>
-      <c r="AA30" s="28">
-        <v>1</v>
-      </c>
-      <c r="AB30" s="29">
-        <v>0</v>
-      </c>
-      <c r="AC30" s="10" t="s">
+      <c r="V30" s="36"/>
+      <c r="W30" s="36"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="37"/>
+      <c r="Z30" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AD30" s="8"/>
-      <c r="AE30" s="8"/>
-      <c r="AF30" s="8"/>
-      <c r="AG30" s="9"/>
-      <c r="AH30" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI30" s="20">
-        <v>0</v>
-      </c>
-      <c r="AJ30" s="20">
-        <v>0</v>
-      </c>
-      <c r="AK30" s="20">
-        <v>0</v>
-      </c>
-      <c r="AL30" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM30" s="20">
-        <v>1</v>
-      </c>
-      <c r="AN30" s="26">
-        <v>1</v>
-      </c>
-      <c r="AP30" s="53">
-        <v>0</v>
-      </c>
-      <c r="AQ30" s="54">
-        <v>0</v>
-      </c>
-      <c r="AR30" s="54">
-        <v>1</v>
-      </c>
-      <c r="AS30" s="55">
-        <v>1</v>
-      </c>
-      <c r="AT30" s="34" t="s">
+      <c r="AD30" s="36"/>
+      <c r="AE30" s="36"/>
+      <c r="AF30" s="36"/>
+      <c r="AG30" s="37"/>
+      <c r="AH30" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN30" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP30" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="AU30" s="33"/>
-    </row>
-    <row r="31" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="30" t="s">
+      <c r="AQ30" s="56"/>
+      <c r="AR30" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS30" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT30" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU30" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW30" s="57">
+        <v>1</v>
+      </c>
+      <c r="AX30" s="57">
+        <v>1</v>
+      </c>
+      <c r="AY30" s="57">
+        <v>1</v>
+      </c>
+      <c r="AZ30" s="57">
+        <v>0</v>
+      </c>
+      <c r="BA30" s="57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="24" t="s">
+      <c r="E31" s="34"/>
+      <c r="F31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I31" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="10" t="s">
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="37"/>
+      <c r="P31" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="10" t="s">
+      <c r="Q31" s="36"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="36"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA31" s="20">
-        <v>1</v>
-      </c>
-      <c r="AB31" s="21">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="10" t="s">
+      <c r="V31" s="36"/>
+      <c r="W31" s="36"/>
+      <c r="X31" s="36"/>
+      <c r="Y31" s="37"/>
+      <c r="Z31" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="AD31" s="8"/>
-      <c r="AE31" s="8"/>
-      <c r="AF31" s="8"/>
-      <c r="AG31" s="9"/>
-      <c r="AH31" s="19">
-        <v>0</v>
-      </c>
-      <c r="AI31" s="20">
-        <v>1</v>
-      </c>
-      <c r="AJ31" s="20">
-        <v>0</v>
-      </c>
-      <c r="AK31" s="20">
-        <v>0</v>
-      </c>
-      <c r="AL31" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM31" s="20">
-        <v>1</v>
-      </c>
-      <c r="AN31" s="26">
-        <v>1</v>
-      </c>
-      <c r="AP31" s="53">
-        <v>0</v>
-      </c>
-      <c r="AQ31" s="54">
-        <v>0</v>
-      </c>
-      <c r="AR31" s="54">
-        <v>1</v>
-      </c>
-      <c r="AS31" s="55">
-        <v>1</v>
-      </c>
-      <c r="AT31" s="34" t="s">
+      <c r="AD31" s="36"/>
+      <c r="AE31" s="36"/>
+      <c r="AF31" s="36"/>
+      <c r="AG31" s="37"/>
+      <c r="AH31" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN31" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP31" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="AU31" s="33"/>
-    </row>
-    <row r="32" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="30" t="s">
+      <c r="AQ31" s="56"/>
+      <c r="AR31" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS31" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT31" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU31" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW31" s="57">
+        <v>1</v>
+      </c>
+      <c r="AX31" s="57">
+        <v>0</v>
+      </c>
+      <c r="AY31" s="57">
+        <v>1</v>
+      </c>
+      <c r="AZ31" s="57">
+        <v>1</v>
+      </c>
+      <c r="BA31" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="56" t="s">
+      <c r="E32" s="34"/>
+      <c r="F32" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="I32" s="25" t="s">
+      <c r="I32" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J32" s="7" t="s">
+      <c r="J32" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="10" t="s">
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="10" t="s">
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="36"/>
+      <c r="T32" s="37"/>
+      <c r="U32" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA32" s="20">
-        <v>0</v>
-      </c>
-      <c r="AB32" s="21">
-        <v>0</v>
-      </c>
-      <c r="AC32" s="10" t="s">
+      <c r="V32" s="36"/>
+      <c r="W32" s="36"/>
+      <c r="X32" s="36"/>
+      <c r="Y32" s="37"/>
+      <c r="Z32" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="AD32" s="8"/>
-      <c r="AE32" s="8"/>
-      <c r="AF32" s="9"/>
-      <c r="AG32" s="21" t="s">
+      <c r="AD32" s="36"/>
+      <c r="AE32" s="36"/>
+      <c r="AF32" s="37"/>
+      <c r="AG32" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AH32" s="19">
-        <v>1</v>
-      </c>
-      <c r="AI32" s="20">
-        <v>1</v>
-      </c>
-      <c r="AJ32" s="20">
-        <v>0</v>
-      </c>
-      <c r="AK32" s="20">
-        <v>0</v>
-      </c>
-      <c r="AL32" s="20">
-        <v>0</v>
-      </c>
-      <c r="AM32" s="20">
-        <v>1</v>
-      </c>
-      <c r="AN32" s="26">
-        <v>1</v>
-      </c>
-      <c r="AP32" s="53">
-        <v>0</v>
-      </c>
-      <c r="AQ32" s="54">
-        <v>1</v>
-      </c>
-      <c r="AR32" s="54">
-        <v>0</v>
-      </c>
-      <c r="AS32" s="55">
-        <v>0</v>
-      </c>
-      <c r="AT32" s="34" t="s">
+      <c r="AH32" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI32" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN32" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP32" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="AU32" s="33"/>
-    </row>
-    <row r="33" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="30" t="s">
+      <c r="AQ32" s="56"/>
+      <c r="AR32" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS32" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT32" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU32" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW32" s="57"/>
+      <c r="AX32" s="57"/>
+      <c r="AY32" s="57"/>
+      <c r="AZ32" s="57"/>
+      <c r="BA32" s="57"/>
+    </row>
+    <row r="33" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="57" t="s">
+      <c r="E33" s="34"/>
+      <c r="F33" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="I33" s="17" t="s">
+      <c r="I33" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J33" s="10" t="s">
+      <c r="J33" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="18" t="s">
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U33" s="10" t="s">
+      <c r="U33" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
-      <c r="AB33" s="9"/>
-      <c r="AC33" s="10" t="s">
+      <c r="V33" s="36"/>
+      <c r="W33" s="36"/>
+      <c r="X33" s="36"/>
+      <c r="Y33" s="36"/>
+      <c r="Z33" s="36"/>
+      <c r="AA33" s="36"/>
+      <c r="AB33" s="37"/>
+      <c r="AC33" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="AD33" s="8"/>
-      <c r="AE33" s="8"/>
-      <c r="AF33" s="8"/>
-      <c r="AG33" s="9"/>
-      <c r="AH33" s="19">
-        <v>1</v>
-      </c>
-      <c r="AI33" s="20">
-        <v>1</v>
-      </c>
-      <c r="AJ33" s="20">
-        <v>0</v>
-      </c>
-      <c r="AK33" s="20">
-        <v>1</v>
-      </c>
-      <c r="AL33" s="20">
-        <v>1</v>
-      </c>
-      <c r="AM33" s="20">
-        <v>1</v>
-      </c>
-      <c r="AN33" s="26">
-        <v>1</v>
-      </c>
-      <c r="AP33" s="53">
-        <v>0</v>
-      </c>
-      <c r="AQ33" s="54">
-        <v>0</v>
-      </c>
-      <c r="AR33" s="54">
-        <v>1</v>
-      </c>
-      <c r="AS33" s="55">
-        <v>1</v>
-      </c>
-      <c r="AT33" s="34" t="s">
+      <c r="AD33" s="36"/>
+      <c r="AE33" s="36"/>
+      <c r="AF33" s="36"/>
+      <c r="AG33" s="37"/>
+      <c r="AH33" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN33" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP33" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="AU33" s="33"/>
+      <c r="AQ33" s="56"/>
+      <c r="AR33" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS33" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT33" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU33" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW33" s="57"/>
+      <c r="AX33" s="57"/>
+      <c r="AY33" s="57"/>
+      <c r="AZ33" s="57"/>
+      <c r="BA33" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="84">
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="AT33:AU33"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="U33:AB33"/>
-    <mergeCell ref="AC33:AG33"/>
-    <mergeCell ref="J32:O32"/>
-    <mergeCell ref="AT27:AU27"/>
-    <mergeCell ref="AT28:AU28"/>
-    <mergeCell ref="AT29:AU29"/>
-    <mergeCell ref="AT30:AU30"/>
-    <mergeCell ref="AT31:AU31"/>
-    <mergeCell ref="AT32:AU32"/>
-    <mergeCell ref="AP26:AS26"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="P32:T32"/>
-    <mergeCell ref="U32:Y32"/>
-    <mergeCell ref="AC32:AF32"/>
+  <mergeCells count="85">
+    <mergeCell ref="AW25:BA25"/>
+    <mergeCell ref="AP27:AQ27"/>
+    <mergeCell ref="AP28:AQ28"/>
+    <mergeCell ref="AP29:AQ29"/>
+    <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="AP31:AQ31"/>
+    <mergeCell ref="AP32:AQ32"/>
+    <mergeCell ref="AP33:AQ33"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="I8:O8"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="U8:Y8"/>
+    <mergeCell ref="Z8:AB8"/>
+    <mergeCell ref="AC8:AG8"/>
+    <mergeCell ref="AH8:AN8"/>
+    <mergeCell ref="U11:Y11"/>
+    <mergeCell ref="Z11:AB11"/>
+    <mergeCell ref="AC11:AG11"/>
+    <mergeCell ref="AH11:AN11"/>
+    <mergeCell ref="AH14:AN14"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="I14:O14"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="AH23:AN23"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="AH17:AN17"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="AC20:AG20"/>
+    <mergeCell ref="AH20:AN20"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="AC30:AG30"/>
+    <mergeCell ref="P17:T17"/>
+    <mergeCell ref="U17:Y17"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="AC23:AG23"/>
+    <mergeCell ref="I11:T11"/>
+    <mergeCell ref="I20:AB20"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="U23:AB23"/>
+    <mergeCell ref="AC17:AF17"/>
+    <mergeCell ref="U14:Y14"/>
+    <mergeCell ref="Z14:AB14"/>
+    <mergeCell ref="AC14:AG14"/>
     <mergeCell ref="AP2:AU2"/>
     <mergeCell ref="AP11:AQ11"/>
     <mergeCell ref="AP10:AQ10"/>
@@ -2699,6 +2886,11 @@
     <mergeCell ref="AP5:AQ5"/>
     <mergeCell ref="AP4:AQ4"/>
     <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AP26:AS26"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="P32:T32"/>
+    <mergeCell ref="U32:Y32"/>
+    <mergeCell ref="AC32:AF32"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="U27:Y27"/>
     <mergeCell ref="AC27:AG27"/>
@@ -2710,6 +2902,7 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="I29:T29"/>
+    <mergeCell ref="J32:O32"/>
     <mergeCell ref="U29:Y29"/>
     <mergeCell ref="AC29:AG29"/>
     <mergeCell ref="I31:O31"/>
@@ -2717,45 +2910,12 @@
     <mergeCell ref="U31:Y31"/>
     <mergeCell ref="AC31:AG31"/>
     <mergeCell ref="I30:T30"/>
-    <mergeCell ref="I11:T11"/>
-    <mergeCell ref="I20:AB20"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="U23:AB23"/>
-    <mergeCell ref="AC17:AF17"/>
     <mergeCell ref="P27:T27"/>
     <mergeCell ref="U30:Y30"/>
-    <mergeCell ref="AC30:AG30"/>
-    <mergeCell ref="P17:T17"/>
-    <mergeCell ref="U17:Y17"/>
-    <mergeCell ref="Z17:AB17"/>
-    <mergeCell ref="AC23:AG23"/>
-    <mergeCell ref="AH23:AN23"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="AH17:AN17"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="AC20:AG20"/>
-    <mergeCell ref="AH20:AN20"/>
-    <mergeCell ref="U14:Y14"/>
-    <mergeCell ref="Z14:AB14"/>
-    <mergeCell ref="AC14:AG14"/>
-    <mergeCell ref="AH14:AN14"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="I14:O14"/>
-    <mergeCell ref="P14:T14"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="AC8:AG8"/>
-    <mergeCell ref="AH8:AN8"/>
-    <mergeCell ref="U11:Y11"/>
-    <mergeCell ref="Z11:AB11"/>
-    <mergeCell ref="AC11:AG11"/>
-    <mergeCell ref="AH11:AN11"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="I8:O8"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="U8:Y8"/>
-    <mergeCell ref="Z8:AB8"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="J33:S33"/>
+    <mergeCell ref="U33:AB33"/>
+    <mergeCell ref="AC33:AG33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
expanded design to implement JAL
</commit_message>
<xml_diff>
--- a/doc/decoding.xlsx
+++ b/doc/decoding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\SystemVerilog\FRiscV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B6E9F7-0074-4CCE-B152-90B9D0EA0C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DCFBA8-5272-41CF-8A72-F9FF186E2958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="1785" windowWidth="25965" windowHeight="13860" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,6 +61,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="AW32" authorId="0" shapeId="0" xr:uid="{EC372BE6-EF51-477F-B18A-BFF0C74E0CC5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+if zero is 1
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D33" authorId="0" shapeId="0" xr:uid="{94E066D9-6740-478B-B1BE-00F56432855D}">
       <text>
         <r>
@@ -90,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
   <si>
     <t>R-TYPE</t>
   </si>
@@ -240,6 +265,27 @@
   </si>
   <si>
     <t>aluSrc</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>Uses  Z?</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -567,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -743,6 +789,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1059,14 +1111,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA95D64-5055-4174-A4D5-0BDBECB18FB0}">
-  <dimension ref="D2:BA33"/>
+  <dimension ref="D2:BB33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="19" topLeftCell="P24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="19" topLeftCell="H24" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
       <selection pane="topRight" activeCell="H5" sqref="H5"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="AW32" sqref="AW32"/>
+      <selection pane="bottomRight" activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1083,7 +1135,8 @@
     <col min="51" max="51" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="4.7109375" style="3"/>
+    <col min="54" max="54" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="4.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:47" ht="15" x14ac:dyDescent="0.2">
@@ -1805,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:53" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="51" t="s">
         <v>3</v>
       </c>
@@ -1861,7 +1914,7 @@
       <c r="AM17" s="36"/>
       <c r="AN17" s="49"/>
     </row>
-    <row r="18" spans="4:53" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:54" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1899,7 +1952,7 @@
       <c r="AM18" s="4"/>
       <c r="AN18" s="4"/>
     </row>
-    <row r="19" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1923,7 +1976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:53" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="50" t="s">
         <v>4</v>
       </c>
@@ -1969,7 +2022,7 @@
       <c r="AM20" s="36"/>
       <c r="AN20" s="49"/>
     </row>
-    <row r="21" spans="4:53" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:54" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -2007,7 +2060,7 @@
       <c r="AM21" s="4"/>
       <c r="AN21" s="4"/>
     </row>
-    <row r="22" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -2043,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:53" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="54" t="s">
         <v>5</v>
       </c>
@@ -2095,7 +2148,7 @@
       <c r="AM23" s="36"/>
       <c r="AN23" s="49"/>
     </row>
-    <row r="25" spans="4:53" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:54" ht="15" x14ac:dyDescent="0.25">
       <c r="AW25" s="60" t="s">
         <v>48</v>
       </c>
@@ -2104,7 +2157,7 @@
       <c r="AZ25" s="60"/>
       <c r="BA25" s="60"/>
     </row>
-    <row r="26" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AP26" s="39" t="s">
         <v>41</v>
       </c>
@@ -2128,8 +2181,11 @@
       <c r="BA26" s="59" t="s">
         <v>47</v>
       </c>
+      <c r="BB26" s="59" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="27" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="34" t="s">
         <v>26</v>
       </c>
@@ -2237,11 +2293,14 @@
       <c r="AZ27" s="57">
         <v>0</v>
       </c>
-      <c r="BA27" s="57">
-        <v>0</v>
+      <c r="BA27" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB27" s="57" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="28" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="34" t="s">
         <v>28</v>
       </c>
@@ -2349,11 +2408,14 @@
       <c r="AZ28" s="57">
         <v>0</v>
       </c>
-      <c r="BA28" s="57">
-        <v>0</v>
+      <c r="BA28" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB28" s="57" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="29" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="34" t="s">
         <v>25</v>
       </c>
@@ -2447,11 +2509,14 @@
       <c r="AZ29" s="57">
         <v>0</v>
       </c>
-      <c r="BA29" s="57">
-        <v>0</v>
+      <c r="BA29" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB29" s="57" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="30" spans="4:53" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="34" t="s">
         <v>20</v>
       </c>
@@ -2545,11 +2610,14 @@
       <c r="AZ30" s="57">
         <v>0</v>
       </c>
-      <c r="BA30" s="57">
-        <v>1</v>
+      <c r="BA30" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB30" s="57" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="31" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="34" t="s">
         <v>21</v>
       </c>
@@ -2645,11 +2713,14 @@
       <c r="AZ31" s="57">
         <v>1</v>
       </c>
-      <c r="BA31" s="57">
-        <v>0</v>
+      <c r="BA31" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB31" s="57" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="32" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="34" t="s">
         <v>38</v>
       </c>
@@ -2737,13 +2808,26 @@
       <c r="AU32" s="31">
         <v>0</v>
       </c>
-      <c r="AW32" s="57"/>
-      <c r="AX32" s="57"/>
-      <c r="AY32" s="57"/>
-      <c r="AZ32" s="57"/>
-      <c r="BA32" s="57"/>
+      <c r="AW32" s="57">
+        <v>1</v>
+      </c>
+      <c r="AX32" s="57">
+        <v>0</v>
+      </c>
+      <c r="AY32" s="57">
+        <v>0</v>
+      </c>
+      <c r="AZ32" s="57">
+        <v>0</v>
+      </c>
+      <c r="BA32" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB32" s="57" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="33" spans="4:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D33" s="34" t="s">
         <v>43</v>
       </c>
@@ -2823,11 +2907,24 @@
       <c r="AU33" s="31">
         <v>1</v>
       </c>
-      <c r="AW33" s="57"/>
-      <c r="AX33" s="57"/>
-      <c r="AY33" s="57"/>
-      <c r="AZ33" s="57"/>
-      <c r="BA33" s="57"/>
+      <c r="AW33" s="57">
+        <v>0</v>
+      </c>
+      <c r="AX33" s="57">
+        <v>1</v>
+      </c>
+      <c r="AY33" s="57">
+        <v>1</v>
+      </c>
+      <c r="AZ33" s="57">
+        <v>0</v>
+      </c>
+      <c r="BA33" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB33" s="57" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="85">

</xml_diff>

<commit_message>
added R and immediate to decoding spreadsheet
</commit_message>
<xml_diff>
--- a/doc/decoding.xlsx
+++ b/doc/decoding.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\SystemVerilog\FRiscV\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\SV\FRiscV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EEFCC2-25DF-4C20-8289-97657FCB8484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BE3535-8985-4DAC-A826-2DD4567B1738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28035" windowHeight="16440" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="D32" authorId="0" shapeId="0" xr:uid="{E8182568-AF53-41D0-80C8-04611138DC73}">
+    <comment ref="D48" authorId="0" shapeId="0" xr:uid="{E8182568-AF53-41D0-80C8-04611138DC73}">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW32" authorId="0" shapeId="0" xr:uid="{EC372BE6-EF51-477F-B18A-BFF0C74E0CC5}">
+    <comment ref="AW48" authorId="0" shapeId="0" xr:uid="{EC372BE6-EF51-477F-B18A-BFF0C74E0CC5}">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D33" authorId="0" shapeId="0" xr:uid="{94E066D9-6740-478B-B1BE-00F56432855D}">
+    <comment ref="D49" authorId="0" shapeId="0" xr:uid="{94E066D9-6740-478B-B1BE-00F56432855D}">
       <text>
         <r>
           <rPr>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="69">
   <si>
     <t>R-TYPE</t>
   </si>
@@ -286,13 +286,49 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>done?</t>
+  </si>
+  <si>
+    <t>SRA</t>
+  </si>
+  <si>
+    <t>SRL</t>
+  </si>
+  <si>
+    <t>SLTU</t>
+  </si>
+  <si>
+    <t>XORI</t>
+  </si>
+  <si>
+    <t>ORI</t>
+  </si>
+  <si>
+    <t>ANDI</t>
+  </si>
+  <si>
+    <t>SLLI</t>
+  </si>
+  <si>
+    <t>SRLI</t>
+  </si>
+  <si>
+    <t>SRAI</t>
+  </si>
+  <si>
+    <t>SLTI</t>
+  </si>
+  <si>
+    <t>SLTIU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +369,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -613,7 +655,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -727,59 +769,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -788,13 +779,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1111,19 +1177,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA95D64-5055-4174-A4D5-0BDBECB18FB0}">
-  <dimension ref="D2:BB33"/>
+  <dimension ref="C2:BB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="19" topLeftCell="H24" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A5" sqref="A5"/>
-      <selection pane="topRight" activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="7" ySplit="23" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="AH36" sqref="AH36"/>
+      <selection pane="bottomRight" activeCell="AT35" sqref="AT35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="4.7109375" style="3"/>
+    <col min="1" max="2" width="4.7109375" style="3"/>
+    <col min="3" max="3" width="7.42578125" style="3" customWidth="1"/>
+    <col min="4" max="8" width="4.7109375" style="3"/>
     <col min="9" max="9" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="19" width="4.7109375" style="3"/>
     <col min="20" max="20" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -1140,20 +1207,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP2" s="40" t="s">
+      <c r="AP2" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="AQ2" s="41"/>
-      <c r="AR2" s="41"/>
-      <c r="AS2" s="41"/>
-      <c r="AT2" s="41"/>
-      <c r="AU2" s="42"/>
+      <c r="AQ2" s="59"/>
+      <c r="AR2" s="59"/>
+      <c r="AS2" s="59"/>
+      <c r="AT2" s="59"/>
+      <c r="AU2" s="60"/>
     </row>
     <row r="3" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP3" s="47" t="s">
+      <c r="AP3" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="48"/>
+      <c r="AQ3" s="66"/>
       <c r="AR3" s="21">
         <v>0</v>
       </c>
@@ -1168,10 +1235,10 @@
       </c>
     </row>
     <row r="4" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP4" s="45" t="s">
+      <c r="AP4" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="AQ4" s="46"/>
+      <c r="AQ4" s="64"/>
       <c r="AR4" s="21">
         <v>0</v>
       </c>
@@ -1282,10 +1349,10 @@
       <c r="AN5" s="2">
         <v>0</v>
       </c>
-      <c r="AP5" s="45" t="s">
+      <c r="AP5" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="AQ5" s="46"/>
+      <c r="AQ5" s="64"/>
       <c r="AR5" s="21">
         <v>0</v>
       </c>
@@ -1332,10 +1399,10 @@
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
-      <c r="AP6" s="45" t="s">
+      <c r="AP6" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="AQ6" s="46"/>
+      <c r="AQ6" s="64"/>
       <c r="AR6" s="21">
         <v>0</v>
       </c>
@@ -1386,10 +1453,10 @@
       <c r="AN7" s="3">
         <v>0</v>
       </c>
-      <c r="AP7" s="45" t="s">
+      <c r="AP7" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="AQ7" s="46"/>
+      <c r="AQ7" s="64"/>
       <c r="AR7" s="21">
         <v>0</v>
       </c>
@@ -1404,60 +1471,60 @@
       </c>
     </row>
     <row r="8" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="I8" s="38" t="s">
+      <c r="D8" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="I8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="35" t="s">
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="35" t="s">
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V8" s="36"/>
-      <c r="W8" s="36"/>
-      <c r="X8" s="36"/>
-      <c r="Y8" s="37"/>
-      <c r="Z8" s="35" t="s">
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="50"/>
+      <c r="Z8" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="36"/>
-      <c r="AB8" s="37"/>
-      <c r="AC8" s="35" t="s">
+      <c r="AA8" s="49"/>
+      <c r="AB8" s="50"/>
+      <c r="AC8" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AD8" s="36"/>
-      <c r="AE8" s="36"/>
-      <c r="AF8" s="36"/>
-      <c r="AG8" s="37"/>
-      <c r="AH8" s="35" t="s">
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="50"/>
+      <c r="AH8" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="AI8" s="36"/>
-      <c r="AJ8" s="36"/>
-      <c r="AK8" s="36"/>
-      <c r="AL8" s="36"/>
-      <c r="AM8" s="36"/>
-      <c r="AN8" s="49"/>
-      <c r="AP8" s="45" t="s">
+      <c r="AI8" s="49"/>
+      <c r="AJ8" s="49"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="49"/>
+      <c r="AM8" s="49"/>
+      <c r="AN8" s="52"/>
+      <c r="AP8" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="AQ8" s="46"/>
+      <c r="AQ8" s="64"/>
       <c r="AR8" s="21">
         <v>0</v>
       </c>
@@ -1508,10 +1575,10 @@
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
-      <c r="AP9" s="45" t="s">
+      <c r="AP9" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="AQ9" s="46"/>
+      <c r="AQ9" s="64"/>
       <c r="AR9" s="21">
         <v>0</v>
       </c>
@@ -1560,10 +1627,10 @@
       <c r="AN10" s="3">
         <v>0</v>
       </c>
-      <c r="AP10" s="45" t="s">
+      <c r="AP10" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="AQ10" s="46"/>
+      <c r="AQ10" s="64"/>
       <c r="AR10" s="21">
         <v>0</v>
       </c>
@@ -1578,58 +1645,58 @@
       </c>
     </row>
     <row r="11" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="I11" s="38" t="s">
+      <c r="D11" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="I11" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="36"/>
-      <c r="S11" s="36"/>
-      <c r="T11" s="37"/>
-      <c r="U11" s="35" t="s">
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V11" s="36"/>
-      <c r="W11" s="36"/>
-      <c r="X11" s="36"/>
-      <c r="Y11" s="37"/>
-      <c r="Z11" s="35" t="s">
+      <c r="V11" s="49"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="50"/>
+      <c r="Z11" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="AA11" s="36"/>
-      <c r="AB11" s="37"/>
-      <c r="AC11" s="35" t="s">
+      <c r="AA11" s="49"/>
+      <c r="AB11" s="50"/>
+      <c r="AC11" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AD11" s="36"/>
-      <c r="AE11" s="36"/>
-      <c r="AF11" s="36"/>
-      <c r="AG11" s="37"/>
-      <c r="AH11" s="35" t="s">
+      <c r="AD11" s="49"/>
+      <c r="AE11" s="49"/>
+      <c r="AF11" s="49"/>
+      <c r="AG11" s="50"/>
+      <c r="AH11" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="AI11" s="36"/>
-      <c r="AJ11" s="36"/>
-      <c r="AK11" s="36"/>
-      <c r="AL11" s="36"/>
-      <c r="AM11" s="36"/>
-      <c r="AN11" s="49"/>
-      <c r="AP11" s="43" t="s">
+      <c r="AI11" s="49"/>
+      <c r="AJ11" s="49"/>
+      <c r="AK11" s="49"/>
+      <c r="AL11" s="49"/>
+      <c r="AM11" s="49"/>
+      <c r="AN11" s="52"/>
+      <c r="AP11" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="AQ11" s="44"/>
+      <c r="AQ11" s="62"/>
       <c r="AR11" s="23">
         <v>1</v>
       </c>
@@ -1724,56 +1791,56 @@
       </c>
     </row>
     <row r="14" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="I14" s="38" t="s">
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="I14" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="35" t="s">
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="35" t="s">
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V14" s="36"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="36"/>
-      <c r="Y14" s="37"/>
-      <c r="Z14" s="35" t="s">
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="AA14" s="36"/>
-      <c r="AB14" s="37"/>
-      <c r="AC14" s="35" t="s">
+      <c r="AA14" s="49"/>
+      <c r="AB14" s="50"/>
+      <c r="AC14" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AD14" s="36"/>
-      <c r="AE14" s="36"/>
-      <c r="AF14" s="36"/>
-      <c r="AG14" s="37"/>
-      <c r="AH14" s="35" t="s">
+      <c r="AD14" s="49"/>
+      <c r="AE14" s="49"/>
+      <c r="AF14" s="49"/>
+      <c r="AG14" s="50"/>
+      <c r="AH14" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="AI14" s="36"/>
-      <c r="AJ14" s="36"/>
-      <c r="AK14" s="36"/>
-      <c r="AL14" s="36"/>
-      <c r="AM14" s="36"/>
-      <c r="AN14" s="49"/>
+      <c r="AI14" s="49"/>
+      <c r="AJ14" s="49"/>
+      <c r="AK14" s="49"/>
+      <c r="AL14" s="49"/>
+      <c r="AM14" s="49"/>
+      <c r="AN14" s="52"/>
     </row>
     <row r="15" spans="4:47" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
@@ -1858,63 +1925,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="51" t="s">
+    <row r="17" spans="3:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
       <c r="I17" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="38" t="s">
+      <c r="J17" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="35" t="s">
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="37"/>
-      <c r="U17" s="35" t="s">
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
-      <c r="X17" s="36"/>
-      <c r="Y17" s="37"/>
-      <c r="Z17" s="35" t="s">
+      <c r="V17" s="49"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="AA17" s="36"/>
-      <c r="AB17" s="37"/>
-      <c r="AC17" s="35" t="s">
+      <c r="AA17" s="49"/>
+      <c r="AB17" s="50"/>
+      <c r="AC17" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AD17" s="36"/>
-      <c r="AE17" s="36"/>
-      <c r="AF17" s="37"/>
+      <c r="AD17" s="49"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="50"/>
       <c r="AG17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AH17" s="35" t="s">
+      <c r="AH17" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="AI17" s="36"/>
-      <c r="AJ17" s="36"/>
-      <c r="AK17" s="36"/>
-      <c r="AL17" s="36"/>
-      <c r="AM17" s="36"/>
-      <c r="AN17" s="49"/>
+      <c r="AI17" s="49"/>
+      <c r="AJ17" s="49"/>
+      <c r="AK17" s="49"/>
+      <c r="AL17" s="49"/>
+      <c r="AM17" s="49"/>
+      <c r="AN17" s="52"/>
     </row>
-    <row r="18" spans="4:54" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:54" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1952,7 +2019,7 @@
       <c r="AM18" s="4"/>
       <c r="AN18" s="4"/>
     </row>
-    <row r="19" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1976,53 +2043,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="50" t="s">
+    <row r="20" spans="3:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="I20" s="38" t="s">
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="I20" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="36"/>
-      <c r="Z20" s="36"/>
-      <c r="AA20" s="36"/>
-      <c r="AB20" s="37"/>
-      <c r="AC20" s="35" t="s">
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="49"/>
+      <c r="V20" s="49"/>
+      <c r="W20" s="49"/>
+      <c r="X20" s="49"/>
+      <c r="Y20" s="49"/>
+      <c r="Z20" s="49"/>
+      <c r="AA20" s="49"/>
+      <c r="AB20" s="50"/>
+      <c r="AC20" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AD20" s="36"/>
-      <c r="AE20" s="36"/>
-      <c r="AF20" s="36"/>
-      <c r="AG20" s="37"/>
-      <c r="AH20" s="35" t="s">
+      <c r="AD20" s="49"/>
+      <c r="AE20" s="49"/>
+      <c r="AF20" s="49"/>
+      <c r="AG20" s="50"/>
+      <c r="AH20" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="AI20" s="36"/>
-      <c r="AJ20" s="36"/>
-      <c r="AK20" s="36"/>
-      <c r="AL20" s="36"/>
-      <c r="AM20" s="36"/>
-      <c r="AN20" s="49"/>
+      <c r="AI20" s="49"/>
+      <c r="AJ20" s="49"/>
+      <c r="AK20" s="49"/>
+      <c r="AL20" s="49"/>
+      <c r="AM20" s="49"/>
+      <c r="AN20" s="52"/>
     </row>
-    <row r="21" spans="4:54" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:54" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -2060,7 +2127,7 @@
       <c r="AM21" s="4"/>
       <c r="AN21" s="4"/>
     </row>
-    <row r="22" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -2096,100 +2163,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="54" t="s">
+    <row r="23" spans="3:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
       <c r="I23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="35" t="s">
+      <c r="J23" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
       <c r="T23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U23" s="35" t="s">
+      <c r="U23" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="V23" s="36"/>
-      <c r="W23" s="36"/>
-      <c r="X23" s="36"/>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="36"/>
-      <c r="AA23" s="36"/>
-      <c r="AB23" s="37"/>
-      <c r="AC23" s="35" t="s">
+      <c r="V23" s="49"/>
+      <c r="W23" s="49"/>
+      <c r="X23" s="49"/>
+      <c r="Y23" s="49"/>
+      <c r="Z23" s="49"/>
+      <c r="AA23" s="49"/>
+      <c r="AB23" s="50"/>
+      <c r="AC23" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AD23" s="36"/>
-      <c r="AE23" s="36"/>
-      <c r="AF23" s="36"/>
-      <c r="AG23" s="37"/>
-      <c r="AH23" s="35" t="s">
+      <c r="AD23" s="49"/>
+      <c r="AE23" s="49"/>
+      <c r="AF23" s="49"/>
+      <c r="AG23" s="50"/>
+      <c r="AH23" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="AI23" s="36"/>
-      <c r="AJ23" s="36"/>
-      <c r="AK23" s="36"/>
-      <c r="AL23" s="36"/>
-      <c r="AM23" s="36"/>
-      <c r="AN23" s="49"/>
+      <c r="AI23" s="49"/>
+      <c r="AJ23" s="49"/>
+      <c r="AK23" s="49"/>
+      <c r="AL23" s="49"/>
+      <c r="AM23" s="49"/>
+      <c r="AN23" s="52"/>
     </row>
-    <row r="25" spans="4:54" ht="15" x14ac:dyDescent="0.25">
-      <c r="AW25" s="60" t="s">
+    <row r="25" spans="3:54" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW25" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="AX25" s="60"/>
-      <c r="AY25" s="60"/>
-      <c r="AZ25" s="60"/>
-      <c r="BA25" s="60"/>
+      <c r="AX25" s="45"/>
+      <c r="AY25" s="45"/>
+      <c r="AZ25" s="45"/>
+      <c r="BA25" s="45"/>
     </row>
-    <row r="26" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AP26" s="39" t="s">
+    <row r="26" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP26" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="AQ26" s="39"/>
-      <c r="AR26" s="39"/>
-      <c r="AS26" s="39"/>
+      <c r="AQ26" s="67"/>
+      <c r="AR26" s="67"/>
+      <c r="AS26" s="67"/>
       <c r="AT26" s="25"/>
       <c r="AU26" s="25"/>
-      <c r="AW26" s="58" t="s">
+      <c r="AW26" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="AX26" s="58" t="s">
+      <c r="AX26" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="AY26" s="58" t="s">
+      <c r="AY26" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="AZ26" s="58" t="s">
+      <c r="AZ26" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="BA26" s="59" t="s">
+      <c r="BA26" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="BB26" s="59" t="s">
+      <c r="BB26" s="42" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="34" t="s">
+    <row r="27" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="34"/>
+      <c r="E27" s="68"/>
       <c r="F27" s="19" t="s">
         <v>27</v>
       </c>
@@ -2214,20 +2287,20 @@
       <c r="O27" s="10">
         <v>0</v>
       </c>
-      <c r="P27" s="35" t="s">
+      <c r="P27" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="Q27" s="36"/>
-      <c r="R27" s="36"/>
-      <c r="S27" s="36"/>
-      <c r="T27" s="37"/>
-      <c r="U27" s="35" t="s">
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V27" s="36"/>
-      <c r="W27" s="36"/>
-      <c r="X27" s="36"/>
-      <c r="Y27" s="37"/>
+      <c r="V27" s="49"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="49"/>
+      <c r="Y27" s="50"/>
       <c r="Z27" s="16">
         <v>0</v>
       </c>
@@ -2237,13 +2310,13 @@
       <c r="AB27" s="18">
         <v>0</v>
       </c>
-      <c r="AC27" s="35" t="s">
+      <c r="AC27" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AD27" s="36"/>
-      <c r="AE27" s="36"/>
-      <c r="AF27" s="36"/>
-      <c r="AG27" s="37"/>
+      <c r="AD27" s="49"/>
+      <c r="AE27" s="49"/>
+      <c r="AF27" s="49"/>
+      <c r="AG27" s="50"/>
       <c r="AH27" s="8">
         <v>0</v>
       </c>
@@ -2265,10 +2338,10 @@
       <c r="AN27" s="15">
         <v>1</v>
       </c>
-      <c r="AP27" s="56" t="s">
+      <c r="AP27" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="AQ27" s="56"/>
+      <c r="AQ27" s="46"/>
       <c r="AR27" s="26">
         <v>0</v>
       </c>
@@ -2281,30 +2354,33 @@
       <c r="AU27" s="28">
         <v>1</v>
       </c>
-      <c r="AW27" s="57">
-        <v>1</v>
-      </c>
-      <c r="AX27" s="57">
-        <v>1</v>
-      </c>
-      <c r="AY27" s="57">
-        <v>0</v>
-      </c>
-      <c r="AZ27" s="57">
-        <v>0</v>
-      </c>
-      <c r="BA27" s="61" t="s">
+      <c r="AW27" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX27" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY27" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ27" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA27" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="BB27" s="57" t="s">
+      <c r="BB27" s="40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="34" t="s">
+    <row r="28" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="34"/>
+      <c r="E28" s="68"/>
       <c r="F28" s="19" t="s">
         <v>27</v>
       </c>
@@ -2329,20 +2405,20 @@
       <c r="O28" s="10">
         <v>0</v>
       </c>
-      <c r="P28" s="35" t="s">
+      <c r="P28" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="Q28" s="36"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="37"/>
-      <c r="U28" s="35" t="s">
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V28" s="36"/>
-      <c r="W28" s="36"/>
-      <c r="X28" s="36"/>
-      <c r="Y28" s="37"/>
+      <c r="V28" s="49"/>
+      <c r="W28" s="49"/>
+      <c r="X28" s="49"/>
+      <c r="Y28" s="50"/>
       <c r="Z28" s="16">
         <v>0</v>
       </c>
@@ -2352,13 +2428,13 @@
       <c r="AB28" s="18">
         <v>0</v>
       </c>
-      <c r="AC28" s="35" t="s">
+      <c r="AC28" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AD28" s="36"/>
-      <c r="AE28" s="36"/>
-      <c r="AF28" s="36"/>
-      <c r="AG28" s="37"/>
+      <c r="AD28" s="49"/>
+      <c r="AE28" s="49"/>
+      <c r="AF28" s="49"/>
+      <c r="AG28" s="50"/>
       <c r="AH28" s="8">
         <v>0</v>
       </c>
@@ -2380,10 +2456,10 @@
       <c r="AN28" s="15">
         <v>1</v>
       </c>
-      <c r="AP28" s="56" t="s">
+      <c r="AP28" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="AQ28" s="56"/>
+      <c r="AQ28" s="46"/>
       <c r="AR28" s="29">
         <v>0</v>
       </c>
@@ -2396,546 +2472,2363 @@
       <c r="AU28" s="31">
         <v>0</v>
       </c>
-      <c r="AW28" s="57">
-        <v>1</v>
-      </c>
-      <c r="AX28" s="57">
-        <v>1</v>
-      </c>
-      <c r="AY28" s="57">
-        <v>0</v>
-      </c>
-      <c r="AZ28" s="57">
-        <v>0</v>
-      </c>
-      <c r="BA28" s="61" t="s">
+      <c r="AW28" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX28" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY28" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ28" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA28" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="BB28" s="57" t="s">
+      <c r="BB28" s="40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="34" t="s">
+    <row r="29" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="68"/>
+      <c r="F29" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I29" s="38">
+        <v>0</v>
+      </c>
+      <c r="J29" s="36">
+        <v>0</v>
+      </c>
+      <c r="K29" s="36">
+        <v>0</v>
+      </c>
+      <c r="L29" s="36">
+        <v>0</v>
+      </c>
+      <c r="M29" s="36">
+        <v>0</v>
+      </c>
+      <c r="N29" s="36">
+        <v>0</v>
+      </c>
+      <c r="O29" s="37">
+        <v>0</v>
+      </c>
+      <c r="P29" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V29" s="49"/>
+      <c r="W29" s="49"/>
+      <c r="X29" s="49"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD29" s="49"/>
+      <c r="AE29" s="49"/>
+      <c r="AF29" s="49"/>
+      <c r="AG29" s="50"/>
+      <c r="AH29" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI29" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ29" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK29" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM29" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN29" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP29" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ29" s="70"/>
+      <c r="AR29" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS29" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT29" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU29" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW29" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX29" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY29" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ29" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA29" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB29" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="68"/>
+      <c r="F30" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="38">
+        <v>0</v>
+      </c>
+      <c r="J30" s="36">
+        <v>0</v>
+      </c>
+      <c r="K30" s="36">
+        <v>0</v>
+      </c>
+      <c r="L30" s="36">
+        <v>0</v>
+      </c>
+      <c r="M30" s="36">
+        <v>0</v>
+      </c>
+      <c r="N30" s="36">
+        <v>0</v>
+      </c>
+      <c r="O30" s="37">
+        <v>0</v>
+      </c>
+      <c r="P30" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V30" s="49"/>
+      <c r="W30" s="49"/>
+      <c r="X30" s="49"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD30" s="49"/>
+      <c r="AE30" s="49"/>
+      <c r="AF30" s="49"/>
+      <c r="AG30" s="50"/>
+      <c r="AH30" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI30" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ30" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK30" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL30" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM30" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN30" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP30" s="69" t="s">
+        <v>30</v>
+      </c>
+      <c r="AQ30" s="70"/>
+      <c r="AR30" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS30" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT30" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU30" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW30" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX30" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY30" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ30" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA30" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB30" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="68"/>
+      <c r="F31" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="38">
+        <v>0</v>
+      </c>
+      <c r="J31" s="36">
+        <v>0</v>
+      </c>
+      <c r="K31" s="36">
+        <v>0</v>
+      </c>
+      <c r="L31" s="36">
+        <v>0</v>
+      </c>
+      <c r="M31" s="36">
+        <v>0</v>
+      </c>
+      <c r="N31" s="36">
+        <v>0</v>
+      </c>
+      <c r="O31" s="37">
+        <v>0</v>
+      </c>
+      <c r="P31" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="50"/>
+      <c r="U31" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V31" s="49"/>
+      <c r="W31" s="49"/>
+      <c r="X31" s="49"/>
+      <c r="Y31" s="50"/>
+      <c r="Z31" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB31" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC31" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD31" s="49"/>
+      <c r="AE31" s="49"/>
+      <c r="AF31" s="49"/>
+      <c r="AG31" s="50"/>
+      <c r="AH31" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI31" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK31" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL31" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM31" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN31" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP31" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ31" s="70"/>
+      <c r="AR31" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS31" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT31" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU31" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW31" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX31" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY31" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ31" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA31" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB31" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="68"/>
+      <c r="F32" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" s="38">
+        <v>0</v>
+      </c>
+      <c r="J32" s="36">
+        <v>0</v>
+      </c>
+      <c r="K32" s="36">
+        <v>0</v>
+      </c>
+      <c r="L32" s="36">
+        <v>0</v>
+      </c>
+      <c r="M32" s="36">
+        <v>0</v>
+      </c>
+      <c r="N32" s="36">
+        <v>0</v>
+      </c>
+      <c r="O32" s="37">
+        <v>0</v>
+      </c>
+      <c r="P32" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="50"/>
+      <c r="U32" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V32" s="49"/>
+      <c r="W32" s="49"/>
+      <c r="X32" s="49"/>
+      <c r="Y32" s="50"/>
+      <c r="Z32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD32" s="49"/>
+      <c r="AE32" s="49"/>
+      <c r="AF32" s="49"/>
+      <c r="AG32" s="50"/>
+      <c r="AH32" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK32" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL32" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN32" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP32" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ32" s="70"/>
+      <c r="AR32" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS32" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT32" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU32" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW32" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX32" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY32" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ32" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA32" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB32" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="68"/>
+      <c r="F33" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33" s="38">
+        <v>0</v>
+      </c>
+      <c r="J33" s="36">
+        <v>0</v>
+      </c>
+      <c r="K33" s="36">
+        <v>0</v>
+      </c>
+      <c r="L33" s="36">
+        <v>0</v>
+      </c>
+      <c r="M33" s="36">
+        <v>0</v>
+      </c>
+      <c r="N33" s="36">
+        <v>0</v>
+      </c>
+      <c r="O33" s="37">
+        <v>0</v>
+      </c>
+      <c r="P33" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="50"/>
+      <c r="U33" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V33" s="49"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="49"/>
+      <c r="Y33" s="50"/>
+      <c r="Z33" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD33" s="49"/>
+      <c r="AE33" s="49"/>
+      <c r="AF33" s="49"/>
+      <c r="AG33" s="50"/>
+      <c r="AH33" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ33" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK33" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM33" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN33" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP33" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ33" s="70"/>
+      <c r="AR33" s="29">
+        <v>1</v>
+      </c>
+      <c r="AS33" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT33" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU33" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW33" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX33" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY33" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ33" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA33" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB33" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="68"/>
+      <c r="F34" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="38">
+        <v>0</v>
+      </c>
+      <c r="J34" s="36">
+        <v>1</v>
+      </c>
+      <c r="K34" s="36">
+        <v>0</v>
+      </c>
+      <c r="L34" s="36">
+        <v>0</v>
+      </c>
+      <c r="M34" s="36">
+        <v>0</v>
+      </c>
+      <c r="N34" s="36">
+        <v>0</v>
+      </c>
+      <c r="O34" s="37">
+        <v>0</v>
+      </c>
+      <c r="P34" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="50"/>
+      <c r="U34" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V34" s="49"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="49"/>
+      <c r="Y34" s="50"/>
+      <c r="Z34" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD34" s="49"/>
+      <c r="AE34" s="49"/>
+      <c r="AF34" s="49"/>
+      <c r="AG34" s="50"/>
+      <c r="AH34" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ34" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK34" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM34" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN34" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP34" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ34" s="70"/>
+      <c r="AR34" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS34" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT34" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU34" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW34" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX34" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY34" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ34" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA34" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB34" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="68"/>
+      <c r="F35" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I35" s="38">
+        <v>0</v>
+      </c>
+      <c r="J35" s="36">
+        <v>0</v>
+      </c>
+      <c r="K35" s="36">
+        <v>0</v>
+      </c>
+      <c r="L35" s="36">
+        <v>0</v>
+      </c>
+      <c r="M35" s="36">
+        <v>0</v>
+      </c>
+      <c r="N35" s="36">
+        <v>0</v>
+      </c>
+      <c r="O35" s="37">
+        <v>0</v>
+      </c>
+      <c r="P35" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="50"/>
+      <c r="U35" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V35" s="49"/>
+      <c r="W35" s="49"/>
+      <c r="X35" s="49"/>
+      <c r="Y35" s="50"/>
+      <c r="Z35" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD35" s="49"/>
+      <c r="AE35" s="49"/>
+      <c r="AF35" s="49"/>
+      <c r="AG35" s="50"/>
+      <c r="AH35" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ35" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK35" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL35" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM35" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN35" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP35" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ35" s="70"/>
+      <c r="AR35" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS35" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT35" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU35" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW35" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX35" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY35" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ35" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA35" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB35" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="68"/>
+      <c r="F36" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36" s="38">
+        <v>0</v>
+      </c>
+      <c r="J36" s="36">
+        <v>0</v>
+      </c>
+      <c r="K36" s="36">
+        <v>0</v>
+      </c>
+      <c r="L36" s="36">
+        <v>0</v>
+      </c>
+      <c r="M36" s="36">
+        <v>0</v>
+      </c>
+      <c r="N36" s="36">
+        <v>0</v>
+      </c>
+      <c r="O36" s="37">
+        <v>0</v>
+      </c>
+      <c r="P36" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V36" s="49"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="49"/>
+      <c r="Y36" s="50"/>
+      <c r="Z36" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC36" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD36" s="49"/>
+      <c r="AE36" s="49"/>
+      <c r="AF36" s="49"/>
+      <c r="AG36" s="50"/>
+      <c r="AH36" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI36" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ36" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK36" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL36" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM36" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN36" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP36" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ36" s="70"/>
+      <c r="AR36" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS36" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT36" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU36" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW36" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX36" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY36" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ36" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA36" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB36" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="12" t="s">
+      <c r="E37" s="68"/>
+      <c r="F37" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="38" t="s">
+      <c r="I37" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="36"/>
-      <c r="O29" s="36"/>
-      <c r="P29" s="36"/>
-      <c r="Q29" s="36"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="36"/>
-      <c r="T29" s="37"/>
-      <c r="U29" s="35" t="s">
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="50"/>
+      <c r="U37" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V29" s="36"/>
-      <c r="W29" s="36"/>
-      <c r="X29" s="36"/>
-      <c r="Y29" s="37"/>
-      <c r="Z29" s="16">
-        <v>0</v>
-      </c>
-      <c r="AA29" s="17">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC29" s="35" t="s">
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="50"/>
+      <c r="Z37" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AD29" s="36"/>
-      <c r="AE29" s="36"/>
-      <c r="AF29" s="36"/>
-      <c r="AG29" s="37"/>
-      <c r="AH29" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AJ29" s="9">
-        <v>1</v>
-      </c>
-      <c r="AK29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM29" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN29" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP29" s="56" t="s">
+      <c r="AD37" s="49"/>
+      <c r="AE37" s="49"/>
+      <c r="AF37" s="49"/>
+      <c r="AG37" s="50"/>
+      <c r="AH37" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI37" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ37" s="9">
+        <v>1</v>
+      </c>
+      <c r="AK37" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM37" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN37" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP37" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="AQ29" s="56"/>
-      <c r="AR29" s="29">
-        <v>0</v>
-      </c>
-      <c r="AS29" s="30">
-        <v>0</v>
-      </c>
-      <c r="AT29" s="30">
-        <v>1</v>
-      </c>
-      <c r="AU29" s="31">
-        <v>1</v>
-      </c>
-      <c r="AW29" s="57">
-        <v>1</v>
-      </c>
-      <c r="AX29" s="57">
-        <v>1</v>
-      </c>
-      <c r="AY29" s="57">
-        <v>1</v>
-      </c>
-      <c r="AZ29" s="57">
-        <v>0</v>
-      </c>
-      <c r="BA29" s="61" t="s">
+      <c r="AQ37" s="46"/>
+      <c r="AR37" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS37" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT37" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU37" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW37" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX37" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY37" s="40">
+        <v>1</v>
+      </c>
+      <c r="AZ37" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA37" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="BB29" s="57" t="s">
+      <c r="BB37" s="40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="4:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="34" t="s">
+    <row r="38" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="68"/>
+      <c r="F38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="49"/>
+      <c r="R38" s="49"/>
+      <c r="S38" s="49"/>
+      <c r="T38" s="50"/>
+      <c r="U38" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V38" s="49"/>
+      <c r="W38" s="49"/>
+      <c r="X38" s="49"/>
+      <c r="Y38" s="50"/>
+      <c r="Z38" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA38" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD38" s="49"/>
+      <c r="AE38" s="49"/>
+      <c r="AF38" s="49"/>
+      <c r="AG38" s="50"/>
+      <c r="AH38" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI38" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ38" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK38" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN38" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP38" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ38" s="46"/>
+      <c r="AR38" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS38" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT38" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU38" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW38" s="40"/>
+      <c r="AX38" s="40"/>
+      <c r="AY38" s="40"/>
+      <c r="AZ38" s="40"/>
+      <c r="BA38" s="43"/>
+      <c r="BB38" s="40"/>
+    </row>
+    <row r="39" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="68"/>
+      <c r="F39" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="50"/>
+      <c r="U39" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V39" s="49"/>
+      <c r="W39" s="49"/>
+      <c r="X39" s="49"/>
+      <c r="Y39" s="50"/>
+      <c r="Z39" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD39" s="49"/>
+      <c r="AE39" s="49"/>
+      <c r="AF39" s="49"/>
+      <c r="AG39" s="50"/>
+      <c r="AH39" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI39" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ39" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK39" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL39" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM39" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN39" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP39" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="AQ39" s="46"/>
+      <c r="AR39" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS39" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT39" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU39" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW39" s="40"/>
+      <c r="AX39" s="40"/>
+      <c r="AY39" s="40"/>
+      <c r="AZ39" s="40"/>
+      <c r="BA39" s="43"/>
+      <c r="BB39" s="40"/>
+    </row>
+    <row r="40" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="68"/>
+      <c r="F40" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="50"/>
+      <c r="U40" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V40" s="49"/>
+      <c r="W40" s="49"/>
+      <c r="X40" s="49"/>
+      <c r="Y40" s="50"/>
+      <c r="Z40" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB40" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC40" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD40" s="49"/>
+      <c r="AE40" s="49"/>
+      <c r="AF40" s="49"/>
+      <c r="AG40" s="50"/>
+      <c r="AH40" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI40" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ40" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK40" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM40" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN40" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP40" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ40" s="46"/>
+      <c r="AR40" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS40" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT40" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU40" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW40" s="40"/>
+      <c r="AX40" s="40"/>
+      <c r="AY40" s="40"/>
+      <c r="AZ40" s="40"/>
+      <c r="BA40" s="43"/>
+      <c r="BB40" s="40"/>
+    </row>
+    <row r="41" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="68"/>
+      <c r="F41" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" s="38">
+        <v>0</v>
+      </c>
+      <c r="J41" s="36">
+        <v>0</v>
+      </c>
+      <c r="K41" s="36">
+        <v>0</v>
+      </c>
+      <c r="L41" s="36">
+        <v>0</v>
+      </c>
+      <c r="M41" s="36">
+        <v>0</v>
+      </c>
+      <c r="N41" s="36">
+        <v>0</v>
+      </c>
+      <c r="O41" s="36">
+        <v>0</v>
+      </c>
+      <c r="P41" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q41" s="49"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="50"/>
+      <c r="U41" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="V41" s="49"/>
+      <c r="W41" s="49"/>
+      <c r="X41" s="49"/>
+      <c r="Y41" s="50"/>
+      <c r="Z41" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC41" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD41" s="49"/>
+      <c r="AE41" s="49"/>
+      <c r="AF41" s="49"/>
+      <c r="AG41" s="50"/>
+      <c r="AH41" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI41" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ41" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK41" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL41" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM41" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN41" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP41" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ41" s="46"/>
+      <c r="AR41" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS41" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT41" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU41" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW41" s="40"/>
+      <c r="AX41" s="40"/>
+      <c r="AY41" s="40"/>
+      <c r="AZ41" s="40"/>
+      <c r="BA41" s="43"/>
+      <c r="BB41" s="40"/>
+    </row>
+    <row r="42" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" s="68"/>
+      <c r="F42" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I42" s="38">
+        <v>0</v>
+      </c>
+      <c r="J42" s="36">
+        <v>0</v>
+      </c>
+      <c r="K42" s="36">
+        <v>0</v>
+      </c>
+      <c r="L42" s="36">
+        <v>0</v>
+      </c>
+      <c r="M42" s="36">
+        <v>0</v>
+      </c>
+      <c r="N42" s="36">
+        <v>0</v>
+      </c>
+      <c r="O42" s="36">
+        <v>0</v>
+      </c>
+      <c r="P42" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="50"/>
+      <c r="U42" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="V42" s="49"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="49"/>
+      <c r="Y42" s="50"/>
+      <c r="Z42" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA42" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC42" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD42" s="49"/>
+      <c r="AE42" s="49"/>
+      <c r="AF42" s="49"/>
+      <c r="AG42" s="50"/>
+      <c r="AH42" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ42" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK42" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL42" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM42" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN42" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP42" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ42" s="46"/>
+      <c r="AR42" s="29">
+        <v>1</v>
+      </c>
+      <c r="AS42" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT42" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU42" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW42" s="40"/>
+      <c r="AX42" s="40"/>
+      <c r="AY42" s="40"/>
+      <c r="AZ42" s="40"/>
+      <c r="BA42" s="43"/>
+      <c r="BB42" s="40"/>
+    </row>
+    <row r="43" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="68"/>
+      <c r="F43" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" s="38">
+        <v>0</v>
+      </c>
+      <c r="J43" s="36">
+        <v>0</v>
+      </c>
+      <c r="K43" s="36">
+        <v>1</v>
+      </c>
+      <c r="L43" s="36">
+        <v>0</v>
+      </c>
+      <c r="M43" s="36">
+        <v>0</v>
+      </c>
+      <c r="N43" s="36">
+        <v>0</v>
+      </c>
+      <c r="O43" s="36">
+        <v>0</v>
+      </c>
+      <c r="P43" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q43" s="49"/>
+      <c r="R43" s="49"/>
+      <c r="S43" s="49"/>
+      <c r="T43" s="50"/>
+      <c r="U43" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="V43" s="49"/>
+      <c r="W43" s="49"/>
+      <c r="X43" s="49"/>
+      <c r="Y43" s="50"/>
+      <c r="Z43" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA43" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC43" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD43" s="49"/>
+      <c r="AE43" s="49"/>
+      <c r="AF43" s="49"/>
+      <c r="AG43" s="50"/>
+      <c r="AH43" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ43" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK43" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL43" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM43" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN43" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP43" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ43" s="46"/>
+      <c r="AR43" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS43" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT43" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU43" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW43" s="40"/>
+      <c r="AX43" s="40"/>
+      <c r="AY43" s="40"/>
+      <c r="AZ43" s="40"/>
+      <c r="BA43" s="43"/>
+      <c r="BB43" s="40"/>
+    </row>
+    <row r="44" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" s="68"/>
+      <c r="F44" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="49"/>
+      <c r="R44" s="49"/>
+      <c r="S44" s="49"/>
+      <c r="T44" s="50"/>
+      <c r="U44" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V44" s="49"/>
+      <c r="W44" s="49"/>
+      <c r="X44" s="49"/>
+      <c r="Y44" s="50"/>
+      <c r="Z44" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB44" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD44" s="49"/>
+      <c r="AE44" s="49"/>
+      <c r="AF44" s="49"/>
+      <c r="AG44" s="50"/>
+      <c r="AH44" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI44" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ44" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK44" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL44" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM44" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN44" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP44" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ44" s="46"/>
+      <c r="AR44" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS44" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT44" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU44" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW44" s="40"/>
+      <c r="AX44" s="40"/>
+      <c r="AY44" s="40"/>
+      <c r="AZ44" s="40"/>
+      <c r="BA44" s="43"/>
+      <c r="BB44" s="40"/>
+    </row>
+    <row r="45" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45" s="68"/>
+      <c r="F45" s="12"/>
+      <c r="I45" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="J45" s="49"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
+      <c r="P45" s="49"/>
+      <c r="Q45" s="49"/>
+      <c r="R45" s="49"/>
+      <c r="S45" s="49"/>
+      <c r="T45" s="50"/>
+      <c r="U45" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="V45" s="49"/>
+      <c r="W45" s="49"/>
+      <c r="X45" s="49"/>
+      <c r="Y45" s="50"/>
+      <c r="Z45" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB45" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC45" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD45" s="49"/>
+      <c r="AE45" s="49"/>
+      <c r="AF45" s="49"/>
+      <c r="AG45" s="50"/>
+      <c r="AH45" s="35">
+        <v>0</v>
+      </c>
+      <c r="AI45" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ45" s="36">
+        <v>1</v>
+      </c>
+      <c r="AK45" s="36">
+        <v>0</v>
+      </c>
+      <c r="AL45" s="36">
+        <v>0</v>
+      </c>
+      <c r="AM45" s="36">
+        <v>1</v>
+      </c>
+      <c r="AN45" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP45" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ45" s="46"/>
+      <c r="AR45" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS45" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT45" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU45" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW45" s="40"/>
+      <c r="AX45" s="40"/>
+      <c r="AY45" s="40"/>
+      <c r="AZ45" s="40"/>
+      <c r="BA45" s="43"/>
+      <c r="BB45" s="40"/>
+    </row>
+    <row r="46" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="12" t="s">
+      <c r="E46" s="68"/>
+      <c r="F46" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="38" t="s">
+      <c r="I46" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="36"/>
-      <c r="O30" s="36"/>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="36"/>
-      <c r="R30" s="36"/>
-      <c r="S30" s="36"/>
-      <c r="T30" s="37"/>
-      <c r="U30" s="35" t="s">
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+      <c r="L46" s="49"/>
+      <c r="M46" s="49"/>
+      <c r="N46" s="49"/>
+      <c r="O46" s="49"/>
+      <c r="P46" s="49"/>
+      <c r="Q46" s="49"/>
+      <c r="R46" s="49"/>
+      <c r="S46" s="49"/>
+      <c r="T46" s="50"/>
+      <c r="U46" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V30" s="36"/>
-      <c r="W30" s="36"/>
-      <c r="X30" s="36"/>
-      <c r="Y30" s="37"/>
-      <c r="Z30" s="16">
-        <v>0</v>
-      </c>
-      <c r="AA30" s="17">
-        <v>1</v>
-      </c>
-      <c r="AB30" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC30" s="35" t="s">
+      <c r="V46" s="49"/>
+      <c r="W46" s="49"/>
+      <c r="X46" s="49"/>
+      <c r="Y46" s="50"/>
+      <c r="Z46" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB46" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AD30" s="36"/>
-      <c r="AE30" s="36"/>
-      <c r="AF30" s="36"/>
-      <c r="AG30" s="37"/>
-      <c r="AH30" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AJ30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM30" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN30" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP30" s="56" t="s">
+      <c r="AD46" s="49"/>
+      <c r="AE46" s="49"/>
+      <c r="AF46" s="49"/>
+      <c r="AG46" s="50"/>
+      <c r="AH46" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI46" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ46" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL46" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM46" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN46" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP46" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="AQ30" s="56"/>
-      <c r="AR30" s="29">
-        <v>0</v>
-      </c>
-      <c r="AS30" s="30">
-        <v>0</v>
-      </c>
-      <c r="AT30" s="30">
-        <v>1</v>
-      </c>
-      <c r="AU30" s="31">
-        <v>1</v>
-      </c>
-      <c r="AW30" s="57">
-        <v>1</v>
-      </c>
-      <c r="AX30" s="57">
-        <v>1</v>
-      </c>
-      <c r="AY30" s="57">
-        <v>1</v>
-      </c>
-      <c r="AZ30" s="57">
-        <v>0</v>
-      </c>
-      <c r="BA30" s="61" t="s">
+      <c r="AQ46" s="46"/>
+      <c r="AR46" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS46" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT46" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU46" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW46" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX46" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY46" s="40">
+        <v>1</v>
+      </c>
+      <c r="AZ46" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA46" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="BB30" s="57" t="s">
+      <c r="BB46" s="40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="34" t="s">
+    <row r="47" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="13" t="s">
+      <c r="E47" s="68"/>
+      <c r="F47" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="38" t="s">
+      <c r="I47" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="37"/>
-      <c r="P31" s="35" t="s">
+      <c r="J47" s="49"/>
+      <c r="K47" s="49"/>
+      <c r="L47" s="49"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="49"/>
+      <c r="O47" s="50"/>
+      <c r="P47" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="36"/>
-      <c r="S31" s="36"/>
-      <c r="T31" s="37"/>
-      <c r="U31" s="35" t="s">
+      <c r="Q47" s="49"/>
+      <c r="R47" s="49"/>
+      <c r="S47" s="49"/>
+      <c r="T47" s="50"/>
+      <c r="U47" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V31" s="36"/>
-      <c r="W31" s="36"/>
-      <c r="X31" s="36"/>
-      <c r="Y31" s="37"/>
-      <c r="Z31" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA31" s="9">
-        <v>1</v>
-      </c>
-      <c r="AB31" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="35" t="s">
+      <c r="V47" s="49"/>
+      <c r="W47" s="49"/>
+      <c r="X47" s="49"/>
+      <c r="Y47" s="50"/>
+      <c r="Z47" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB47" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="AD31" s="36"/>
-      <c r="AE31" s="36"/>
-      <c r="AF31" s="36"/>
-      <c r="AG31" s="37"/>
-      <c r="AH31" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI31" s="9">
-        <v>1</v>
-      </c>
-      <c r="AJ31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM31" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN31" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP31" s="56" t="s">
+      <c r="AD47" s="49"/>
+      <c r="AE47" s="49"/>
+      <c r="AF47" s="49"/>
+      <c r="AG47" s="50"/>
+      <c r="AH47" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ47" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL47" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM47" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN47" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP47" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="AQ31" s="56"/>
-      <c r="AR31" s="29">
-        <v>0</v>
-      </c>
-      <c r="AS31" s="30">
-        <v>0</v>
-      </c>
-      <c r="AT31" s="30">
-        <v>1</v>
-      </c>
-      <c r="AU31" s="31">
-        <v>1</v>
-      </c>
-      <c r="AW31" s="57">
-        <v>1</v>
-      </c>
-      <c r="AX31" s="57">
-        <v>0</v>
-      </c>
-      <c r="AY31" s="57">
-        <v>1</v>
-      </c>
-      <c r="AZ31" s="57">
-        <v>1</v>
-      </c>
-      <c r="BA31" s="61" t="s">
+      <c r="AQ47" s="46"/>
+      <c r="AR47" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS47" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT47" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU47" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW47" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX47" s="40">
+        <v>0</v>
+      </c>
+      <c r="AY47" s="40">
+        <v>1</v>
+      </c>
+      <c r="AZ47" s="40">
+        <v>1</v>
+      </c>
+      <c r="BA47" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="BB31" s="57" t="s">
+      <c r="BB47" s="40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="34" t="s">
+    <row r="48" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="32" t="s">
+      <c r="E48" s="68"/>
+      <c r="F48" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I48" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J32" s="38" t="s">
+      <c r="J48" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="35" t="s">
+      <c r="K48" s="49"/>
+      <c r="L48" s="49"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="49"/>
+      <c r="O48" s="50"/>
+      <c r="P48" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="36"/>
-      <c r="T32" s="37"/>
-      <c r="U32" s="35" t="s">
+      <c r="Q48" s="49"/>
+      <c r="R48" s="49"/>
+      <c r="S48" s="49"/>
+      <c r="T48" s="50"/>
+      <c r="U48" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V32" s="36"/>
-      <c r="W32" s="36"/>
-      <c r="X32" s="36"/>
-      <c r="Y32" s="37"/>
-      <c r="Z32" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB32" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC32" s="35" t="s">
+      <c r="V48" s="49"/>
+      <c r="W48" s="49"/>
+      <c r="X48" s="49"/>
+      <c r="Y48" s="50"/>
+      <c r="Z48" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="AD32" s="36"/>
-      <c r="AE32" s="36"/>
-      <c r="AF32" s="37"/>
-      <c r="AG32" s="10" t="s">
+      <c r="AD48" s="49"/>
+      <c r="AE48" s="49"/>
+      <c r="AF48" s="50"/>
+      <c r="AG48" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AH32" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI32" s="9">
-        <v>1</v>
-      </c>
-      <c r="AJ32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM32" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN32" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP32" s="56" t="s">
+      <c r="AH48" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI48" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ48" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK48" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL48" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM48" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN48" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP48" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="AQ32" s="56"/>
-      <c r="AR32" s="29">
-        <v>0</v>
-      </c>
-      <c r="AS32" s="30">
-        <v>1</v>
-      </c>
-      <c r="AT32" s="30">
-        <v>0</v>
-      </c>
-      <c r="AU32" s="31">
-        <v>0</v>
-      </c>
-      <c r="AW32" s="57">
-        <v>1</v>
-      </c>
-      <c r="AX32" s="57">
-        <v>0</v>
-      </c>
-      <c r="AY32" s="57">
-        <v>0</v>
-      </c>
-      <c r="AZ32" s="57">
-        <v>0</v>
-      </c>
-      <c r="BA32" s="57" t="s">
+      <c r="AQ48" s="46"/>
+      <c r="AR48" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS48" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT48" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU48" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW48" s="40">
+        <v>1</v>
+      </c>
+      <c r="AX48" s="40">
+        <v>0</v>
+      </c>
+      <c r="AY48" s="40">
+        <v>0</v>
+      </c>
+      <c r="AZ48" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA48" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="BB32" s="57" t="s">
+      <c r="BB48" s="40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="34" t="s">
+    <row r="49" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="33" t="s">
+      <c r="E49" s="68"/>
+      <c r="F49" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I49" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J33" s="35" t="s">
+      <c r="J49" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="36"/>
-      <c r="O33" s="36"/>
-      <c r="P33" s="36"/>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="36"/>
-      <c r="S33" s="36"/>
-      <c r="T33" s="7" t="s">
+      <c r="K49" s="49"/>
+      <c r="L49" s="49"/>
+      <c r="M49" s="49"/>
+      <c r="N49" s="49"/>
+      <c r="O49" s="49"/>
+      <c r="P49" s="49"/>
+      <c r="Q49" s="49"/>
+      <c r="R49" s="49"/>
+      <c r="S49" s="49"/>
+      <c r="T49" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U33" s="35" t="s">
+      <c r="U49" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="V33" s="36"/>
-      <c r="W33" s="36"/>
-      <c r="X33" s="36"/>
-      <c r="Y33" s="36"/>
-      <c r="Z33" s="36"/>
-      <c r="AA33" s="36"/>
-      <c r="AB33" s="37"/>
-      <c r="AC33" s="35" t="s">
+      <c r="V49" s="49"/>
+      <c r="W49" s="49"/>
+      <c r="X49" s="49"/>
+      <c r="Y49" s="49"/>
+      <c r="Z49" s="49"/>
+      <c r="AA49" s="49"/>
+      <c r="AB49" s="50"/>
+      <c r="AC49" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="AD33" s="36"/>
-      <c r="AE33" s="36"/>
-      <c r="AF33" s="36"/>
-      <c r="AG33" s="37"/>
-      <c r="AH33" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI33" s="9">
-        <v>1</v>
-      </c>
-      <c r="AJ33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK33" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL33" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM33" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN33" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP33" s="56" t="s">
+      <c r="AD49" s="49"/>
+      <c r="AE49" s="49"/>
+      <c r="AF49" s="49"/>
+      <c r="AG49" s="50"/>
+      <c r="AH49" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI49" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ49" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK49" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL49" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM49" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN49" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP49" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="AQ33" s="56"/>
-      <c r="AR33" s="29">
-        <v>0</v>
-      </c>
-      <c r="AS33" s="30">
-        <v>0</v>
-      </c>
-      <c r="AT33" s="30">
-        <v>1</v>
-      </c>
-      <c r="AU33" s="31">
-        <v>1</v>
-      </c>
-      <c r="AW33" s="57">
-        <v>0</v>
-      </c>
-      <c r="AX33" s="57">
-        <v>1</v>
-      </c>
-      <c r="AY33" s="57">
-        <v>1</v>
-      </c>
-      <c r="AZ33" s="57">
-        <v>0</v>
-      </c>
-      <c r="BA33" s="62" t="s">
+      <c r="AQ49" s="46"/>
+      <c r="AR49" s="29">
+        <v>0</v>
+      </c>
+      <c r="AS49" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT49" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU49" s="31">
+        <v>1</v>
+      </c>
+      <c r="AW49" s="40">
+        <v>0</v>
+      </c>
+      <c r="AX49" s="40">
+        <v>1</v>
+      </c>
+      <c r="AY49" s="40">
+        <v>1</v>
+      </c>
+      <c r="AZ49" s="40">
+        <v>0</v>
+      </c>
+      <c r="BA49" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="BB33" s="57" t="s">
+      <c r="BB49" s="40" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="85">
-    <mergeCell ref="AW25:BA25"/>
-    <mergeCell ref="AP27:AQ27"/>
-    <mergeCell ref="AP28:AQ28"/>
-    <mergeCell ref="AP29:AQ29"/>
-    <mergeCell ref="AP30:AQ30"/>
-    <mergeCell ref="AP31:AQ31"/>
+  <mergeCells count="165">
+    <mergeCell ref="AC45:AG45"/>
+    <mergeCell ref="AP45:AQ45"/>
+    <mergeCell ref="P41:T41"/>
+    <mergeCell ref="P42:T42"/>
+    <mergeCell ref="P43:T43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="I45:T45"/>
+    <mergeCell ref="U45:Y45"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="U44:Y44"/>
+    <mergeCell ref="AC44:AG44"/>
+    <mergeCell ref="AP44:AQ44"/>
+    <mergeCell ref="I38:T38"/>
+    <mergeCell ref="I39:T39"/>
+    <mergeCell ref="I40:T40"/>
+    <mergeCell ref="I44:T44"/>
+    <mergeCell ref="U42:Y42"/>
+    <mergeCell ref="AC42:AG42"/>
+    <mergeCell ref="AP42:AQ42"/>
+    <mergeCell ref="U43:Y43"/>
+    <mergeCell ref="AC43:AG43"/>
+    <mergeCell ref="AP43:AQ43"/>
+    <mergeCell ref="U40:Y40"/>
+    <mergeCell ref="AC40:AG40"/>
+    <mergeCell ref="AP40:AQ40"/>
+    <mergeCell ref="U41:Y41"/>
+    <mergeCell ref="AC41:AG41"/>
+    <mergeCell ref="AP41:AQ41"/>
+    <mergeCell ref="U38:Y38"/>
+    <mergeCell ref="AC38:AG38"/>
+    <mergeCell ref="AP38:AQ38"/>
+    <mergeCell ref="U39:Y39"/>
+    <mergeCell ref="AC39:AG39"/>
+    <mergeCell ref="AP39:AQ39"/>
+    <mergeCell ref="AC35:AG35"/>
+    <mergeCell ref="P36:T36"/>
+    <mergeCell ref="U36:Y36"/>
+    <mergeCell ref="AC36:AG36"/>
     <mergeCell ref="AP32:AQ32"/>
     <mergeCell ref="AP33:AQ33"/>
+    <mergeCell ref="AP34:AQ34"/>
+    <mergeCell ref="AP35:AQ35"/>
+    <mergeCell ref="AP36:AQ36"/>
+    <mergeCell ref="AC32:AG32"/>
+    <mergeCell ref="P33:T33"/>
+    <mergeCell ref="U33:Y33"/>
+    <mergeCell ref="AC33:AG33"/>
+    <mergeCell ref="P34:T34"/>
+    <mergeCell ref="U34:Y34"/>
+    <mergeCell ref="AC34:AG34"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="P31:T31"/>
+    <mergeCell ref="U31:Y31"/>
+    <mergeCell ref="P32:T32"/>
+    <mergeCell ref="U32:Y32"/>
+    <mergeCell ref="P35:T35"/>
+    <mergeCell ref="U35:Y35"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="P29:T29"/>
+    <mergeCell ref="U29:Y29"/>
+    <mergeCell ref="AC29:AG29"/>
+    <mergeCell ref="AP29:AQ29"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="J49:S49"/>
+    <mergeCell ref="U49:AB49"/>
+    <mergeCell ref="AC49:AG49"/>
+    <mergeCell ref="I47:O47"/>
+    <mergeCell ref="P47:T47"/>
+    <mergeCell ref="U47:Y47"/>
+    <mergeCell ref="AC47:AG47"/>
+    <mergeCell ref="I46:T46"/>
+    <mergeCell ref="U46:Y46"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="P48:T48"/>
+    <mergeCell ref="U48:Y48"/>
+    <mergeCell ref="AC48:AF48"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="U27:Y27"/>
+    <mergeCell ref="AC27:AG27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="P28:T28"/>
+    <mergeCell ref="U28:Y28"/>
+    <mergeCell ref="AC28:AG28"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="I37:T37"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="AP2:AU2"/>
+    <mergeCell ref="AP11:AQ11"/>
+    <mergeCell ref="AP10:AQ10"/>
+    <mergeCell ref="AP9:AQ9"/>
+    <mergeCell ref="AP8:AQ8"/>
+    <mergeCell ref="AP7:AQ7"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AC46:AG46"/>
+    <mergeCell ref="P17:T17"/>
+    <mergeCell ref="U17:Y17"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="AC23:AG23"/>
+    <mergeCell ref="I20:AB20"/>
+    <mergeCell ref="J23:S23"/>
+    <mergeCell ref="U23:AB23"/>
+    <mergeCell ref="AC17:AF17"/>
+    <mergeCell ref="U37:Y37"/>
+    <mergeCell ref="AC37:AG37"/>
+    <mergeCell ref="P27:T27"/>
+    <mergeCell ref="P30:T30"/>
+    <mergeCell ref="U30:Y30"/>
+    <mergeCell ref="AC30:AG30"/>
+    <mergeCell ref="AC31:AG31"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="I14:O14"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="AH23:AN23"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="AH17:AN17"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="AC20:AG20"/>
+    <mergeCell ref="AH20:AN20"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="I11:T11"/>
+    <mergeCell ref="U14:Y14"/>
+    <mergeCell ref="Z14:AB14"/>
+    <mergeCell ref="AC14:AG14"/>
+    <mergeCell ref="AP47:AQ47"/>
+    <mergeCell ref="AP48:AQ48"/>
+    <mergeCell ref="AP49:AQ49"/>
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="I8:O8"/>
     <mergeCell ref="P8:T8"/>
@@ -2949,71 +4842,16 @@
     <mergeCell ref="AH11:AN11"/>
     <mergeCell ref="AH14:AN14"/>
     <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="I14:O14"/>
-    <mergeCell ref="P14:T14"/>
-    <mergeCell ref="AH23:AN23"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="AH17:AN17"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="AC20:AG20"/>
-    <mergeCell ref="AH20:AN20"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="AC30:AG30"/>
-    <mergeCell ref="P17:T17"/>
-    <mergeCell ref="U17:Y17"/>
-    <mergeCell ref="Z17:AB17"/>
-    <mergeCell ref="AC23:AG23"/>
-    <mergeCell ref="I11:T11"/>
-    <mergeCell ref="I20:AB20"/>
-    <mergeCell ref="J23:S23"/>
-    <mergeCell ref="U23:AB23"/>
-    <mergeCell ref="AC17:AF17"/>
-    <mergeCell ref="U14:Y14"/>
-    <mergeCell ref="Z14:AB14"/>
-    <mergeCell ref="AC14:AG14"/>
-    <mergeCell ref="AP2:AU2"/>
-    <mergeCell ref="AP11:AQ11"/>
-    <mergeCell ref="AP10:AQ10"/>
-    <mergeCell ref="AP9:AQ9"/>
-    <mergeCell ref="AP8:AQ8"/>
-    <mergeCell ref="AP7:AQ7"/>
-    <mergeCell ref="AP6:AQ6"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AW25:BA25"/>
+    <mergeCell ref="AP27:AQ27"/>
+    <mergeCell ref="AP28:AQ28"/>
+    <mergeCell ref="AP37:AQ37"/>
+    <mergeCell ref="AP46:AQ46"/>
     <mergeCell ref="AP26:AS26"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="P32:T32"/>
-    <mergeCell ref="U32:Y32"/>
-    <mergeCell ref="AC32:AF32"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="U27:Y27"/>
-    <mergeCell ref="AC27:AG27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="P28:T28"/>
-    <mergeCell ref="U28:Y28"/>
-    <mergeCell ref="AC28:AG28"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="I29:T29"/>
-    <mergeCell ref="J32:O32"/>
-    <mergeCell ref="U29:Y29"/>
-    <mergeCell ref="AC29:AG29"/>
-    <mergeCell ref="I31:O31"/>
-    <mergeCell ref="P31:T31"/>
-    <mergeCell ref="U31:Y31"/>
-    <mergeCell ref="AC31:AG31"/>
-    <mergeCell ref="I30:T30"/>
-    <mergeCell ref="P27:T27"/>
-    <mergeCell ref="U30:Y30"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="J33:S33"/>
-    <mergeCell ref="U33:AB33"/>
-    <mergeCell ref="AC33:AG33"/>
+    <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="AP31:AQ31"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
fixed some typos in decoder and added support for full RV32I R-type instr
</commit_message>
<xml_diff>
--- a/doc/decoding.xlsx
+++ b/doc/decoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\SystemVerilog\FRiscV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9667E23-ED1C-44AD-A3DF-8CD476F56A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1E9745-FB62-4700-9221-11089E3FD7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="69">
   <si>
     <t>R-TYPE</t>
   </si>
@@ -1270,7 +1270,7 @@
       <pane xSplit="7" ySplit="23" topLeftCell="H24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="AW19" sqref="AW19"/>
+      <selection pane="bottomRight" activeCell="P34" sqref="P34:T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2586,6 +2586,9 @@
       </c>
     </row>
     <row r="29" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D29" s="48" t="s">
         <v>31</v>
       </c>
@@ -2701,6 +2704,9 @@
       </c>
     </row>
     <row r="30" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D30" s="48" t="s">
         <v>30</v>
       </c>
@@ -2816,6 +2822,9 @@
       </c>
     </row>
     <row r="31" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D31" s="48" t="s">
         <v>29</v>
       </c>
@@ -2931,6 +2940,9 @@
       </c>
     </row>
     <row r="32" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D32" s="48" t="s">
         <v>33</v>
       </c>
@@ -3046,6 +3058,9 @@
       </c>
     </row>
     <row r="33" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D33" s="48" t="s">
         <v>59</v>
       </c>
@@ -3161,6 +3176,9 @@
       </c>
     </row>
     <row r="34" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D34" s="48" t="s">
         <v>58</v>
       </c>
@@ -3276,6 +3294,9 @@
       </c>
     </row>
     <row r="35" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D35" s="48" t="s">
         <v>32</v>
       </c>
@@ -3391,6 +3412,9 @@
       </c>
     </row>
     <row r="36" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D36" s="48" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
added logic for immediate load instructions. Required additional module to extend byte/half/word loads from memory
</commit_message>
<xml_diff>
--- a/doc/decoding.xlsx
+++ b/doc/decoding.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\SystemVerilog\FRiscV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1E9745-FB62-4700-9221-11089E3FD7EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181436AF-1440-4318-AF20-A03FA9598AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
+    <workbookView xWindow="28305" yWindow="915" windowWidth="25965" windowHeight="14595" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$27:$BB$36</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="D48" authorId="0" shapeId="0" xr:uid="{E8182568-AF53-41D0-80C8-04611138DC73}">
+    <comment ref="D53" authorId="0" shapeId="0" xr:uid="{E8182568-AF53-41D0-80C8-04611138DC73}">
       <text>
         <r>
           <rPr>
@@ -61,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW48" authorId="0" shapeId="0" xr:uid="{EC372BE6-EF51-477F-B18A-BFF0C74E0CC5}">
+    <comment ref="AW53" authorId="0" shapeId="0" xr:uid="{EC372BE6-EF51-477F-B18A-BFF0C74E0CC5}">
       <text>
         <r>
           <rPr>
@@ -86,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D49" authorId="0" shapeId="0" xr:uid="{94E066D9-6740-478B-B1BE-00F56432855D}">
+    <comment ref="D54" authorId="0" shapeId="0" xr:uid="{94E066D9-6740-478B-B1BE-00F56432855D}">
       <text>
         <r>
           <rPr>
@@ -115,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="74">
   <si>
     <t>R-TYPE</t>
   </si>
@@ -322,6 +325,21 @@
   </si>
   <si>
     <t>SLTIU</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>LH</t>
+  </si>
+  <si>
+    <t>LBU</t>
+  </si>
+  <si>
+    <t>LHU</t>
+  </si>
+  <si>
+    <t>JALR</t>
   </si>
 </sst>
 </file>
@@ -730,7 +748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -850,6 +868,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1264,16 +1294,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA95D64-5055-4174-A4D5-0BDBECB18FB0}">
-  <dimension ref="C1:BB49"/>
+  <dimension ref="C1:BB54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="23" topLeftCell="H24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="23" topLeftCell="J24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="P34" sqref="P34:T34"/>
+      <selection pane="bottomRight" activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="4.7109375" style="3"/>
     <col min="3" max="3" width="7.42578125" style="3" customWidth="1"/>
@@ -1295,20 +1325,20 @@
   <sheetData>
     <row r="1" spans="4:47" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP2" s="65" t="s">
+      <c r="AP2" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="AQ2" s="66"/>
-      <c r="AR2" s="66"/>
-      <c r="AS2" s="66"/>
-      <c r="AT2" s="66"/>
-      <c r="AU2" s="67"/>
+      <c r="AQ2" s="70"/>
+      <c r="AR2" s="70"/>
+      <c r="AS2" s="70"/>
+      <c r="AT2" s="70"/>
+      <c r="AU2" s="71"/>
     </row>
     <row r="3" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP3" s="68" t="s">
+      <c r="AP3" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="53"/>
+      <c r="AQ3" s="57"/>
       <c r="AR3" s="21">
         <v>0</v>
       </c>
@@ -1318,15 +1348,15 @@
       <c r="AT3" s="21">
         <v>0</v>
       </c>
-      <c r="AU3" s="69">
+      <c r="AU3" s="73">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP4" s="70" t="s">
+      <c r="AP4" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="AQ4" s="52"/>
+      <c r="AQ4" s="56"/>
       <c r="AR4" s="21">
         <v>0</v>
       </c>
@@ -1336,7 +1366,7 @@
       <c r="AT4" s="21">
         <v>0</v>
       </c>
-      <c r="AU4" s="69">
+      <c r="AU4" s="73">
         <v>1</v>
       </c>
     </row>
@@ -1437,10 +1467,10 @@
       <c r="AN5" s="2">
         <v>0</v>
       </c>
-      <c r="AP5" s="70" t="s">
+      <c r="AP5" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="AQ5" s="52"/>
+      <c r="AQ5" s="56"/>
       <c r="AR5" s="21">
         <v>0</v>
       </c>
@@ -1450,7 +1480,7 @@
       <c r="AT5" s="21">
         <v>1</v>
       </c>
-      <c r="AU5" s="69">
+      <c r="AU5" s="73">
         <v>0</v>
       </c>
     </row>
@@ -1487,10 +1517,10 @@
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
-      <c r="AP6" s="70" t="s">
+      <c r="AP6" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="AQ6" s="52"/>
+      <c r="AQ6" s="56"/>
       <c r="AR6" s="21">
         <v>0</v>
       </c>
@@ -1500,7 +1530,7 @@
       <c r="AT6" s="21">
         <v>1</v>
       </c>
-      <c r="AU6" s="69">
+      <c r="AU6" s="73">
         <v>1</v>
       </c>
     </row>
@@ -1541,10 +1571,10 @@
       <c r="AN7" s="3">
         <v>0</v>
       </c>
-      <c r="AP7" s="70" t="s">
+      <c r="AP7" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="AQ7" s="52"/>
+      <c r="AQ7" s="56"/>
       <c r="AR7" s="21">
         <v>0</v>
       </c>
@@ -1554,65 +1584,65 @@
       <c r="AT7" s="21">
         <v>0</v>
       </c>
-      <c r="AU7" s="69">
+      <c r="AU7" s="73">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="I8" s="49" t="s">
+      <c r="D8" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="I8" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="44" t="s">
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="44" t="s">
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="46"/>
-      <c r="Z8" s="44" t="s">
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="50"/>
+      <c r="Z8" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="45"/>
-      <c r="AB8" s="46"/>
-      <c r="AC8" s="44" t="s">
+      <c r="AA8" s="49"/>
+      <c r="AB8" s="50"/>
+      <c r="AC8" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD8" s="45"/>
-      <c r="AE8" s="45"/>
-      <c r="AF8" s="45"/>
-      <c r="AG8" s="46"/>
-      <c r="AH8" s="44" t="s">
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="50"/>
+      <c r="AH8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AI8" s="45"/>
-      <c r="AJ8" s="45"/>
-      <c r="AK8" s="45"/>
-      <c r="AL8" s="45"/>
-      <c r="AM8" s="45"/>
-      <c r="AN8" s="56"/>
-      <c r="AP8" s="70" t="s">
+      <c r="AI8" s="49"/>
+      <c r="AJ8" s="49"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="49"/>
+      <c r="AM8" s="49"/>
+      <c r="AN8" s="60"/>
+      <c r="AP8" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="AQ8" s="52"/>
+      <c r="AQ8" s="56"/>
       <c r="AR8" s="21">
         <v>0</v>
       </c>
@@ -1622,7 +1652,7 @@
       <c r="AT8" s="21">
         <v>0</v>
       </c>
-      <c r="AU8" s="69">
+      <c r="AU8" s="73">
         <v>1</v>
       </c>
     </row>
@@ -1663,10 +1693,10 @@
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
-      <c r="AP9" s="70" t="s">
+      <c r="AP9" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="AQ9" s="52"/>
+      <c r="AQ9" s="56"/>
       <c r="AR9" s="21">
         <v>0</v>
       </c>
@@ -1676,7 +1706,7 @@
       <c r="AT9" s="21">
         <v>1</v>
       </c>
-      <c r="AU9" s="69">
+      <c r="AU9" s="73">
         <v>0</v>
       </c>
     </row>
@@ -1715,10 +1745,10 @@
       <c r="AN10" s="3">
         <v>0</v>
       </c>
-      <c r="AP10" s="70" t="s">
+      <c r="AP10" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="AQ10" s="52"/>
+      <c r="AQ10" s="56"/>
       <c r="AR10" s="21">
         <v>0</v>
       </c>
@@ -1728,73 +1758,73 @@
       <c r="AT10" s="21">
         <v>1</v>
       </c>
-      <c r="AU10" s="69">
+      <c r="AU10" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="I11" s="49" t="s">
+      <c r="D11" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="I11" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="44" t="s">
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V11" s="45"/>
-      <c r="W11" s="45"/>
-      <c r="X11" s="45"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="44" t="s">
+      <c r="V11" s="49"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="50"/>
+      <c r="Z11" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AA11" s="45"/>
-      <c r="AB11" s="46"/>
-      <c r="AC11" s="44" t="s">
+      <c r="AA11" s="49"/>
+      <c r="AB11" s="50"/>
+      <c r="AC11" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD11" s="45"/>
-      <c r="AE11" s="45"/>
-      <c r="AF11" s="45"/>
-      <c r="AG11" s="46"/>
-      <c r="AH11" s="44" t="s">
+      <c r="AD11" s="49"/>
+      <c r="AE11" s="49"/>
+      <c r="AF11" s="49"/>
+      <c r="AG11" s="50"/>
+      <c r="AH11" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AI11" s="45"/>
-      <c r="AJ11" s="45"/>
-      <c r="AK11" s="45"/>
-      <c r="AL11" s="45"/>
-      <c r="AM11" s="45"/>
-      <c r="AN11" s="56"/>
-      <c r="AP11" s="71" t="s">
+      <c r="AI11" s="49"/>
+      <c r="AJ11" s="49"/>
+      <c r="AK11" s="49"/>
+      <c r="AL11" s="49"/>
+      <c r="AM11" s="49"/>
+      <c r="AN11" s="60"/>
+      <c r="AP11" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="AQ11" s="72"/>
-      <c r="AR11" s="73">
-        <v>1</v>
-      </c>
-      <c r="AS11" s="73">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="73">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="74">
+      <c r="AQ11" s="76"/>
+      <c r="AR11" s="77">
+        <v>1</v>
+      </c>
+      <c r="AS11" s="77">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="77">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="78">
         <v>0</v>
       </c>
     </row>
@@ -1835,12 +1865,12 @@
       <c r="AL12" s="4"/>
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
-      <c r="AP12" s="63"/>
-      <c r="AQ12" s="63"/>
-      <c r="AR12" s="64"/>
-      <c r="AS12" s="64"/>
-      <c r="AT12" s="64"/>
-      <c r="AU12" s="64"/>
+      <c r="AP12" s="67"/>
+      <c r="AQ12" s="67"/>
+      <c r="AR12" s="68"/>
+      <c r="AS12" s="68"/>
+      <c r="AT12" s="68"/>
+      <c r="AU12" s="68"/>
     </row>
     <row r="13" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="5"/>
@@ -1885,56 +1915,56 @@
       </c>
     </row>
     <row r="14" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="55" t="s">
+      <c r="D14" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="I14" s="49" t="s">
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="I14" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="44" t="s">
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="46"/>
-      <c r="U14" s="44" t="s">
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V14" s="45"/>
-      <c r="W14" s="45"/>
-      <c r="X14" s="45"/>
-      <c r="Y14" s="46"/>
-      <c r="Z14" s="44" t="s">
+      <c r="V14" s="49"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49"/>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AA14" s="45"/>
-      <c r="AB14" s="46"/>
-      <c r="AC14" s="44" t="s">
+      <c r="AA14" s="49"/>
+      <c r="AB14" s="50"/>
+      <c r="AC14" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="AD14" s="45"/>
-      <c r="AE14" s="45"/>
-      <c r="AF14" s="45"/>
-      <c r="AG14" s="46"/>
-      <c r="AH14" s="44" t="s">
+      <c r="AD14" s="49"/>
+      <c r="AE14" s="49"/>
+      <c r="AF14" s="49"/>
+      <c r="AG14" s="50"/>
+      <c r="AH14" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AI14" s="45"/>
-      <c r="AJ14" s="45"/>
-      <c r="AK14" s="45"/>
-      <c r="AL14" s="45"/>
-      <c r="AM14" s="45"/>
-      <c r="AN14" s="56"/>
+      <c r="AI14" s="49"/>
+      <c r="AJ14" s="49"/>
+      <c r="AK14" s="49"/>
+      <c r="AL14" s="49"/>
+      <c r="AM14" s="49"/>
+      <c r="AN14" s="60"/>
     </row>
     <row r="15" spans="4:47" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
@@ -2020,60 +2050,60 @@
       </c>
     </row>
     <row r="17" spans="3:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
       <c r="I17" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="49" t="s">
+      <c r="J17" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="44" t="s">
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="46"/>
-      <c r="U17" s="44" t="s">
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V17" s="45"/>
-      <c r="W17" s="45"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="46"/>
-      <c r="Z17" s="44" t="s">
+      <c r="V17" s="49"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="AA17" s="45"/>
-      <c r="AB17" s="46"/>
-      <c r="AC17" s="44" t="s">
+      <c r="AA17" s="49"/>
+      <c r="AB17" s="50"/>
+      <c r="AC17" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="AD17" s="45"/>
-      <c r="AE17" s="45"/>
-      <c r="AF17" s="46"/>
+      <c r="AD17" s="49"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="50"/>
       <c r="AG17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AH17" s="44" t="s">
+      <c r="AH17" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AI17" s="45"/>
-      <c r="AJ17" s="45"/>
-      <c r="AK17" s="45"/>
-      <c r="AL17" s="45"/>
-      <c r="AM17" s="45"/>
-      <c r="AN17" s="56"/>
+      <c r="AI17" s="49"/>
+      <c r="AJ17" s="49"/>
+      <c r="AK17" s="49"/>
+      <c r="AL17" s="49"/>
+      <c r="AM17" s="49"/>
+      <c r="AN17" s="60"/>
     </row>
     <row r="18" spans="3:54" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
@@ -2138,50 +2168,50 @@
       </c>
     </row>
     <row r="20" spans="3:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="I20" s="49" t="s">
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="I20" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-      <c r="U20" s="45"/>
-      <c r="V20" s="45"/>
-      <c r="W20" s="45"/>
-      <c r="X20" s="45"/>
-      <c r="Y20" s="45"/>
-      <c r="Z20" s="45"/>
-      <c r="AA20" s="45"/>
-      <c r="AB20" s="46"/>
-      <c r="AC20" s="44" t="s">
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="49"/>
+      <c r="V20" s="49"/>
+      <c r="W20" s="49"/>
+      <c r="X20" s="49"/>
+      <c r="Y20" s="49"/>
+      <c r="Z20" s="49"/>
+      <c r="AA20" s="49"/>
+      <c r="AB20" s="50"/>
+      <c r="AC20" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD20" s="45"/>
-      <c r="AE20" s="45"/>
-      <c r="AF20" s="45"/>
-      <c r="AG20" s="46"/>
-      <c r="AH20" s="44" t="s">
+      <c r="AD20" s="49"/>
+      <c r="AE20" s="49"/>
+      <c r="AF20" s="49"/>
+      <c r="AG20" s="50"/>
+      <c r="AH20" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AI20" s="45"/>
-      <c r="AJ20" s="45"/>
-      <c r="AK20" s="45"/>
-      <c r="AL20" s="45"/>
-      <c r="AM20" s="45"/>
-      <c r="AN20" s="56"/>
+      <c r="AI20" s="49"/>
+      <c r="AJ20" s="49"/>
+      <c r="AK20" s="49"/>
+      <c r="AL20" s="49"/>
+      <c r="AM20" s="49"/>
+      <c r="AN20" s="60"/>
     </row>
     <row r="21" spans="3:54" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
@@ -2232,6 +2262,12 @@
       <c r="J22" s="3">
         <v>30</v>
       </c>
+      <c r="O22" s="3">
+        <v>25</v>
+      </c>
+      <c r="P22" s="3">
+        <v>24</v>
+      </c>
       <c r="S22" s="3">
         <v>21</v>
       </c>
@@ -2258,76 +2294,76 @@
       </c>
     </row>
     <row r="23" spans="3:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
       <c r="I23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="44" t="s">
+      <c r="J23" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="45"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
       <c r="T23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U23" s="44" t="s">
+      <c r="U23" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="V23" s="45"/>
-      <c r="W23" s="45"/>
-      <c r="X23" s="45"/>
-      <c r="Y23" s="45"/>
-      <c r="Z23" s="45"/>
-      <c r="AA23" s="45"/>
-      <c r="AB23" s="46"/>
-      <c r="AC23" s="44" t="s">
+      <c r="V23" s="49"/>
+      <c r="W23" s="49"/>
+      <c r="X23" s="49"/>
+      <c r="Y23" s="49"/>
+      <c r="Z23" s="49"/>
+      <c r="AA23" s="49"/>
+      <c r="AB23" s="50"/>
+      <c r="AC23" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD23" s="45"/>
-      <c r="AE23" s="45"/>
-      <c r="AF23" s="45"/>
-      <c r="AG23" s="46"/>
-      <c r="AH23" s="44" t="s">
+      <c r="AD23" s="49"/>
+      <c r="AE23" s="49"/>
+      <c r="AF23" s="49"/>
+      <c r="AG23" s="50"/>
+      <c r="AH23" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="AI23" s="45"/>
-      <c r="AJ23" s="45"/>
-      <c r="AK23" s="45"/>
-      <c r="AL23" s="45"/>
-      <c r="AM23" s="45"/>
-      <c r="AN23" s="56"/>
+      <c r="AI23" s="49"/>
+      <c r="AJ23" s="49"/>
+      <c r="AK23" s="49"/>
+      <c r="AL23" s="49"/>
+      <c r="AM23" s="49"/>
+      <c r="AN23" s="60"/>
     </row>
     <row r="25" spans="3:54" ht="15" x14ac:dyDescent="0.25">
-      <c r="AW25" s="61" t="s">
+      <c r="AW25" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="AX25" s="61"/>
-      <c r="AY25" s="61"/>
-      <c r="AZ25" s="61"/>
-      <c r="BA25" s="61"/>
+      <c r="AX25" s="65"/>
+      <c r="AY25" s="65"/>
+      <c r="AZ25" s="65"/>
+      <c r="BA25" s="65"/>
     </row>
     <row r="26" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="AP26" s="62" t="s">
+      <c r="AP26" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="AQ26" s="62"/>
-      <c r="AR26" s="62"/>
-      <c r="AS26" s="62"/>
+      <c r="AQ26" s="66"/>
+      <c r="AR26" s="66"/>
+      <c r="AS26" s="66"/>
       <c r="AT26" s="22"/>
       <c r="AU26" s="22"/>
       <c r="AW26" s="38" t="s">
@@ -2349,14 +2385,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="48" t="s">
+      <c r="D27" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="48"/>
+      <c r="E27" s="52"/>
       <c r="F27" s="19" t="s">
         <v>27</v>
       </c>
@@ -2381,20 +2417,20 @@
       <c r="O27" s="10">
         <v>0</v>
       </c>
-      <c r="P27" s="44" t="s">
+      <c r="P27" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="46"/>
-      <c r="U27" s="44" t="s">
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V27" s="45"/>
-      <c r="W27" s="45"/>
-      <c r="X27" s="45"/>
-      <c r="Y27" s="46"/>
+      <c r="V27" s="49"/>
+      <c r="W27" s="49"/>
+      <c r="X27" s="49"/>
+      <c r="Y27" s="50"/>
       <c r="Z27" s="16">
         <v>0</v>
       </c>
@@ -2404,13 +2440,13 @@
       <c r="AB27" s="18">
         <v>0</v>
       </c>
-      <c r="AC27" s="44" t="s">
+      <c r="AC27" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD27" s="45"/>
-      <c r="AE27" s="45"/>
-      <c r="AF27" s="45"/>
-      <c r="AG27" s="46"/>
+      <c r="AD27" s="49"/>
+      <c r="AE27" s="49"/>
+      <c r="AF27" s="49"/>
+      <c r="AG27" s="50"/>
       <c r="AH27" s="8">
         <v>0</v>
       </c>
@@ -2432,10 +2468,10 @@
       <c r="AN27" s="15">
         <v>1</v>
       </c>
-      <c r="AP27" s="47" t="s">
+      <c r="AP27" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="AQ27" s="47"/>
+      <c r="AQ27" s="51"/>
       <c r="AR27" s="23">
         <v>0</v>
       </c>
@@ -2467,14 +2503,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="48"/>
+      <c r="E28" s="52"/>
       <c r="F28" s="19" t="s">
         <v>27</v>
       </c>
@@ -2499,20 +2535,20 @@
       <c r="O28" s="10">
         <v>0</v>
       </c>
-      <c r="P28" s="44" t="s">
+      <c r="P28" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="46"/>
-      <c r="U28" s="44" t="s">
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V28" s="45"/>
-      <c r="W28" s="45"/>
-      <c r="X28" s="45"/>
-      <c r="Y28" s="46"/>
+      <c r="V28" s="49"/>
+      <c r="W28" s="49"/>
+      <c r="X28" s="49"/>
+      <c r="Y28" s="50"/>
       <c r="Z28" s="16">
         <v>0</v>
       </c>
@@ -2522,13 +2558,13 @@
       <c r="AB28" s="18">
         <v>0</v>
       </c>
-      <c r="AC28" s="44" t="s">
+      <c r="AC28" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD28" s="45"/>
-      <c r="AE28" s="45"/>
-      <c r="AF28" s="45"/>
-      <c r="AG28" s="46"/>
+      <c r="AD28" s="49"/>
+      <c r="AE28" s="49"/>
+      <c r="AF28" s="49"/>
+      <c r="AG28" s="50"/>
       <c r="AH28" s="8">
         <v>0</v>
       </c>
@@ -2550,10 +2586,10 @@
       <c r="AN28" s="15">
         <v>1</v>
       </c>
-      <c r="AP28" s="47" t="s">
+      <c r="AP28" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="AQ28" s="47"/>
+      <c r="AQ28" s="51"/>
       <c r="AR28" s="26">
         <v>0</v>
       </c>
@@ -2585,14 +2621,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="48" t="s">
+      <c r="D29" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="48"/>
+      <c r="E29" s="52"/>
       <c r="F29" s="19" t="s">
         <v>27</v>
       </c>
@@ -2617,20 +2653,20 @@
       <c r="O29" s="34">
         <v>0</v>
       </c>
-      <c r="P29" s="44" t="s">
+      <c r="P29" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="46"/>
-      <c r="U29" s="44" t="s">
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V29" s="45"/>
-      <c r="W29" s="45"/>
-      <c r="X29" s="45"/>
-      <c r="Y29" s="46"/>
+      <c r="V29" s="49"/>
+      <c r="W29" s="49"/>
+      <c r="X29" s="49"/>
+      <c r="Y29" s="50"/>
       <c r="Z29" s="16">
         <v>1</v>
       </c>
@@ -2640,13 +2676,13 @@
       <c r="AB29" s="18">
         <v>0</v>
       </c>
-      <c r="AC29" s="44" t="s">
+      <c r="AC29" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD29" s="45"/>
-      <c r="AE29" s="45"/>
-      <c r="AF29" s="45"/>
-      <c r="AG29" s="46"/>
+      <c r="AD29" s="49"/>
+      <c r="AE29" s="49"/>
+      <c r="AF29" s="49"/>
+      <c r="AG29" s="50"/>
       <c r="AH29" s="32">
         <v>0</v>
       </c>
@@ -2668,10 +2704,10 @@
       <c r="AN29" s="36">
         <v>1</v>
       </c>
-      <c r="AP29" s="50" t="s">
+      <c r="AP29" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="AQ29" s="51"/>
+      <c r="AQ29" s="55"/>
       <c r="AR29" s="26">
         <v>0</v>
       </c>
@@ -2703,14 +2739,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="48" t="s">
+      <c r="D30" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="48"/>
+      <c r="E30" s="52"/>
       <c r="F30" s="19" t="s">
         <v>27</v>
       </c>
@@ -2735,20 +2771,20 @@
       <c r="O30" s="34">
         <v>0</v>
       </c>
-      <c r="P30" s="44" t="s">
+      <c r="P30" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="46"/>
-      <c r="U30" s="44" t="s">
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V30" s="45"/>
-      <c r="W30" s="45"/>
-      <c r="X30" s="45"/>
-      <c r="Y30" s="46"/>
+      <c r="V30" s="49"/>
+      <c r="W30" s="49"/>
+      <c r="X30" s="49"/>
+      <c r="Y30" s="50"/>
       <c r="Z30" s="16">
         <v>1</v>
       </c>
@@ -2758,13 +2794,13 @@
       <c r="AB30" s="18">
         <v>0</v>
       </c>
-      <c r="AC30" s="44" t="s">
+      <c r="AC30" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD30" s="45"/>
-      <c r="AE30" s="45"/>
-      <c r="AF30" s="45"/>
-      <c r="AG30" s="46"/>
+      <c r="AD30" s="49"/>
+      <c r="AE30" s="49"/>
+      <c r="AF30" s="49"/>
+      <c r="AG30" s="50"/>
       <c r="AH30" s="32">
         <v>0</v>
       </c>
@@ -2786,10 +2822,10 @@
       <c r="AN30" s="36">
         <v>1</v>
       </c>
-      <c r="AP30" s="50" t="s">
+      <c r="AP30" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="AQ30" s="51"/>
+      <c r="AQ30" s="55"/>
       <c r="AR30" s="26">
         <v>0</v>
       </c>
@@ -2821,14 +2857,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="48" t="s">
+      <c r="D31" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="48"/>
+      <c r="E31" s="52"/>
       <c r="F31" s="19" t="s">
         <v>27</v>
       </c>
@@ -2853,20 +2889,20 @@
       <c r="O31" s="34">
         <v>0</v>
       </c>
-      <c r="P31" s="44" t="s">
+      <c r="P31" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="45"/>
-      <c r="T31" s="46"/>
-      <c r="U31" s="44" t="s">
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
+      <c r="T31" s="50"/>
+      <c r="U31" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V31" s="45"/>
-      <c r="W31" s="45"/>
-      <c r="X31" s="45"/>
-      <c r="Y31" s="46"/>
+      <c r="V31" s="49"/>
+      <c r="W31" s="49"/>
+      <c r="X31" s="49"/>
+      <c r="Y31" s="50"/>
       <c r="Z31" s="16">
         <v>1</v>
       </c>
@@ -2876,13 +2912,13 @@
       <c r="AB31" s="18">
         <v>1</v>
       </c>
-      <c r="AC31" s="44" t="s">
+      <c r="AC31" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD31" s="45"/>
-      <c r="AE31" s="45"/>
-      <c r="AF31" s="45"/>
-      <c r="AG31" s="46"/>
+      <c r="AD31" s="49"/>
+      <c r="AE31" s="49"/>
+      <c r="AF31" s="49"/>
+      <c r="AG31" s="50"/>
       <c r="AH31" s="32">
         <v>0</v>
       </c>
@@ -2904,10 +2940,10 @@
       <c r="AN31" s="36">
         <v>1</v>
       </c>
-      <c r="AP31" s="50" t="s">
+      <c r="AP31" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="AQ31" s="51"/>
+      <c r="AQ31" s="55"/>
       <c r="AR31" s="26">
         <v>0</v>
       </c>
@@ -2939,14 +2975,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="48" t="s">
+      <c r="D32" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="48"/>
+      <c r="E32" s="52"/>
       <c r="F32" s="19" t="s">
         <v>27</v>
       </c>
@@ -2971,20 +3007,20 @@
       <c r="O32" s="34">
         <v>0</v>
       </c>
-      <c r="P32" s="44" t="s">
+      <c r="P32" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q32" s="45"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="44" t="s">
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
+      <c r="T32" s="50"/>
+      <c r="U32" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V32" s="45"/>
-      <c r="W32" s="45"/>
-      <c r="X32" s="45"/>
-      <c r="Y32" s="46"/>
+      <c r="V32" s="49"/>
+      <c r="W32" s="49"/>
+      <c r="X32" s="49"/>
+      <c r="Y32" s="50"/>
       <c r="Z32" s="16">
         <v>0</v>
       </c>
@@ -2994,13 +3030,13 @@
       <c r="AB32" s="18">
         <v>1</v>
       </c>
-      <c r="AC32" s="44" t="s">
+      <c r="AC32" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD32" s="45"/>
-      <c r="AE32" s="45"/>
-      <c r="AF32" s="45"/>
-      <c r="AG32" s="46"/>
+      <c r="AD32" s="49"/>
+      <c r="AE32" s="49"/>
+      <c r="AF32" s="49"/>
+      <c r="AG32" s="50"/>
       <c r="AH32" s="32">
         <v>0</v>
       </c>
@@ -3022,10 +3058,10 @@
       <c r="AN32" s="36">
         <v>1</v>
       </c>
-      <c r="AP32" s="50" t="s">
+      <c r="AP32" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="AQ32" s="51"/>
+      <c r="AQ32" s="55"/>
       <c r="AR32" s="26">
         <v>0</v>
       </c>
@@ -3057,14 +3093,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="48" t="s">
+      <c r="D33" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="48"/>
+      <c r="E33" s="52"/>
       <c r="F33" s="19" t="s">
         <v>27</v>
       </c>
@@ -3089,20 +3125,20 @@
       <c r="O33" s="34">
         <v>0</v>
       </c>
-      <c r="P33" s="44" t="s">
+      <c r="P33" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="44" t="s">
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+      <c r="T33" s="50"/>
+      <c r="U33" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V33" s="45"/>
-      <c r="W33" s="45"/>
-      <c r="X33" s="45"/>
-      <c r="Y33" s="46"/>
+      <c r="V33" s="49"/>
+      <c r="W33" s="49"/>
+      <c r="X33" s="49"/>
+      <c r="Y33" s="50"/>
       <c r="Z33" s="16">
         <v>1</v>
       </c>
@@ -3112,13 +3148,13 @@
       <c r="AB33" s="18">
         <v>1</v>
       </c>
-      <c r="AC33" s="44" t="s">
+      <c r="AC33" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD33" s="45"/>
-      <c r="AE33" s="45"/>
-      <c r="AF33" s="45"/>
-      <c r="AG33" s="46"/>
+      <c r="AD33" s="49"/>
+      <c r="AE33" s="49"/>
+      <c r="AF33" s="49"/>
+      <c r="AG33" s="50"/>
       <c r="AH33" s="32">
         <v>0</v>
       </c>
@@ -3140,10 +3176,10 @@
       <c r="AN33" s="36">
         <v>1</v>
       </c>
-      <c r="AP33" s="50" t="s">
+      <c r="AP33" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="AQ33" s="51"/>
+      <c r="AQ33" s="55"/>
       <c r="AR33" s="26">
         <v>1</v>
       </c>
@@ -3175,14 +3211,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="48"/>
+      <c r="E34" s="52"/>
       <c r="F34" s="19" t="s">
         <v>27</v>
       </c>
@@ -3207,20 +3243,20 @@
       <c r="O34" s="34">
         <v>0</v>
       </c>
-      <c r="P34" s="44" t="s">
+      <c r="P34" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q34" s="45"/>
-      <c r="R34" s="45"/>
-      <c r="S34" s="45"/>
-      <c r="T34" s="46"/>
-      <c r="U34" s="44" t="s">
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="50"/>
+      <c r="U34" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V34" s="45"/>
-      <c r="W34" s="45"/>
-      <c r="X34" s="45"/>
-      <c r="Y34" s="46"/>
+      <c r="V34" s="49"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="49"/>
+      <c r="Y34" s="50"/>
       <c r="Z34" s="16">
         <v>1</v>
       </c>
@@ -3230,13 +3266,13 @@
       <c r="AB34" s="18">
         <v>1</v>
       </c>
-      <c r="AC34" s="44" t="s">
+      <c r="AC34" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD34" s="45"/>
-      <c r="AE34" s="45"/>
-      <c r="AF34" s="45"/>
-      <c r="AG34" s="46"/>
+      <c r="AD34" s="49"/>
+      <c r="AE34" s="49"/>
+      <c r="AF34" s="49"/>
+      <c r="AG34" s="50"/>
       <c r="AH34" s="32">
         <v>0</v>
       </c>
@@ -3258,10 +3294,10 @@
       <c r="AN34" s="36">
         <v>1</v>
       </c>
-      <c r="AP34" s="50" t="s">
+      <c r="AP34" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="AQ34" s="51"/>
+      <c r="AQ34" s="55"/>
       <c r="AR34" s="26">
         <v>0</v>
       </c>
@@ -3293,14 +3329,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="48" t="s">
+      <c r="D35" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="48"/>
+      <c r="E35" s="52"/>
       <c r="F35" s="19" t="s">
         <v>27</v>
       </c>
@@ -3325,20 +3361,20 @@
       <c r="O35" s="34">
         <v>0</v>
       </c>
-      <c r="P35" s="44" t="s">
+      <c r="P35" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q35" s="45"/>
-      <c r="R35" s="45"/>
-      <c r="S35" s="45"/>
-      <c r="T35" s="46"/>
-      <c r="U35" s="44" t="s">
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="50"/>
+      <c r="U35" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V35" s="45"/>
-      <c r="W35" s="45"/>
-      <c r="X35" s="45"/>
-      <c r="Y35" s="46"/>
+      <c r="V35" s="49"/>
+      <c r="W35" s="49"/>
+      <c r="X35" s="49"/>
+      <c r="Y35" s="50"/>
       <c r="Z35" s="16">
         <v>0</v>
       </c>
@@ -3348,13 +3384,13 @@
       <c r="AB35" s="18">
         <v>0</v>
       </c>
-      <c r="AC35" s="44" t="s">
+      <c r="AC35" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD35" s="45"/>
-      <c r="AE35" s="45"/>
-      <c r="AF35" s="45"/>
-      <c r="AG35" s="46"/>
+      <c r="AD35" s="49"/>
+      <c r="AE35" s="49"/>
+      <c r="AF35" s="49"/>
+      <c r="AG35" s="50"/>
       <c r="AH35" s="32">
         <v>0</v>
       </c>
@@ -3376,10 +3412,10 @@
       <c r="AN35" s="36">
         <v>1</v>
       </c>
-      <c r="AP35" s="50" t="s">
+      <c r="AP35" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="AQ35" s="51"/>
+      <c r="AQ35" s="55"/>
       <c r="AR35" s="26">
         <v>0</v>
       </c>
@@ -3411,14 +3447,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="48" t="s">
+      <c r="D36" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="48"/>
+      <c r="E36" s="52"/>
       <c r="F36" s="19" t="s">
         <v>27</v>
       </c>
@@ -3443,20 +3479,20 @@
       <c r="O36" s="34">
         <v>0</v>
       </c>
-      <c r="P36" s="44" t="s">
+      <c r="P36" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45"/>
-      <c r="T36" s="46"/>
-      <c r="U36" s="44" t="s">
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V36" s="45"/>
-      <c r="W36" s="45"/>
-      <c r="X36" s="45"/>
-      <c r="Y36" s="46"/>
+      <c r="V36" s="49"/>
+      <c r="W36" s="49"/>
+      <c r="X36" s="49"/>
+      <c r="Y36" s="50"/>
       <c r="Z36" s="16">
         <v>0</v>
       </c>
@@ -3466,13 +3502,13 @@
       <c r="AB36" s="18">
         <v>1</v>
       </c>
-      <c r="AC36" s="44" t="s">
+      <c r="AC36" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD36" s="45"/>
-      <c r="AE36" s="45"/>
-      <c r="AF36" s="45"/>
-      <c r="AG36" s="46"/>
+      <c r="AD36" s="49"/>
+      <c r="AE36" s="49"/>
+      <c r="AF36" s="49"/>
+      <c r="AG36" s="50"/>
       <c r="AH36" s="32">
         <v>0</v>
       </c>
@@ -3494,10 +3530,10 @@
       <c r="AN36" s="36">
         <v>1</v>
       </c>
-      <c r="AP36" s="50" t="s">
+      <c r="AP36" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="AQ36" s="51"/>
+      <c r="AQ36" s="55"/>
       <c r="AR36" s="26">
         <v>1</v>
       </c>
@@ -3529,38 +3565,38 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="48" t="s">
+      <c r="D37" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="48"/>
+      <c r="E37" s="52"/>
       <c r="F37" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I37" s="49" t="s">
+      <c r="I37" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
-      <c r="T37" s="46"/>
-      <c r="U37" s="44" t="s">
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="50"/>
+      <c r="U37" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V37" s="45"/>
-      <c r="W37" s="45"/>
-      <c r="X37" s="45"/>
-      <c r="Y37" s="46"/>
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="50"/>
       <c r="Z37" s="16">
         <v>0</v>
       </c>
@@ -3570,13 +3606,13 @@
       <c r="AB37" s="18">
         <v>0</v>
       </c>
-      <c r="AC37" s="44" t="s">
+      <c r="AC37" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD37" s="45"/>
-      <c r="AE37" s="45"/>
-      <c r="AF37" s="45"/>
-      <c r="AG37" s="46"/>
+      <c r="AD37" s="49"/>
+      <c r="AE37" s="49"/>
+      <c r="AF37" s="49"/>
+      <c r="AG37" s="50"/>
       <c r="AH37" s="8">
         <v>0</v>
       </c>
@@ -3598,10 +3634,10 @@
       <c r="AN37" s="15">
         <v>1</v>
       </c>
-      <c r="AP37" s="47" t="s">
+      <c r="AP37" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="AQ37" s="47"/>
+      <c r="AQ37" s="51"/>
       <c r="AR37" s="26">
         <v>0</v>
       </c>
@@ -3633,35 +3669,38 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="48" t="s">
+    <row r="38" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="48"/>
+      <c r="E38" s="52"/>
       <c r="F38" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="49" t="s">
+      <c r="I38" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="45"/>
-      <c r="R38" s="45"/>
-      <c r="S38" s="45"/>
-      <c r="T38" s="46"/>
-      <c r="U38" s="44" t="s">
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="49"/>
+      <c r="R38" s="49"/>
+      <c r="S38" s="49"/>
+      <c r="T38" s="50"/>
+      <c r="U38" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V38" s="45"/>
-      <c r="W38" s="45"/>
-      <c r="X38" s="45"/>
-      <c r="Y38" s="46"/>
+      <c r="V38" s="49"/>
+      <c r="W38" s="49"/>
+      <c r="X38" s="49"/>
+      <c r="Y38" s="50"/>
       <c r="Z38" s="16">
         <v>1</v>
       </c>
@@ -3671,13 +3710,13 @@
       <c r="AB38" s="18">
         <v>0</v>
       </c>
-      <c r="AC38" s="44" t="s">
+      <c r="AC38" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD38" s="45"/>
-      <c r="AE38" s="45"/>
-      <c r="AF38" s="45"/>
-      <c r="AG38" s="46"/>
+      <c r="AD38" s="49"/>
+      <c r="AE38" s="49"/>
+      <c r="AF38" s="49"/>
+      <c r="AG38" s="50"/>
       <c r="AH38" s="32">
         <v>0</v>
       </c>
@@ -3699,10 +3738,10 @@
       <c r="AN38" s="36">
         <v>1</v>
       </c>
-      <c r="AP38" s="47" t="s">
+      <c r="AP38" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="AQ38" s="47"/>
+      <c r="AQ38" s="51"/>
       <c r="AR38" s="26">
         <v>0</v>
       </c>
@@ -3734,35 +3773,38 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="48" t="s">
+    <row r="39" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="48"/>
+      <c r="E39" s="52"/>
       <c r="F39" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="49" t="s">
+      <c r="I39" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="45"/>
-      <c r="R39" s="45"/>
-      <c r="S39" s="45"/>
-      <c r="T39" s="46"/>
-      <c r="U39" s="44" t="s">
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
+      <c r="T39" s="50"/>
+      <c r="U39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V39" s="45"/>
-      <c r="W39" s="45"/>
-      <c r="X39" s="45"/>
-      <c r="Y39" s="46"/>
+      <c r="V39" s="49"/>
+      <c r="W39" s="49"/>
+      <c r="X39" s="49"/>
+      <c r="Y39" s="50"/>
       <c r="Z39" s="16">
         <v>1</v>
       </c>
@@ -3772,13 +3814,13 @@
       <c r="AB39" s="18">
         <v>0</v>
       </c>
-      <c r="AC39" s="44" t="s">
+      <c r="AC39" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD39" s="45"/>
-      <c r="AE39" s="45"/>
-      <c r="AF39" s="45"/>
-      <c r="AG39" s="46"/>
+      <c r="AD39" s="49"/>
+      <c r="AE39" s="49"/>
+      <c r="AF39" s="49"/>
+      <c r="AG39" s="50"/>
       <c r="AH39" s="32">
         <v>0</v>
       </c>
@@ -3800,10 +3842,10 @@
       <c r="AN39" s="36">
         <v>1</v>
       </c>
-      <c r="AP39" s="47" t="s">
+      <c r="AP39" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AQ39" s="47"/>
+      <c r="AQ39" s="51"/>
       <c r="AR39" s="26">
         <v>0</v>
       </c>
@@ -3835,35 +3877,38 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="48" t="s">
+    <row r="40" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="48"/>
+      <c r="E40" s="52"/>
       <c r="F40" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I40" s="49" t="s">
+      <c r="I40" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J40" s="45"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="45"/>
-      <c r="N40" s="45"/>
-      <c r="O40" s="45"/>
-      <c r="P40" s="45"/>
-      <c r="Q40" s="45"/>
-      <c r="R40" s="45"/>
-      <c r="S40" s="45"/>
-      <c r="T40" s="46"/>
-      <c r="U40" s="44" t="s">
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="50"/>
+      <c r="U40" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V40" s="45"/>
-      <c r="W40" s="45"/>
-      <c r="X40" s="45"/>
-      <c r="Y40" s="46"/>
+      <c r="V40" s="49"/>
+      <c r="W40" s="49"/>
+      <c r="X40" s="49"/>
+      <c r="Y40" s="50"/>
       <c r="Z40" s="16">
         <v>1</v>
       </c>
@@ -3873,13 +3918,13 @@
       <c r="AB40" s="18">
         <v>1</v>
       </c>
-      <c r="AC40" s="44" t="s">
+      <c r="AC40" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD40" s="45"/>
-      <c r="AE40" s="45"/>
-      <c r="AF40" s="45"/>
-      <c r="AG40" s="46"/>
+      <c r="AD40" s="49"/>
+      <c r="AE40" s="49"/>
+      <c r="AF40" s="49"/>
+      <c r="AG40" s="50"/>
       <c r="AH40" s="32">
         <v>0</v>
       </c>
@@ -3901,10 +3946,10 @@
       <c r="AN40" s="36">
         <v>1</v>
       </c>
-      <c r="AP40" s="47" t="s">
+      <c r="AP40" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="AQ40" s="47"/>
+      <c r="AQ40" s="51"/>
       <c r="AR40" s="26">
         <v>0</v>
       </c>
@@ -3936,11 +3981,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="48" t="s">
+    <row r="41" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="E41" s="48"/>
+      <c r="E41" s="52"/>
       <c r="F41" s="12" t="s">
         <v>22</v>
       </c>
@@ -3965,20 +4013,20 @@
       <c r="O41" s="33">
         <v>0</v>
       </c>
-      <c r="P41" s="44" t="s">
+      <c r="P41" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="Q41" s="45"/>
-      <c r="R41" s="45"/>
-      <c r="S41" s="45"/>
-      <c r="T41" s="46"/>
-      <c r="U41" s="45" t="s">
+      <c r="Q41" s="49"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="50"/>
+      <c r="U41" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V41" s="45"/>
-      <c r="W41" s="45"/>
-      <c r="X41" s="45"/>
-      <c r="Y41" s="46"/>
+      <c r="V41" s="49"/>
+      <c r="W41" s="49"/>
+      <c r="X41" s="49"/>
+      <c r="Y41" s="50"/>
       <c r="Z41" s="16">
         <v>0</v>
       </c>
@@ -3988,13 +4036,13 @@
       <c r="AB41" s="18">
         <v>1</v>
       </c>
-      <c r="AC41" s="44" t="s">
+      <c r="AC41" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD41" s="45"/>
-      <c r="AE41" s="45"/>
-      <c r="AF41" s="45"/>
-      <c r="AG41" s="46"/>
+      <c r="AD41" s="49"/>
+      <c r="AE41" s="49"/>
+      <c r="AF41" s="49"/>
+      <c r="AG41" s="50"/>
       <c r="AH41" s="32">
         <v>0</v>
       </c>
@@ -4016,10 +4064,10 @@
       <c r="AN41" s="36">
         <v>1</v>
       </c>
-      <c r="AP41" s="47" t="s">
+      <c r="AP41" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="AQ41" s="47"/>
+      <c r="AQ41" s="51"/>
       <c r="AR41" s="26">
         <v>0</v>
       </c>
@@ -4051,11 +4099,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="48" t="s">
+    <row r="42" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="48"/>
+      <c r="E42" s="52"/>
       <c r="F42" s="12" t="s">
         <v>22</v>
       </c>
@@ -4080,20 +4131,20 @@
       <c r="O42" s="33">
         <v>0</v>
       </c>
-      <c r="P42" s="44" t="s">
+      <c r="P42" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="Q42" s="45"/>
-      <c r="R42" s="45"/>
-      <c r="S42" s="45"/>
-      <c r="T42" s="46"/>
-      <c r="U42" s="45" t="s">
+      <c r="Q42" s="49"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="50"/>
+      <c r="U42" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V42" s="45"/>
-      <c r="W42" s="45"/>
-      <c r="X42" s="45"/>
-      <c r="Y42" s="46"/>
+      <c r="V42" s="49"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="49"/>
+      <c r="Y42" s="50"/>
       <c r="Z42" s="16">
         <v>1</v>
       </c>
@@ -4103,13 +4154,13 @@
       <c r="AB42" s="18">
         <v>1</v>
       </c>
-      <c r="AC42" s="44" t="s">
+      <c r="AC42" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD42" s="45"/>
-      <c r="AE42" s="45"/>
-      <c r="AF42" s="45"/>
-      <c r="AG42" s="46"/>
+      <c r="AD42" s="49"/>
+      <c r="AE42" s="49"/>
+      <c r="AF42" s="49"/>
+      <c r="AG42" s="50"/>
       <c r="AH42" s="32">
         <v>0</v>
       </c>
@@ -4131,10 +4182,10 @@
       <c r="AN42" s="36">
         <v>1</v>
       </c>
-      <c r="AP42" s="47" t="s">
+      <c r="AP42" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="AQ42" s="47"/>
+      <c r="AQ42" s="51"/>
       <c r="AR42" s="26">
         <v>1</v>
       </c>
@@ -4166,11 +4217,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="48" t="s">
+    <row r="43" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="48"/>
+      <c r="E43" s="52"/>
       <c r="F43" s="12" t="s">
         <v>22</v>
       </c>
@@ -4195,20 +4249,20 @@
       <c r="O43" s="33">
         <v>0</v>
       </c>
-      <c r="P43" s="44" t="s">
+      <c r="P43" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="Q43" s="45"/>
-      <c r="R43" s="45"/>
-      <c r="S43" s="45"/>
-      <c r="T43" s="46"/>
-      <c r="U43" s="45" t="s">
+      <c r="Q43" s="49"/>
+      <c r="R43" s="49"/>
+      <c r="S43" s="49"/>
+      <c r="T43" s="50"/>
+      <c r="U43" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V43" s="45"/>
-      <c r="W43" s="45"/>
-      <c r="X43" s="45"/>
-      <c r="Y43" s="46"/>
+      <c r="V43" s="49"/>
+      <c r="W43" s="49"/>
+      <c r="X43" s="49"/>
+      <c r="Y43" s="50"/>
       <c r="Z43" s="16">
         <v>1</v>
       </c>
@@ -4218,13 +4272,13 @@
       <c r="AB43" s="18">
         <v>1</v>
       </c>
-      <c r="AC43" s="44" t="s">
+      <c r="AC43" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD43" s="45"/>
-      <c r="AE43" s="45"/>
-      <c r="AF43" s="45"/>
-      <c r="AG43" s="46"/>
+      <c r="AD43" s="49"/>
+      <c r="AE43" s="49"/>
+      <c r="AF43" s="49"/>
+      <c r="AG43" s="50"/>
       <c r="AH43" s="32">
         <v>0</v>
       </c>
@@ -4246,10 +4300,10 @@
       <c r="AN43" s="36">
         <v>1</v>
       </c>
-      <c r="AP43" s="47" t="s">
+      <c r="AP43" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="AQ43" s="47"/>
+      <c r="AQ43" s="51"/>
       <c r="AR43" s="26">
         <v>0</v>
       </c>
@@ -4281,35 +4335,38 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="48" t="s">
+    <row r="44" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="48"/>
+      <c r="E44" s="52"/>
       <c r="F44" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I44" s="49" t="s">
+      <c r="I44" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J44" s="45"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="45"/>
-      <c r="M44" s="45"/>
-      <c r="N44" s="45"/>
-      <c r="O44" s="45"/>
-      <c r="P44" s="45"/>
-      <c r="Q44" s="45"/>
-      <c r="R44" s="45"/>
-      <c r="S44" s="45"/>
-      <c r="T44" s="46"/>
-      <c r="U44" s="44" t="s">
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="49"/>
+      <c r="R44" s="49"/>
+      <c r="S44" s="49"/>
+      <c r="T44" s="50"/>
+      <c r="U44" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V44" s="45"/>
-      <c r="W44" s="45"/>
-      <c r="X44" s="45"/>
-      <c r="Y44" s="46"/>
+      <c r="V44" s="49"/>
+      <c r="W44" s="49"/>
+      <c r="X44" s="49"/>
+      <c r="Y44" s="50"/>
       <c r="Z44" s="16">
         <v>0</v>
       </c>
@@ -4319,13 +4376,13 @@
       <c r="AB44" s="18">
         <v>0</v>
       </c>
-      <c r="AC44" s="44" t="s">
+      <c r="AC44" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD44" s="45"/>
-      <c r="AE44" s="45"/>
-      <c r="AF44" s="45"/>
-      <c r="AG44" s="46"/>
+      <c r="AD44" s="49"/>
+      <c r="AE44" s="49"/>
+      <c r="AF44" s="49"/>
+      <c r="AG44" s="50"/>
       <c r="AH44" s="32">
         <v>0</v>
       </c>
@@ -4347,10 +4404,10 @@
       <c r="AN44" s="36">
         <v>1</v>
       </c>
-      <c r="AP44" s="47" t="s">
+      <c r="AP44" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="AQ44" s="47"/>
+      <c r="AQ44" s="51"/>
       <c r="AR44" s="26">
         <v>0</v>
       </c>
@@ -4382,33 +4439,36 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="48" t="s">
+    <row r="45" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="48"/>
+      <c r="E45" s="52"/>
       <c r="F45" s="12"/>
-      <c r="I45" s="49" t="s">
+      <c r="I45" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J45" s="45"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="45"/>
-      <c r="M45" s="45"/>
-      <c r="N45" s="45"/>
-      <c r="O45" s="45"/>
-      <c r="P45" s="45"/>
-      <c r="Q45" s="45"/>
-      <c r="R45" s="45"/>
-      <c r="S45" s="45"/>
-      <c r="T45" s="46"/>
-      <c r="U45" s="44" t="s">
+      <c r="J45" s="49"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
+      <c r="P45" s="49"/>
+      <c r="Q45" s="49"/>
+      <c r="R45" s="49"/>
+      <c r="S45" s="49"/>
+      <c r="T45" s="50"/>
+      <c r="U45" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V45" s="45"/>
-      <c r="W45" s="45"/>
-      <c r="X45" s="45"/>
-      <c r="Y45" s="46"/>
+      <c r="V45" s="49"/>
+      <c r="W45" s="49"/>
+      <c r="X45" s="49"/>
+      <c r="Y45" s="50"/>
       <c r="Z45" s="16">
         <v>0</v>
       </c>
@@ -4418,13 +4478,13 @@
       <c r="AB45" s="18">
         <v>1</v>
       </c>
-      <c r="AC45" s="44" t="s">
+      <c r="AC45" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD45" s="45"/>
-      <c r="AE45" s="45"/>
-      <c r="AF45" s="45"/>
-      <c r="AG45" s="46"/>
+      <c r="AD45" s="49"/>
+      <c r="AE45" s="49"/>
+      <c r="AF45" s="49"/>
+      <c r="AG45" s="50"/>
       <c r="AH45" s="32">
         <v>0</v>
       </c>
@@ -4446,11 +4506,11 @@
       <c r="AN45" s="36">
         <v>1</v>
       </c>
-      <c r="AP45" s="50" t="s">
+      <c r="AP45" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="AQ45" s="51"/>
-      <c r="AR45" s="42">
+      <c r="AQ45" s="55"/>
+      <c r="AR45" s="46">
         <v>1</v>
       </c>
       <c r="AS45" s="27">
@@ -4459,7 +4519,7 @@
       <c r="AT45" s="27">
         <v>0</v>
       </c>
-      <c r="AU45" s="43">
+      <c r="AU45" s="47">
         <v>1</v>
       </c>
       <c r="AW45" s="37">
@@ -4481,80 +4541,80 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:54" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="E46" s="48"/>
+      <c r="D46" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="52"/>
       <c r="F46" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I46" s="49" t="s">
+      <c r="I46" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="45"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="45"/>
-      <c r="M46" s="45"/>
-      <c r="N46" s="45"/>
-      <c r="O46" s="45"/>
-      <c r="P46" s="45"/>
-      <c r="Q46" s="45"/>
-      <c r="R46" s="45"/>
-      <c r="S46" s="45"/>
-      <c r="T46" s="46"/>
-      <c r="U46" s="44" t="s">
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+      <c r="L46" s="49"/>
+      <c r="M46" s="49"/>
+      <c r="N46" s="49"/>
+      <c r="O46" s="49"/>
+      <c r="P46" s="49"/>
+      <c r="Q46" s="49"/>
+      <c r="R46" s="49"/>
+      <c r="S46" s="49"/>
+      <c r="T46" s="50"/>
+      <c r="U46" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V46" s="45"/>
-      <c r="W46" s="45"/>
-      <c r="X46" s="45"/>
-      <c r="Y46" s="46"/>
+      <c r="V46" s="49"/>
+      <c r="W46" s="49"/>
+      <c r="X46" s="49"/>
+      <c r="Y46" s="50"/>
       <c r="Z46" s="16">
         <v>0</v>
       </c>
       <c r="AA46" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB46" s="18">
         <v>0</v>
       </c>
-      <c r="AC46" s="44" t="s">
+      <c r="AC46" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD46" s="45"/>
-      <c r="AE46" s="45"/>
-      <c r="AF46" s="45"/>
-      <c r="AG46" s="46"/>
-      <c r="AH46" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI46" s="9">
-        <v>0</v>
-      </c>
-      <c r="AJ46" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK46" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL46" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM46" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN46" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP46" s="47" t="s">
+      <c r="AD46" s="49"/>
+      <c r="AE46" s="49"/>
+      <c r="AF46" s="49"/>
+      <c r="AG46" s="50"/>
+      <c r="AH46" s="44">
+        <v>0</v>
+      </c>
+      <c r="AI46" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ46" s="43">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="43">
+        <v>0</v>
+      </c>
+      <c r="AL46" s="43">
+        <v>0</v>
+      </c>
+      <c r="AM46" s="43">
+        <v>1</v>
+      </c>
+      <c r="AN46" s="45">
+        <v>1</v>
+      </c>
+      <c r="AP46" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="AQ46" s="47"/>
-      <c r="AR46" s="26">
+      <c r="AQ46" s="51"/>
+      <c r="AR46" s="46">
         <v>0</v>
       </c>
       <c r="AS46" s="27">
@@ -4563,354 +4623,836 @@
       <c r="AT46" s="27">
         <v>1</v>
       </c>
-      <c r="AU46" s="28">
-        <v>1</v>
-      </c>
-      <c r="AW46" s="37">
-        <v>1</v>
-      </c>
-      <c r="AX46" s="37">
-        <v>1</v>
-      </c>
-      <c r="AY46" s="37">
-        <v>1</v>
-      </c>
-      <c r="AZ46" s="37">
+      <c r="AU46" s="47">
+        <v>1</v>
+      </c>
+      <c r="AW46" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX46" s="42">
+        <v>1</v>
+      </c>
+      <c r="AY46" s="42">
+        <v>1</v>
+      </c>
+      <c r="AZ46" s="42">
         <v>0</v>
       </c>
       <c r="BA46" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="BB46" s="37" t="s">
+      <c r="BB46" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:54" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="48" t="s">
+      <c r="D47" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" s="52"/>
+      <c r="F47" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" s="49"/>
+      <c r="K47" s="49"/>
+      <c r="L47" s="49"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="49"/>
+      <c r="O47" s="49"/>
+      <c r="P47" s="49"/>
+      <c r="Q47" s="49"/>
+      <c r="R47" s="49"/>
+      <c r="S47" s="49"/>
+      <c r="T47" s="50"/>
+      <c r="U47" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="V47" s="49"/>
+      <c r="W47" s="49"/>
+      <c r="X47" s="49"/>
+      <c r="Y47" s="50"/>
+      <c r="Z47" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC47" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD47" s="49"/>
+      <c r="AE47" s="49"/>
+      <c r="AF47" s="49"/>
+      <c r="AG47" s="50"/>
+      <c r="AH47" s="44">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ47" s="43">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="43">
+        <v>0</v>
+      </c>
+      <c r="AL47" s="43">
+        <v>0</v>
+      </c>
+      <c r="AM47" s="43">
+        <v>1</v>
+      </c>
+      <c r="AN47" s="45">
+        <v>1</v>
+      </c>
+      <c r="AP47" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ47" s="51"/>
+      <c r="AR47" s="46">
+        <v>0</v>
+      </c>
+      <c r="AS47" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT47" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU47" s="47">
+        <v>1</v>
+      </c>
+      <c r="AW47" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX47" s="42">
+        <v>1</v>
+      </c>
+      <c r="AY47" s="42">
+        <v>1</v>
+      </c>
+      <c r="AZ47" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA47" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB47" s="42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" s="52"/>
+      <c r="F48" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="49"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="49"/>
+      <c r="O48" s="49"/>
+      <c r="P48" s="49"/>
+      <c r="Q48" s="49"/>
+      <c r="R48" s="49"/>
+      <c r="S48" s="49"/>
+      <c r="T48" s="50"/>
+      <c r="U48" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="V48" s="49"/>
+      <c r="W48" s="49"/>
+      <c r="X48" s="49"/>
+      <c r="Y48" s="50"/>
+      <c r="Z48" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="17">
+        <v>1</v>
+      </c>
+      <c r="AB48" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD48" s="49"/>
+      <c r="AE48" s="49"/>
+      <c r="AF48" s="49"/>
+      <c r="AG48" s="50"/>
+      <c r="AH48" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI48" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ48" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK48" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL48" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM48" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN48" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP48" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ48" s="51"/>
+      <c r="AR48" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS48" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT48" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU48" s="28">
+        <v>1</v>
+      </c>
+      <c r="AW48" s="37">
+        <v>1</v>
+      </c>
+      <c r="AX48" s="37">
+        <v>1</v>
+      </c>
+      <c r="AY48" s="37">
+        <v>1</v>
+      </c>
+      <c r="AZ48" s="37">
+        <v>0</v>
+      </c>
+      <c r="BA48" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB48" s="37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" s="52"/>
+      <c r="F49" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" s="49"/>
+      <c r="K49" s="49"/>
+      <c r="L49" s="49"/>
+      <c r="M49" s="49"/>
+      <c r="N49" s="49"/>
+      <c r="O49" s="49"/>
+      <c r="P49" s="49"/>
+      <c r="Q49" s="49"/>
+      <c r="R49" s="49"/>
+      <c r="S49" s="49"/>
+      <c r="T49" s="50"/>
+      <c r="U49" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="V49" s="49"/>
+      <c r="W49" s="49"/>
+      <c r="X49" s="49"/>
+      <c r="Y49" s="50"/>
+      <c r="Z49" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA49" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD49" s="49"/>
+      <c r="AE49" s="49"/>
+      <c r="AF49" s="49"/>
+      <c r="AG49" s="50"/>
+      <c r="AH49" s="44">
+        <v>0</v>
+      </c>
+      <c r="AI49" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ49" s="43">
+        <v>0</v>
+      </c>
+      <c r="AK49" s="43">
+        <v>0</v>
+      </c>
+      <c r="AL49" s="43">
+        <v>0</v>
+      </c>
+      <c r="AM49" s="43">
+        <v>1</v>
+      </c>
+      <c r="AN49" s="45">
+        <v>1</v>
+      </c>
+      <c r="AP49" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ49" s="51"/>
+      <c r="AR49" s="46">
+        <v>0</v>
+      </c>
+      <c r="AS49" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT49" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU49" s="47">
+        <v>1</v>
+      </c>
+      <c r="AW49" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX49" s="42">
+        <v>1</v>
+      </c>
+      <c r="AY49" s="42">
+        <v>1</v>
+      </c>
+      <c r="AZ49" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA49" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB49" s="42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" s="52"/>
+      <c r="F50" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="49"/>
+      <c r="N50" s="49"/>
+      <c r="O50" s="49"/>
+      <c r="P50" s="49"/>
+      <c r="Q50" s="49"/>
+      <c r="R50" s="49"/>
+      <c r="S50" s="49"/>
+      <c r="T50" s="50"/>
+      <c r="U50" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="V50" s="49"/>
+      <c r="W50" s="49"/>
+      <c r="X50" s="49"/>
+      <c r="Y50" s="50"/>
+      <c r="Z50" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA50" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="18">
+        <v>1</v>
+      </c>
+      <c r="AC50" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD50" s="49"/>
+      <c r="AE50" s="49"/>
+      <c r="AF50" s="49"/>
+      <c r="AG50" s="50"/>
+      <c r="AH50" s="44">
+        <v>0</v>
+      </c>
+      <c r="AI50" s="43">
+        <v>0</v>
+      </c>
+      <c r="AJ50" s="43">
+        <v>0</v>
+      </c>
+      <c r="AK50" s="43">
+        <v>0</v>
+      </c>
+      <c r="AL50" s="43">
+        <v>0</v>
+      </c>
+      <c r="AM50" s="43">
+        <v>1</v>
+      </c>
+      <c r="AN50" s="45">
+        <v>1</v>
+      </c>
+      <c r="AP50" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ50" s="51"/>
+      <c r="AR50" s="46">
+        <v>0</v>
+      </c>
+      <c r="AS50" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT50" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU50" s="47">
+        <v>1</v>
+      </c>
+      <c r="AW50" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX50" s="42">
+        <v>1</v>
+      </c>
+      <c r="AY50" s="42">
+        <v>1</v>
+      </c>
+      <c r="AZ50" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA50" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB50" s="42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D51" s="52" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="52"/>
+      <c r="F51" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="53"/>
+      <c r="J51" s="49"/>
+      <c r="K51" s="49"/>
+      <c r="L51" s="49"/>
+      <c r="M51" s="49"/>
+      <c r="N51" s="49"/>
+      <c r="O51" s="49"/>
+      <c r="P51" s="49"/>
+      <c r="Q51" s="49"/>
+      <c r="R51" s="49"/>
+      <c r="S51" s="49"/>
+      <c r="T51" s="50"/>
+      <c r="U51" s="48"/>
+      <c r="V51" s="49"/>
+      <c r="W51" s="49"/>
+      <c r="X51" s="49"/>
+      <c r="Y51" s="50"/>
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="17"/>
+      <c r="AB51" s="18"/>
+      <c r="AC51" s="48"/>
+      <c r="AD51" s="49"/>
+      <c r="AE51" s="49"/>
+      <c r="AF51" s="49"/>
+      <c r="AG51" s="50"/>
+      <c r="AH51" s="44"/>
+      <c r="AI51" s="43"/>
+      <c r="AJ51" s="43"/>
+      <c r="AK51" s="43"/>
+      <c r="AL51" s="43"/>
+      <c r="AM51" s="43"/>
+      <c r="AN51" s="45"/>
+      <c r="AP51" s="51"/>
+      <c r="AQ51" s="51"/>
+      <c r="AR51" s="46"/>
+      <c r="AS51" s="27"/>
+      <c r="AT51" s="27"/>
+      <c r="AU51" s="47"/>
+      <c r="AW51" s="42"/>
+      <c r="AX51" s="42"/>
+      <c r="AY51" s="42"/>
+      <c r="AZ51" s="42"/>
+      <c r="BA51" s="40"/>
+      <c r="BB51" s="42"/>
+    </row>
+    <row r="52" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="48"/>
-      <c r="F47" s="13" t="s">
+      <c r="E52" s="52"/>
+      <c r="F52" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I47" s="49" t="s">
+      <c r="I52" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="J47" s="45"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="45"/>
-      <c r="O47" s="46"/>
-      <c r="P47" s="44" t="s">
+      <c r="J52" s="49"/>
+      <c r="K52" s="49"/>
+      <c r="L52" s="49"/>
+      <c r="M52" s="49"/>
+      <c r="N52" s="49"/>
+      <c r="O52" s="50"/>
+      <c r="P52" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q47" s="45"/>
-      <c r="R47" s="45"/>
-      <c r="S47" s="45"/>
-      <c r="T47" s="46"/>
-      <c r="U47" s="44" t="s">
+      <c r="Q52" s="49"/>
+      <c r="R52" s="49"/>
+      <c r="S52" s="49"/>
+      <c r="T52" s="50"/>
+      <c r="U52" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V47" s="45"/>
-      <c r="W47" s="45"/>
-      <c r="X47" s="45"/>
-      <c r="Y47" s="46"/>
-      <c r="Z47" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA47" s="9">
-        <v>1</v>
-      </c>
-      <c r="AB47" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC47" s="44" t="s">
+      <c r="V52" s="49"/>
+      <c r="W52" s="49"/>
+      <c r="X52" s="49"/>
+      <c r="Y52" s="50"/>
+      <c r="Z52" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA52" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB52" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC52" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="AD47" s="45"/>
-      <c r="AE47" s="45"/>
-      <c r="AF47" s="45"/>
-      <c r="AG47" s="46"/>
-      <c r="AH47" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI47" s="9">
-        <v>1</v>
-      </c>
-      <c r="AJ47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM47" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN47" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP47" s="47" t="s">
+      <c r="AD52" s="49"/>
+      <c r="AE52" s="49"/>
+      <c r="AF52" s="49"/>
+      <c r="AG52" s="50"/>
+      <c r="AH52" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI52" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ52" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK52" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM52" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN52" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP52" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="AQ47" s="47"/>
-      <c r="AR47" s="26">
-        <v>0</v>
-      </c>
-      <c r="AS47" s="27">
-        <v>0</v>
-      </c>
-      <c r="AT47" s="27">
-        <v>1</v>
-      </c>
-      <c r="AU47" s="28">
-        <v>1</v>
-      </c>
-      <c r="AW47" s="37">
-        <v>1</v>
-      </c>
-      <c r="AX47" s="37">
-        <v>0</v>
-      </c>
-      <c r="AY47" s="37">
-        <v>1</v>
-      </c>
-      <c r="AZ47" s="37">
-        <v>1</v>
-      </c>
-      <c r="BA47" s="40" t="s">
+      <c r="AQ52" s="51"/>
+      <c r="AR52" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS52" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT52" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU52" s="28">
+        <v>1</v>
+      </c>
+      <c r="AW52" s="37">
+        <v>1</v>
+      </c>
+      <c r="AX52" s="37">
+        <v>0</v>
+      </c>
+      <c r="AY52" s="37">
+        <v>1</v>
+      </c>
+      <c r="AZ52" s="37">
+        <v>1</v>
+      </c>
+      <c r="BA52" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB47" s="37" t="s">
+      <c r="BB52" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="48" t="s">
+    <row r="53" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="48"/>
-      <c r="F48" s="29" t="s">
+      <c r="E53" s="52"/>
+      <c r="F53" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="I48" s="14" t="s">
+      <c r="I53" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J48" s="49" t="s">
+      <c r="J53" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="K48" s="45"/>
-      <c r="L48" s="45"/>
-      <c r="M48" s="45"/>
-      <c r="N48" s="45"/>
-      <c r="O48" s="46"/>
-      <c r="P48" s="44" t="s">
+      <c r="K53" s="49"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="49"/>
+      <c r="O53" s="50"/>
+      <c r="P53" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="Q48" s="45"/>
-      <c r="R48" s="45"/>
-      <c r="S48" s="45"/>
-      <c r="T48" s="46"/>
-      <c r="U48" s="44" t="s">
+      <c r="Q53" s="49"/>
+      <c r="R53" s="49"/>
+      <c r="S53" s="49"/>
+      <c r="T53" s="50"/>
+      <c r="U53" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="V48" s="45"/>
-      <c r="W48" s="45"/>
-      <c r="X48" s="45"/>
-      <c r="Y48" s="46"/>
-      <c r="Z48" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB48" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC48" s="44" t="s">
+      <c r="V53" s="49"/>
+      <c r="W53" s="49"/>
+      <c r="X53" s="49"/>
+      <c r="Y53" s="50"/>
+      <c r="Z53" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="AD48" s="45"/>
-      <c r="AE48" s="45"/>
-      <c r="AF48" s="46"/>
-      <c r="AG48" s="10" t="s">
+      <c r="AD53" s="49"/>
+      <c r="AE53" s="49"/>
+      <c r="AF53" s="50"/>
+      <c r="AG53" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AH48" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI48" s="9">
-        <v>1</v>
-      </c>
-      <c r="AJ48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM48" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN48" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP48" s="47" t="s">
+      <c r="AH53" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI53" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ53" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL53" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM53" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN53" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP53" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="AQ48" s="47"/>
-      <c r="AR48" s="26">
-        <v>0</v>
-      </c>
-      <c r="AS48" s="27">
-        <v>1</v>
-      </c>
-      <c r="AT48" s="27">
-        <v>0</v>
-      </c>
-      <c r="AU48" s="28">
-        <v>0</v>
-      </c>
-      <c r="AW48" s="37">
-        <v>1</v>
-      </c>
-      <c r="AX48" s="37">
-        <v>0</v>
-      </c>
-      <c r="AY48" s="37">
-        <v>0</v>
-      </c>
-      <c r="AZ48" s="37">
-        <v>0</v>
-      </c>
-      <c r="BA48" s="37" t="s">
+      <c r="AQ53" s="51"/>
+      <c r="AR53" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS53" s="27">
+        <v>1</v>
+      </c>
+      <c r="AT53" s="27">
+        <v>0</v>
+      </c>
+      <c r="AU53" s="28">
+        <v>0</v>
+      </c>
+      <c r="AW53" s="37">
+        <v>1</v>
+      </c>
+      <c r="AX53" s="37">
+        <v>0</v>
+      </c>
+      <c r="AY53" s="37">
+        <v>0</v>
+      </c>
+      <c r="AZ53" s="37">
+        <v>0</v>
+      </c>
+      <c r="BA53" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="BB48" s="37" t="s">
+      <c r="BB53" s="37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="4:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="48" t="s">
+    <row r="54" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="48"/>
-      <c r="F49" s="30" t="s">
+      <c r="E54" s="52"/>
+      <c r="F54" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="I49" s="6" t="s">
+      <c r="I54" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J49" s="44" t="s">
+      <c r="J54" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="45"/>
-      <c r="O49" s="45"/>
-      <c r="P49" s="45"/>
-      <c r="Q49" s="45"/>
-      <c r="R49" s="45"/>
-      <c r="S49" s="45"/>
-      <c r="T49" s="7" t="s">
+      <c r="K54" s="49"/>
+      <c r="L54" s="49"/>
+      <c r="M54" s="49"/>
+      <c r="N54" s="49"/>
+      <c r="O54" s="49"/>
+      <c r="P54" s="49"/>
+      <c r="Q54" s="49"/>
+      <c r="R54" s="49"/>
+      <c r="S54" s="49"/>
+      <c r="T54" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U49" s="44" t="s">
+      <c r="U54" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="V49" s="45"/>
-      <c r="W49" s="45"/>
-      <c r="X49" s="45"/>
-      <c r="Y49" s="45"/>
-      <c r="Z49" s="45"/>
-      <c r="AA49" s="45"/>
-      <c r="AB49" s="46"/>
-      <c r="AC49" s="44" t="s">
+      <c r="V54" s="49"/>
+      <c r="W54" s="49"/>
+      <c r="X54" s="49"/>
+      <c r="Y54" s="49"/>
+      <c r="Z54" s="49"/>
+      <c r="AA54" s="49"/>
+      <c r="AB54" s="50"/>
+      <c r="AC54" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="AD49" s="45"/>
-      <c r="AE49" s="45"/>
-      <c r="AF49" s="45"/>
-      <c r="AG49" s="46"/>
-      <c r="AH49" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI49" s="9">
-        <v>1</v>
-      </c>
-      <c r="AJ49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK49" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL49" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM49" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN49" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP49" s="47" t="s">
+      <c r="AD54" s="49"/>
+      <c r="AE54" s="49"/>
+      <c r="AF54" s="49"/>
+      <c r="AG54" s="50"/>
+      <c r="AH54" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI54" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ54" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK54" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL54" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM54" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN54" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP54" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="AQ49" s="47"/>
-      <c r="AR49" s="26">
-        <v>0</v>
-      </c>
-      <c r="AS49" s="27">
-        <v>0</v>
-      </c>
-      <c r="AT49" s="27">
-        <v>1</v>
-      </c>
-      <c r="AU49" s="28">
-        <v>1</v>
-      </c>
-      <c r="AW49" s="37">
-        <v>0</v>
-      </c>
-      <c r="AX49" s="37">
-        <v>1</v>
-      </c>
-      <c r="AY49" s="37">
-        <v>1</v>
-      </c>
-      <c r="AZ49" s="37">
-        <v>0</v>
-      </c>
-      <c r="BA49" s="41" t="s">
+      <c r="AQ54" s="51"/>
+      <c r="AR54" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS54" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT54" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU54" s="28">
+        <v>1</v>
+      </c>
+      <c r="AW54" s="37">
+        <v>0</v>
+      </c>
+      <c r="AX54" s="37">
+        <v>1</v>
+      </c>
+      <c r="AY54" s="37">
+        <v>1</v>
+      </c>
+      <c r="AZ54" s="37">
+        <v>0</v>
+      </c>
+      <c r="BA54" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="BB49" s="37" t="s">
+      <c r="BB54" s="37" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="166">
+  <mergeCells count="191">
+    <mergeCell ref="AP50:AQ50"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="I49:T49"/>
+    <mergeCell ref="U49:Y49"/>
+    <mergeCell ref="AC49:AG49"/>
+    <mergeCell ref="AP49:AQ49"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="I51:T51"/>
+    <mergeCell ref="U51:Y51"/>
+    <mergeCell ref="AC51:AG51"/>
+    <mergeCell ref="AP51:AQ51"/>
     <mergeCell ref="AW25:BA25"/>
     <mergeCell ref="AP27:AQ27"/>
     <mergeCell ref="AP28:AQ28"/>
     <mergeCell ref="AP37:AQ37"/>
-    <mergeCell ref="AP46:AQ46"/>
+    <mergeCell ref="AP48:AQ48"/>
     <mergeCell ref="AP26:AS26"/>
     <mergeCell ref="AP30:AQ30"/>
     <mergeCell ref="AP31:AQ31"/>
     <mergeCell ref="AP12:AQ12"/>
     <mergeCell ref="AP47:AQ47"/>
-    <mergeCell ref="AP48:AQ48"/>
-    <mergeCell ref="AP49:AQ49"/>
+    <mergeCell ref="AP46:AQ46"/>
+    <mergeCell ref="AP52:AQ52"/>
+    <mergeCell ref="AP53:AQ53"/>
+    <mergeCell ref="AP54:AQ54"/>
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="I8:O8"/>
     <mergeCell ref="P8:T8"/>
@@ -4924,6 +5466,14 @@
     <mergeCell ref="AH11:AN11"/>
     <mergeCell ref="AH14:AN14"/>
     <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="I47:T47"/>
+    <mergeCell ref="U47:Y47"/>
+    <mergeCell ref="AC47:AG47"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="I46:T46"/>
+    <mergeCell ref="U46:Y46"/>
+    <mergeCell ref="AC46:AG46"/>
     <mergeCell ref="D11:G11"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="I14:O14"/>
@@ -4971,26 +5521,30 @@
     <mergeCell ref="P28:T28"/>
     <mergeCell ref="U28:Y28"/>
     <mergeCell ref="AC28:AG28"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D52:E52"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="I37:T37"/>
-    <mergeCell ref="AC46:AG46"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="J49:S49"/>
-    <mergeCell ref="U49:AB49"/>
-    <mergeCell ref="AC49:AG49"/>
-    <mergeCell ref="I47:O47"/>
-    <mergeCell ref="P47:T47"/>
-    <mergeCell ref="U47:Y47"/>
-    <mergeCell ref="AC47:AG47"/>
-    <mergeCell ref="I46:T46"/>
-    <mergeCell ref="U46:Y46"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="P48:T48"/>
+    <mergeCell ref="AC48:AG48"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="I50:T50"/>
+    <mergeCell ref="U50:Y50"/>
+    <mergeCell ref="AC50:AG50"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="J54:S54"/>
+    <mergeCell ref="U54:AB54"/>
+    <mergeCell ref="AC54:AG54"/>
+    <mergeCell ref="I52:O52"/>
+    <mergeCell ref="P52:T52"/>
+    <mergeCell ref="U52:Y52"/>
+    <mergeCell ref="AC52:AG52"/>
+    <mergeCell ref="I48:T48"/>
     <mergeCell ref="U48:Y48"/>
-    <mergeCell ref="AC48:AF48"/>
-    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="P53:T53"/>
+    <mergeCell ref="U53:Y53"/>
+    <mergeCell ref="AC53:AF53"/>
+    <mergeCell ref="J53:O53"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>

</xml_diff>

<commit_message>
implemented all I-type instr
</commit_message>
<xml_diff>
--- a/doc/decoding.xlsx
+++ b/doc/decoding.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\SystemVerilog\FRiscV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181436AF-1440-4318-AF20-A03FA9598AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9EFA7B-1B8B-43F9-B2BB-3C9009AB4554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28305" yWindow="915" windowWidth="25965" windowHeight="14595" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
+    <workbookView xWindow="29490" yWindow="1470" windowWidth="25965" windowHeight="14595" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$27:$BB$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$27:$BC$36</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="75">
   <si>
     <t>R-TYPE</t>
   </si>
@@ -340,6 +340,9 @@
   </si>
   <si>
     <t>JALR</t>
+  </si>
+  <si>
+    <t>jSrc</t>
   </si>
 </sst>
 </file>
@@ -748,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -979,6 +982,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1294,16 +1300,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA95D64-5055-4174-A4D5-0BDBECB18FB0}">
-  <dimension ref="C1:BB54"/>
+  <dimension ref="C1:BC54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="23" topLeftCell="J24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="7" ySplit="23" topLeftCell="H33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="F52" sqref="F52"/>
+      <selection pane="bottomRight" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="4.7109375" style="3"/>
     <col min="3" max="3" width="7.42578125" style="3" customWidth="1"/>
@@ -1318,9 +1324,10 @@
     <col min="50" max="50" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="4.7109375" style="3"/>
+    <col min="53" max="53" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="56" max="16384" width="4.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:47" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2049,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:55" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="64" t="s">
         <v>3</v>
       </c>
@@ -2105,7 +2112,7 @@
       <c r="AM17" s="49"/>
       <c r="AN17" s="60"/>
     </row>
-    <row r="18" spans="3:54" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:55" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -2143,7 +2150,7 @@
       <c r="AM18" s="4"/>
       <c r="AN18" s="4"/>
     </row>
-    <row r="19" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -2167,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:55" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="61" t="s">
         <v>4</v>
       </c>
@@ -2213,7 +2220,7 @@
       <c r="AM20" s="49"/>
       <c r="AN20" s="60"/>
     </row>
-    <row r="21" spans="3:54" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:55" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -2251,7 +2258,7 @@
       <c r="AM21" s="4"/>
       <c r="AN21" s="4"/>
     </row>
-    <row r="22" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -2293,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:54" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:55" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="62" t="s">
         <v>5</v>
       </c>
@@ -2345,7 +2352,7 @@
       <c r="AM23" s="49"/>
       <c r="AN23" s="60"/>
     </row>
-    <row r="25" spans="3:54" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:55" ht="15" x14ac:dyDescent="0.25">
       <c r="AW25" s="65" t="s">
         <v>48</v>
       </c>
@@ -2353,8 +2360,9 @@
       <c r="AY25" s="65"/>
       <c r="AZ25" s="65"/>
       <c r="BA25" s="65"/>
+      <c r="BB25" s="65"/>
     </row>
-    <row r="26" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="31" t="s">
         <v>57</v>
       </c>
@@ -2378,14 +2386,17 @@
       <c r="AZ26" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="BA26" s="39" t="s">
+      <c r="BA26" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="BB26" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="BB26" s="39" t="s">
+      <c r="BC26" s="39" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
@@ -2496,14 +2507,17 @@
       <c r="AZ27" s="37">
         <v>0</v>
       </c>
-      <c r="BA27" s="40" t="s">
+      <c r="BA27" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB27" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB27" s="37" t="s">
+      <c r="BC27" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
         <v>51</v>
       </c>
@@ -2614,14 +2628,17 @@
       <c r="AZ28" s="37">
         <v>0</v>
       </c>
-      <c r="BA28" s="40" t="s">
+      <c r="BA28" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB28" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB28" s="37" t="s">
+      <c r="BC28" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="3" t="s">
         <v>51</v>
       </c>
@@ -2732,14 +2749,17 @@
       <c r="AZ29" s="37">
         <v>0</v>
       </c>
-      <c r="BA29" s="40" t="s">
+      <c r="BA29" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB29" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB29" s="37" t="s">
+      <c r="BC29" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
         <v>51</v>
       </c>
@@ -2850,14 +2870,17 @@
       <c r="AZ30" s="37">
         <v>0</v>
       </c>
-      <c r="BA30" s="40" t="s">
+      <c r="BA30" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB30" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB30" s="37" t="s">
+      <c r="BC30" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
         <v>51</v>
       </c>
@@ -2968,14 +2991,17 @@
       <c r="AZ31" s="37">
         <v>0</v>
       </c>
-      <c r="BA31" s="40" t="s">
+      <c r="BA31" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB31" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB31" s="37" t="s">
+      <c r="BC31" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3" t="s">
         <v>51</v>
       </c>
@@ -3086,14 +3112,17 @@
       <c r="AZ32" s="37">
         <v>0</v>
       </c>
-      <c r="BA32" s="40" t="s">
+      <c r="BA32" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB32" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB32" s="37" t="s">
+      <c r="BC32" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
@@ -3204,14 +3233,17 @@
       <c r="AZ33" s="37">
         <v>0</v>
       </c>
-      <c r="BA33" s="40" t="s">
+      <c r="BA33" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB33" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB33" s="37" t="s">
+      <c r="BC33" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3" t="s">
         <v>51</v>
       </c>
@@ -3322,14 +3354,17 @@
       <c r="AZ34" s="37">
         <v>0</v>
       </c>
-      <c r="BA34" s="40" t="s">
+      <c r="BA34" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB34" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB34" s="37" t="s">
+      <c r="BC34" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
         <v>51</v>
       </c>
@@ -3440,14 +3475,17 @@
       <c r="AZ35" s="37">
         <v>0</v>
       </c>
-      <c r="BA35" s="40" t="s">
+      <c r="BA35" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB35" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB35" s="37" t="s">
+      <c r="BC35" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="3" t="s">
         <v>51</v>
       </c>
@@ -3558,14 +3596,17 @@
       <c r="AZ36" s="37">
         <v>0</v>
       </c>
-      <c r="BA36" s="40" t="s">
+      <c r="BA36" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB36" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB36" s="37" t="s">
+      <c r="BC36" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:55" ht="15.75" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="3" t="s">
         <v>51</v>
       </c>
@@ -3662,14 +3703,17 @@
       <c r="AZ37" s="37">
         <v>0</v>
       </c>
-      <c r="BA37" s="40" t="s">
+      <c r="BA37" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB37" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB37" s="37" t="s">
+      <c r="BC37" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
         <v>51</v>
       </c>
@@ -3766,14 +3810,17 @@
       <c r="AZ38" s="37">
         <v>0</v>
       </c>
-      <c r="BA38" s="40" t="s">
+      <c r="BA38" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB38" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB38" s="37" t="s">
+      <c r="BC38" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
         <v>51</v>
       </c>
@@ -3870,14 +3917,17 @@
       <c r="AZ39" s="37">
         <v>0</v>
       </c>
-      <c r="BA39" s="40" t="s">
+      <c r="BA39" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB39" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB39" s="37" t="s">
+      <c r="BC39" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="3" t="s">
         <v>51</v>
       </c>
@@ -3974,14 +4024,17 @@
       <c r="AZ40" s="37">
         <v>0</v>
       </c>
-      <c r="BA40" s="40" t="s">
+      <c r="BA40" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB40" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB40" s="37" t="s">
+      <c r="BC40" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
         <v>51</v>
       </c>
@@ -4092,14 +4145,17 @@
       <c r="AZ41" s="37">
         <v>0</v>
       </c>
-      <c r="BA41" s="40" t="s">
+      <c r="BA41" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB41" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB41" s="37" t="s">
+      <c r="BC41" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
         <v>51</v>
       </c>
@@ -4210,14 +4266,17 @@
       <c r="AZ42" s="37">
         <v>0</v>
       </c>
-      <c r="BA42" s="40" t="s">
+      <c r="BA42" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB42" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB42" s="37" t="s">
+      <c r="BC42" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="3" t="s">
         <v>51</v>
       </c>
@@ -4328,14 +4387,17 @@
       <c r="AZ43" s="37">
         <v>0</v>
       </c>
-      <c r="BA43" s="40" t="s">
+      <c r="BA43" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB43" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB43" s="37" t="s">
+      <c r="BC43" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
         <v>51</v>
       </c>
@@ -4432,14 +4494,17 @@
       <c r="AZ44" s="37">
         <v>0</v>
       </c>
-      <c r="BA44" s="40" t="s">
+      <c r="BA44" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB44" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB44" s="37" t="s">
+      <c r="BC44" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="3:54" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
         <v>51</v>
       </c>
@@ -4534,14 +4599,17 @@
       <c r="AZ45" s="37">
         <v>0</v>
       </c>
-      <c r="BA45" s="40" t="s">
+      <c r="BA45" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB45" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB45" s="37" t="s">
+      <c r="BC45" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="3:54" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:55" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
         <v>51</v>
       </c>
@@ -4638,14 +4706,17 @@
       <c r="AZ46" s="42">
         <v>0</v>
       </c>
-      <c r="BA46" s="40" t="s">
+      <c r="BA46" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB46" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="BB46" s="42" t="s">
+      <c r="BC46" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="3:54" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:55" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
         <v>51</v>
       </c>
@@ -4742,14 +4813,17 @@
       <c r="AZ47" s="42">
         <v>0</v>
       </c>
-      <c r="BA47" s="40" t="s">
+      <c r="BA47" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB47" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="BB47" s="42" t="s">
+      <c r="BC47" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:55" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="3" t="s">
         <v>51</v>
       </c>
@@ -4846,14 +4920,17 @@
       <c r="AZ48" s="37">
         <v>0</v>
       </c>
-      <c r="BA48" s="40" t="s">
+      <c r="BA48" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB48" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="BB48" s="37" t="s">
+      <c r="BC48" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:55" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="3" t="s">
         <v>51</v>
       </c>
@@ -4950,14 +5027,17 @@
       <c r="AZ49" s="42">
         <v>0</v>
       </c>
-      <c r="BA49" s="40" t="s">
+      <c r="BA49" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB49" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="BB49" s="42" t="s">
+      <c r="BC49" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:55" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="3" t="s">
         <v>51</v>
       </c>
@@ -5054,14 +5134,20 @@
       <c r="AZ50" s="42">
         <v>0</v>
       </c>
-      <c r="BA50" s="40" t="s">
+      <c r="BA50" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB50" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="BB50" s="42" t="s">
+      <c r="BC50" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="3:54" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:55" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="D51" s="52" t="s">
         <v>73</v>
       </c>
@@ -5069,7 +5155,9 @@
       <c r="F51" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I51" s="53"/>
+      <c r="I51" s="53" t="s">
+        <v>8</v>
+      </c>
       <c r="J51" s="49"/>
       <c r="K51" s="49"/>
       <c r="L51" s="49"/>
@@ -5081,40 +5169,89 @@
       <c r="R51" s="49"/>
       <c r="S51" s="49"/>
       <c r="T51" s="50"/>
-      <c r="U51" s="48"/>
+      <c r="U51" s="48" t="s">
+        <v>10</v>
+      </c>
       <c r="V51" s="49"/>
       <c r="W51" s="49"/>
       <c r="X51" s="49"/>
       <c r="Y51" s="50"/>
-      <c r="Z51" s="16"/>
-      <c r="AA51" s="17"/>
-      <c r="AB51" s="18"/>
-      <c r="AC51" s="48"/>
+      <c r="Z51" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="18">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="48" t="s">
+        <v>11</v>
+      </c>
       <c r="AD51" s="49"/>
       <c r="AE51" s="49"/>
       <c r="AF51" s="49"/>
       <c r="AG51" s="50"/>
-      <c r="AH51" s="44"/>
-      <c r="AI51" s="43"/>
-      <c r="AJ51" s="43"/>
-      <c r="AK51" s="43"/>
-      <c r="AL51" s="43"/>
-      <c r="AM51" s="43"/>
-      <c r="AN51" s="45"/>
-      <c r="AP51" s="51"/>
+      <c r="AH51" s="44">
+        <v>1</v>
+      </c>
+      <c r="AI51" s="43">
+        <v>1</v>
+      </c>
+      <c r="AJ51" s="43">
+        <v>0</v>
+      </c>
+      <c r="AK51" s="43">
+        <v>0</v>
+      </c>
+      <c r="AL51" s="43">
+        <v>1</v>
+      </c>
+      <c r="AM51" s="43">
+        <v>1</v>
+      </c>
+      <c r="AN51" s="45">
+        <v>1</v>
+      </c>
+      <c r="AP51" s="51" t="s">
+        <v>26</v>
+      </c>
       <c r="AQ51" s="51"/>
-      <c r="AR51" s="46"/>
-      <c r="AS51" s="27"/>
-      <c r="AT51" s="27"/>
-      <c r="AU51" s="47"/>
-      <c r="AW51" s="42"/>
-      <c r="AX51" s="42"/>
-      <c r="AY51" s="42"/>
-      <c r="AZ51" s="42"/>
-      <c r="BA51" s="40"/>
-      <c r="BB51" s="42"/>
+      <c r="AR51" s="46">
+        <v>0</v>
+      </c>
+      <c r="AS51" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT51" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU51" s="47">
+        <v>1</v>
+      </c>
+      <c r="AW51" s="42">
+        <v>0</v>
+      </c>
+      <c r="AX51" s="42">
+        <v>1</v>
+      </c>
+      <c r="AY51" s="42">
+        <v>1</v>
+      </c>
+      <c r="AZ51" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA51" s="42">
+        <v>1</v>
+      </c>
+      <c r="BB51" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC51" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="52" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
         <v>51</v>
       </c>
@@ -5213,14 +5350,17 @@
       <c r="AZ52" s="37">
         <v>1</v>
       </c>
-      <c r="BA52" s="40" t="s">
+      <c r="BA52" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB52" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BB52" s="37" t="s">
+      <c r="BC52" s="37" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="52" t="s">
         <v>38</v>
       </c>
@@ -5320,14 +5460,17 @@
       <c r="AZ53" s="37">
         <v>0</v>
       </c>
-      <c r="BA53" s="37" t="s">
+      <c r="BA53" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB53" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="BB53" s="37" t="s">
+      <c r="BC53" s="37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="52" t="s">
         <v>43</v>
       </c>
@@ -5419,10 +5562,13 @@
       <c r="AZ54" s="37">
         <v>0</v>
       </c>
-      <c r="BA54" s="41" t="s">
+      <c r="BA54" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB54" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="BB54" s="37" t="s">
+      <c r="BC54" s="37" t="s">
         <v>50</v>
       </c>
     </row>
@@ -5439,7 +5585,7 @@
     <mergeCell ref="U51:Y51"/>
     <mergeCell ref="AC51:AG51"/>
     <mergeCell ref="AP51:AQ51"/>
-    <mergeCell ref="AW25:BA25"/>
+    <mergeCell ref="AW25:BB25"/>
     <mergeCell ref="AP27:AQ27"/>
     <mergeCell ref="AP28:AQ28"/>
     <mergeCell ref="AP37:AQ37"/>

</xml_diff>

<commit_message>
renamed load_data_ext -> write_data_ext and implemented remaining store instr
</commit_message>
<xml_diff>
--- a/doc/decoding.xlsx
+++ b/doc/decoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\SystemVerilog\FRiscV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9EFA7B-1B8B-43F9-B2BB-3C9009AB4554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD699D2-16BE-4546-AF92-23461508F52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29490" yWindow="1470" windowWidth="25965" windowHeight="14595" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
   </bookViews>
@@ -40,7 +40,7 @@
     <author>Tom</author>
   </authors>
   <commentList>
-    <comment ref="D53" authorId="0" shapeId="0" xr:uid="{E8182568-AF53-41D0-80C8-04611138DC73}">
+    <comment ref="D55" authorId="0" shapeId="0" xr:uid="{E8182568-AF53-41D0-80C8-04611138DC73}">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW53" authorId="0" shapeId="0" xr:uid="{EC372BE6-EF51-477F-B18A-BFF0C74E0CC5}">
+    <comment ref="AW55" authorId="0" shapeId="0" xr:uid="{EC372BE6-EF51-477F-B18A-BFF0C74E0CC5}">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D54" authorId="0" shapeId="0" xr:uid="{94E066D9-6740-478B-B1BE-00F56432855D}">
+    <comment ref="D56" authorId="0" shapeId="0" xr:uid="{94E066D9-6740-478B-B1BE-00F56432855D}">
       <text>
         <r>
           <rPr>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="77">
   <si>
     <t>R-TYPE</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>jSrc</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>SH</t>
   </si>
 </sst>
 </file>
@@ -751,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -876,6 +882,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1300,13 +1309,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA95D64-5055-4174-A4D5-0BDBECB18FB0}">
-  <dimension ref="C1:BC54"/>
+  <dimension ref="C1:BC56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="7" ySplit="23" topLeftCell="H33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="23" topLeftCell="H36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -1332,20 +1341,20 @@
   <sheetData>
     <row r="1" spans="4:47" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP2" s="69" t="s">
+      <c r="AP2" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="AQ2" s="70"/>
-      <c r="AR2" s="70"/>
-      <c r="AS2" s="70"/>
-      <c r="AT2" s="70"/>
-      <c r="AU2" s="71"/>
+      <c r="AQ2" s="71"/>
+      <c r="AR2" s="71"/>
+      <c r="AS2" s="71"/>
+      <c r="AT2" s="71"/>
+      <c r="AU2" s="72"/>
     </row>
     <row r="3" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP3" s="72" t="s">
+      <c r="AP3" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="57"/>
+      <c r="AQ3" s="58"/>
       <c r="AR3" s="21">
         <v>0</v>
       </c>
@@ -1355,15 +1364,15 @@
       <c r="AT3" s="21">
         <v>0</v>
       </c>
-      <c r="AU3" s="73">
+      <c r="AU3" s="74">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP4" s="74" t="s">
+      <c r="AP4" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="AQ4" s="56"/>
+      <c r="AQ4" s="57"/>
       <c r="AR4" s="21">
         <v>0</v>
       </c>
@@ -1373,7 +1382,7 @@
       <c r="AT4" s="21">
         <v>0</v>
       </c>
-      <c r="AU4" s="73">
+      <c r="AU4" s="74">
         <v>1</v>
       </c>
     </row>
@@ -1474,10 +1483,10 @@
       <c r="AN5" s="2">
         <v>0</v>
       </c>
-      <c r="AP5" s="74" t="s">
+      <c r="AP5" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="AQ5" s="56"/>
+      <c r="AQ5" s="57"/>
       <c r="AR5" s="21">
         <v>0</v>
       </c>
@@ -1487,7 +1496,7 @@
       <c r="AT5" s="21">
         <v>1</v>
       </c>
-      <c r="AU5" s="73">
+      <c r="AU5" s="74">
         <v>0</v>
       </c>
     </row>
@@ -1524,10 +1533,10 @@
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
-      <c r="AP6" s="74" t="s">
+      <c r="AP6" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="AQ6" s="56"/>
+      <c r="AQ6" s="57"/>
       <c r="AR6" s="21">
         <v>0</v>
       </c>
@@ -1537,7 +1546,7 @@
       <c r="AT6" s="21">
         <v>1</v>
       </c>
-      <c r="AU6" s="73">
+      <c r="AU6" s="74">
         <v>1</v>
       </c>
     </row>
@@ -1578,10 +1587,10 @@
       <c r="AN7" s="3">
         <v>0</v>
       </c>
-      <c r="AP7" s="74" t="s">
+      <c r="AP7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="AQ7" s="56"/>
+      <c r="AQ7" s="57"/>
       <c r="AR7" s="21">
         <v>0</v>
       </c>
@@ -1591,65 +1600,65 @@
       <c r="AT7" s="21">
         <v>0</v>
       </c>
-      <c r="AU7" s="73">
+      <c r="AU7" s="74">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="I8" s="53" t="s">
+      <c r="D8" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="I8" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="48" t="s">
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="48" t="s">
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V8" s="49"/>
-      <c r="W8" s="49"/>
-      <c r="X8" s="49"/>
-      <c r="Y8" s="50"/>
-      <c r="Z8" s="48" t="s">
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="50"/>
+      <c r="Y8" s="51"/>
+      <c r="Z8" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="49"/>
-      <c r="AB8" s="50"/>
-      <c r="AC8" s="48" t="s">
+      <c r="AA8" s="50"/>
+      <c r="AB8" s="51"/>
+      <c r="AC8" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD8" s="49"/>
-      <c r="AE8" s="49"/>
-      <c r="AF8" s="49"/>
-      <c r="AG8" s="50"/>
-      <c r="AH8" s="48" t="s">
+      <c r="AD8" s="50"/>
+      <c r="AE8" s="50"/>
+      <c r="AF8" s="50"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="AI8" s="49"/>
-      <c r="AJ8" s="49"/>
-      <c r="AK8" s="49"/>
-      <c r="AL8" s="49"/>
-      <c r="AM8" s="49"/>
-      <c r="AN8" s="60"/>
-      <c r="AP8" s="74" t="s">
+      <c r="AI8" s="50"/>
+      <c r="AJ8" s="50"/>
+      <c r="AK8" s="50"/>
+      <c r="AL8" s="50"/>
+      <c r="AM8" s="50"/>
+      <c r="AN8" s="61"/>
+      <c r="AP8" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="AQ8" s="56"/>
+      <c r="AQ8" s="57"/>
       <c r="AR8" s="21">
         <v>0</v>
       </c>
@@ -1659,7 +1668,7 @@
       <c r="AT8" s="21">
         <v>0</v>
       </c>
-      <c r="AU8" s="73">
+      <c r="AU8" s="74">
         <v>1</v>
       </c>
     </row>
@@ -1700,10 +1709,10 @@
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
-      <c r="AP9" s="74" t="s">
+      <c r="AP9" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="AQ9" s="56"/>
+      <c r="AQ9" s="57"/>
       <c r="AR9" s="21">
         <v>0</v>
       </c>
@@ -1713,7 +1722,7 @@
       <c r="AT9" s="21">
         <v>1</v>
       </c>
-      <c r="AU9" s="73">
+      <c r="AU9" s="74">
         <v>0</v>
       </c>
     </row>
@@ -1752,10 +1761,10 @@
       <c r="AN10" s="3">
         <v>0</v>
       </c>
-      <c r="AP10" s="74" t="s">
+      <c r="AP10" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="AQ10" s="56"/>
+      <c r="AQ10" s="57"/>
       <c r="AR10" s="21">
         <v>0</v>
       </c>
@@ -1765,73 +1774,73 @@
       <c r="AT10" s="21">
         <v>1</v>
       </c>
-      <c r="AU10" s="73">
+      <c r="AU10" s="74">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="I11" s="53" t="s">
+      <c r="D11" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="I11" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="49"/>
-      <c r="P11" s="49"/>
-      <c r="Q11" s="49"/>
-      <c r="R11" s="49"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="50"/>
-      <c r="U11" s="48" t="s">
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V11" s="49"/>
-      <c r="W11" s="49"/>
-      <c r="X11" s="49"/>
-      <c r="Y11" s="50"/>
-      <c r="Z11" s="48" t="s">
+      <c r="V11" s="50"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
+      <c r="Y11" s="51"/>
+      <c r="Z11" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="AA11" s="49"/>
-      <c r="AB11" s="50"/>
-      <c r="AC11" s="48" t="s">
+      <c r="AA11" s="50"/>
+      <c r="AB11" s="51"/>
+      <c r="AC11" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD11" s="49"/>
-      <c r="AE11" s="49"/>
-      <c r="AF11" s="49"/>
-      <c r="AG11" s="50"/>
-      <c r="AH11" s="48" t="s">
+      <c r="AD11" s="50"/>
+      <c r="AE11" s="50"/>
+      <c r="AF11" s="50"/>
+      <c r="AG11" s="51"/>
+      <c r="AH11" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="AI11" s="49"/>
-      <c r="AJ11" s="49"/>
-      <c r="AK11" s="49"/>
-      <c r="AL11" s="49"/>
-      <c r="AM11" s="49"/>
-      <c r="AN11" s="60"/>
-      <c r="AP11" s="75" t="s">
+      <c r="AI11" s="50"/>
+      <c r="AJ11" s="50"/>
+      <c r="AK11" s="50"/>
+      <c r="AL11" s="50"/>
+      <c r="AM11" s="50"/>
+      <c r="AN11" s="61"/>
+      <c r="AP11" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="AQ11" s="76"/>
-      <c r="AR11" s="77">
-        <v>1</v>
-      </c>
-      <c r="AS11" s="77">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="77">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="78">
+      <c r="AQ11" s="77"/>
+      <c r="AR11" s="78">
+        <v>1</v>
+      </c>
+      <c r="AS11" s="78">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="78">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="79">
         <v>0</v>
       </c>
     </row>
@@ -1872,12 +1881,12 @@
       <c r="AL12" s="4"/>
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
-      <c r="AP12" s="67"/>
-      <c r="AQ12" s="67"/>
-      <c r="AR12" s="68"/>
-      <c r="AS12" s="68"/>
-      <c r="AT12" s="68"/>
-      <c r="AU12" s="68"/>
+      <c r="AP12" s="68"/>
+      <c r="AQ12" s="68"/>
+      <c r="AR12" s="69"/>
+      <c r="AS12" s="69"/>
+      <c r="AT12" s="69"/>
+      <c r="AU12" s="69"/>
     </row>
     <row r="13" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="5"/>
@@ -1922,56 +1931,56 @@
       </c>
     </row>
     <row r="14" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="59" t="s">
+      <c r="D14" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="I14" s="53" t="s">
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="I14" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="48" t="s">
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49"/>
-      <c r="S14" s="49"/>
-      <c r="T14" s="50"/>
-      <c r="U14" s="48" t="s">
+      <c r="Q14" s="50"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="50"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V14" s="49"/>
-      <c r="W14" s="49"/>
-      <c r="X14" s="49"/>
-      <c r="Y14" s="50"/>
-      <c r="Z14" s="48" t="s">
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="50"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="AA14" s="49"/>
-      <c r="AB14" s="50"/>
-      <c r="AC14" s="48" t="s">
+      <c r="AA14" s="50"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="AD14" s="49"/>
-      <c r="AE14" s="49"/>
-      <c r="AF14" s="49"/>
-      <c r="AG14" s="50"/>
-      <c r="AH14" s="48" t="s">
+      <c r="AD14" s="50"/>
+      <c r="AE14" s="50"/>
+      <c r="AF14" s="50"/>
+      <c r="AG14" s="51"/>
+      <c r="AH14" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="AI14" s="49"/>
-      <c r="AJ14" s="49"/>
-      <c r="AK14" s="49"/>
-      <c r="AL14" s="49"/>
-      <c r="AM14" s="49"/>
-      <c r="AN14" s="60"/>
+      <c r="AI14" s="50"/>
+      <c r="AJ14" s="50"/>
+      <c r="AK14" s="50"/>
+      <c r="AL14" s="50"/>
+      <c r="AM14" s="50"/>
+      <c r="AN14" s="61"/>
     </row>
     <row r="15" spans="4:47" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
@@ -2057,60 +2066,60 @@
       </c>
     </row>
     <row r="17" spans="3:55" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="64" t="s">
+      <c r="D17" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
       <c r="I17" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="53" t="s">
+      <c r="J17" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="50"/>
-      <c r="P17" s="48" t="s">
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q17" s="49"/>
-      <c r="R17" s="49"/>
-      <c r="S17" s="49"/>
-      <c r="T17" s="50"/>
-      <c r="U17" s="48" t="s">
+      <c r="Q17" s="50"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V17" s="49"/>
-      <c r="W17" s="49"/>
-      <c r="X17" s="49"/>
-      <c r="Y17" s="50"/>
-      <c r="Z17" s="48" t="s">
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="51"/>
+      <c r="Z17" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="AA17" s="49"/>
-      <c r="AB17" s="50"/>
-      <c r="AC17" s="48" t="s">
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="51"/>
+      <c r="AC17" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="AD17" s="49"/>
-      <c r="AE17" s="49"/>
-      <c r="AF17" s="50"/>
+      <c r="AD17" s="50"/>
+      <c r="AE17" s="50"/>
+      <c r="AF17" s="51"/>
       <c r="AG17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AH17" s="48" t="s">
+      <c r="AH17" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="AI17" s="49"/>
-      <c r="AJ17" s="49"/>
-      <c r="AK17" s="49"/>
-      <c r="AL17" s="49"/>
-      <c r="AM17" s="49"/>
-      <c r="AN17" s="60"/>
+      <c r="AI17" s="50"/>
+      <c r="AJ17" s="50"/>
+      <c r="AK17" s="50"/>
+      <c r="AL17" s="50"/>
+      <c r="AM17" s="50"/>
+      <c r="AN17" s="61"/>
     </row>
     <row r="18" spans="3:55" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
@@ -2175,50 +2184,50 @@
       </c>
     </row>
     <row r="20" spans="3:55" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="I20" s="53" t="s">
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="I20" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="49"/>
-      <c r="S20" s="49"/>
-      <c r="T20" s="49"/>
-      <c r="U20" s="49"/>
-      <c r="V20" s="49"/>
-      <c r="W20" s="49"/>
-      <c r="X20" s="49"/>
-      <c r="Y20" s="49"/>
-      <c r="Z20" s="49"/>
-      <c r="AA20" s="49"/>
-      <c r="AB20" s="50"/>
-      <c r="AC20" s="48" t="s">
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="50"/>
+      <c r="S20" s="50"/>
+      <c r="T20" s="50"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="50"/>
+      <c r="W20" s="50"/>
+      <c r="X20" s="50"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="50"/>
+      <c r="AB20" s="51"/>
+      <c r="AC20" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD20" s="49"/>
-      <c r="AE20" s="49"/>
-      <c r="AF20" s="49"/>
-      <c r="AG20" s="50"/>
-      <c r="AH20" s="48" t="s">
+      <c r="AD20" s="50"/>
+      <c r="AE20" s="50"/>
+      <c r="AF20" s="50"/>
+      <c r="AG20" s="51"/>
+      <c r="AH20" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="AI20" s="49"/>
-      <c r="AJ20" s="49"/>
-      <c r="AK20" s="49"/>
-      <c r="AL20" s="49"/>
-      <c r="AM20" s="49"/>
-      <c r="AN20" s="60"/>
+      <c r="AI20" s="50"/>
+      <c r="AJ20" s="50"/>
+      <c r="AK20" s="50"/>
+      <c r="AL20" s="50"/>
+      <c r="AM20" s="50"/>
+      <c r="AN20" s="61"/>
     </row>
     <row r="21" spans="3:55" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
@@ -2301,77 +2310,77 @@
       </c>
     </row>
     <row r="23" spans="3:55" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="62" t="s">
+      <c r="D23" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
       <c r="I23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="48" t="s">
+      <c r="J23" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="49"/>
-      <c r="Q23" s="49"/>
-      <c r="R23" s="49"/>
-      <c r="S23" s="49"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
       <c r="T23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U23" s="48" t="s">
+      <c r="U23" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="V23" s="49"/>
-      <c r="W23" s="49"/>
-      <c r="X23" s="49"/>
-      <c r="Y23" s="49"/>
-      <c r="Z23" s="49"/>
-      <c r="AA23" s="49"/>
-      <c r="AB23" s="50"/>
-      <c r="AC23" s="48" t="s">
+      <c r="V23" s="50"/>
+      <c r="W23" s="50"/>
+      <c r="X23" s="50"/>
+      <c r="Y23" s="50"/>
+      <c r="Z23" s="50"/>
+      <c r="AA23" s="50"/>
+      <c r="AB23" s="51"/>
+      <c r="AC23" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD23" s="49"/>
-      <c r="AE23" s="49"/>
-      <c r="AF23" s="49"/>
-      <c r="AG23" s="50"/>
-      <c r="AH23" s="48" t="s">
+      <c r="AD23" s="50"/>
+      <c r="AE23" s="50"/>
+      <c r="AF23" s="50"/>
+      <c r="AG23" s="51"/>
+      <c r="AH23" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="AI23" s="49"/>
-      <c r="AJ23" s="49"/>
-      <c r="AK23" s="49"/>
-      <c r="AL23" s="49"/>
-      <c r="AM23" s="49"/>
-      <c r="AN23" s="60"/>
+      <c r="AI23" s="50"/>
+      <c r="AJ23" s="50"/>
+      <c r="AK23" s="50"/>
+      <c r="AL23" s="50"/>
+      <c r="AM23" s="50"/>
+      <c r="AN23" s="61"/>
     </row>
     <row r="25" spans="3:55" ht="15" x14ac:dyDescent="0.25">
-      <c r="AW25" s="65" t="s">
+      <c r="AW25" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="AX25" s="65"/>
-      <c r="AY25" s="65"/>
-      <c r="AZ25" s="65"/>
-      <c r="BA25" s="65"/>
-      <c r="BB25" s="65"/>
+      <c r="AX25" s="66"/>
+      <c r="AY25" s="66"/>
+      <c r="AZ25" s="66"/>
+      <c r="BA25" s="66"/>
+      <c r="BB25" s="66"/>
     </row>
     <row r="26" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="AP26" s="66" t="s">
+      <c r="AP26" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="AQ26" s="66"/>
-      <c r="AR26" s="66"/>
-      <c r="AS26" s="66"/>
+      <c r="AQ26" s="67"/>
+      <c r="AR26" s="67"/>
+      <c r="AS26" s="67"/>
       <c r="AT26" s="22"/>
       <c r="AU26" s="22"/>
       <c r="AW26" s="38" t="s">
@@ -2400,10 +2409,10 @@
       <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="52" t="s">
+      <c r="D27" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="52"/>
+      <c r="E27" s="53"/>
       <c r="F27" s="19" t="s">
         <v>27</v>
       </c>
@@ -2428,20 +2437,20 @@
       <c r="O27" s="10">
         <v>0</v>
       </c>
-      <c r="P27" s="48" t="s">
+      <c r="P27" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="49"/>
-      <c r="S27" s="49"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="48" t="s">
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="51"/>
+      <c r="U27" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V27" s="49"/>
-      <c r="W27" s="49"/>
-      <c r="X27" s="49"/>
-      <c r="Y27" s="50"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="50"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="51"/>
       <c r="Z27" s="16">
         <v>0</v>
       </c>
@@ -2451,13 +2460,13 @@
       <c r="AB27" s="18">
         <v>0</v>
       </c>
-      <c r="AC27" s="48" t="s">
+      <c r="AC27" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD27" s="49"/>
-      <c r="AE27" s="49"/>
-      <c r="AF27" s="49"/>
-      <c r="AG27" s="50"/>
+      <c r="AD27" s="50"/>
+      <c r="AE27" s="50"/>
+      <c r="AF27" s="50"/>
+      <c r="AG27" s="51"/>
       <c r="AH27" s="8">
         <v>0</v>
       </c>
@@ -2479,10 +2488,10 @@
       <c r="AN27" s="15">
         <v>1</v>
       </c>
-      <c r="AP27" s="51" t="s">
+      <c r="AP27" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ27" s="51"/>
+      <c r="AQ27" s="52"/>
       <c r="AR27" s="23">
         <v>0</v>
       </c>
@@ -2521,10 +2530,10 @@
       <c r="C28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="52" t="s">
+      <c r="D28" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="52"/>
+      <c r="E28" s="53"/>
       <c r="F28" s="19" t="s">
         <v>27</v>
       </c>
@@ -2549,20 +2558,20 @@
       <c r="O28" s="10">
         <v>0</v>
       </c>
-      <c r="P28" s="48" t="s">
+      <c r="P28" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
-      <c r="T28" s="50"/>
-      <c r="U28" s="48" t="s">
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V28" s="49"/>
-      <c r="W28" s="49"/>
-      <c r="X28" s="49"/>
-      <c r="Y28" s="50"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="51"/>
       <c r="Z28" s="16">
         <v>0</v>
       </c>
@@ -2572,13 +2581,13 @@
       <c r="AB28" s="18">
         <v>0</v>
       </c>
-      <c r="AC28" s="48" t="s">
+      <c r="AC28" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD28" s="49"/>
-      <c r="AE28" s="49"/>
-      <c r="AF28" s="49"/>
-      <c r="AG28" s="50"/>
+      <c r="AD28" s="50"/>
+      <c r="AE28" s="50"/>
+      <c r="AF28" s="50"/>
+      <c r="AG28" s="51"/>
       <c r="AH28" s="8">
         <v>0</v>
       </c>
@@ -2600,10 +2609,10 @@
       <c r="AN28" s="15">
         <v>1</v>
       </c>
-      <c r="AP28" s="51" t="s">
+      <c r="AP28" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="AQ28" s="51"/>
+      <c r="AQ28" s="52"/>
       <c r="AR28" s="26">
         <v>0</v>
       </c>
@@ -2642,10 +2651,10 @@
       <c r="C29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="52" t="s">
+      <c r="D29" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="52"/>
+      <c r="E29" s="53"/>
       <c r="F29" s="19" t="s">
         <v>27</v>
       </c>
@@ -2670,20 +2679,20 @@
       <c r="O29" s="34">
         <v>0</v>
       </c>
-      <c r="P29" s="48" t="s">
+      <c r="P29" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="49"/>
-      <c r="S29" s="49"/>
-      <c r="T29" s="50"/>
-      <c r="U29" s="48" t="s">
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V29" s="49"/>
-      <c r="W29" s="49"/>
-      <c r="X29" s="49"/>
-      <c r="Y29" s="50"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="50"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="51"/>
       <c r="Z29" s="16">
         <v>1</v>
       </c>
@@ -2693,13 +2702,13 @@
       <c r="AB29" s="18">
         <v>0</v>
       </c>
-      <c r="AC29" s="48" t="s">
+      <c r="AC29" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD29" s="49"/>
-      <c r="AE29" s="49"/>
-      <c r="AF29" s="49"/>
-      <c r="AG29" s="50"/>
+      <c r="AD29" s="50"/>
+      <c r="AE29" s="50"/>
+      <c r="AF29" s="50"/>
+      <c r="AG29" s="51"/>
       <c r="AH29" s="32">
         <v>0</v>
       </c>
@@ -2721,10 +2730,10 @@
       <c r="AN29" s="36">
         <v>1</v>
       </c>
-      <c r="AP29" s="54" t="s">
+      <c r="AP29" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="AQ29" s="55"/>
+      <c r="AQ29" s="56"/>
       <c r="AR29" s="26">
         <v>0</v>
       </c>
@@ -2763,10 +2772,10 @@
       <c r="C30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="52"/>
+      <c r="E30" s="53"/>
       <c r="F30" s="19" t="s">
         <v>27</v>
       </c>
@@ -2791,20 +2800,20 @@
       <c r="O30" s="34">
         <v>0</v>
       </c>
-      <c r="P30" s="48" t="s">
+      <c r="P30" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="50"/>
-      <c r="U30" s="48" t="s">
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="51"/>
+      <c r="U30" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V30" s="49"/>
-      <c r="W30" s="49"/>
-      <c r="X30" s="49"/>
-      <c r="Y30" s="50"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="51"/>
       <c r="Z30" s="16">
         <v>1</v>
       </c>
@@ -2814,13 +2823,13 @@
       <c r="AB30" s="18">
         <v>0</v>
       </c>
-      <c r="AC30" s="48" t="s">
+      <c r="AC30" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD30" s="49"/>
-      <c r="AE30" s="49"/>
-      <c r="AF30" s="49"/>
-      <c r="AG30" s="50"/>
+      <c r="AD30" s="50"/>
+      <c r="AE30" s="50"/>
+      <c r="AF30" s="50"/>
+      <c r="AG30" s="51"/>
       <c r="AH30" s="32">
         <v>0</v>
       </c>
@@ -2842,10 +2851,10 @@
       <c r="AN30" s="36">
         <v>1</v>
       </c>
-      <c r="AP30" s="54" t="s">
+      <c r="AP30" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="AQ30" s="55"/>
+      <c r="AQ30" s="56"/>
       <c r="AR30" s="26">
         <v>0</v>
       </c>
@@ -2884,10 +2893,10 @@
       <c r="C31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="52"/>
+      <c r="E31" s="53"/>
       <c r="F31" s="19" t="s">
         <v>27</v>
       </c>
@@ -2912,20 +2921,20 @@
       <c r="O31" s="34">
         <v>0</v>
       </c>
-      <c r="P31" s="48" t="s">
+      <c r="P31" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
-      <c r="T31" s="50"/>
-      <c r="U31" s="48" t="s">
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V31" s="49"/>
-      <c r="W31" s="49"/>
-      <c r="X31" s="49"/>
-      <c r="Y31" s="50"/>
+      <c r="V31" s="50"/>
+      <c r="W31" s="50"/>
+      <c r="X31" s="50"/>
+      <c r="Y31" s="51"/>
       <c r="Z31" s="16">
         <v>1</v>
       </c>
@@ -2935,13 +2944,13 @@
       <c r="AB31" s="18">
         <v>1</v>
       </c>
-      <c r="AC31" s="48" t="s">
+      <c r="AC31" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD31" s="49"/>
-      <c r="AE31" s="49"/>
-      <c r="AF31" s="49"/>
-      <c r="AG31" s="50"/>
+      <c r="AD31" s="50"/>
+      <c r="AE31" s="50"/>
+      <c r="AF31" s="50"/>
+      <c r="AG31" s="51"/>
       <c r="AH31" s="32">
         <v>0</v>
       </c>
@@ -2963,10 +2972,10 @@
       <c r="AN31" s="36">
         <v>1</v>
       </c>
-      <c r="AP31" s="54" t="s">
+      <c r="AP31" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="AQ31" s="55"/>
+      <c r="AQ31" s="56"/>
       <c r="AR31" s="26">
         <v>0</v>
       </c>
@@ -3005,10 +3014,10 @@
       <c r="C32" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="52" t="s">
+      <c r="D32" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="52"/>
+      <c r="E32" s="53"/>
       <c r="F32" s="19" t="s">
         <v>27</v>
       </c>
@@ -3033,20 +3042,20 @@
       <c r="O32" s="34">
         <v>0</v>
       </c>
-      <c r="P32" s="48" t="s">
+      <c r="P32" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="49"/>
-      <c r="S32" s="49"/>
-      <c r="T32" s="50"/>
-      <c r="U32" s="48" t="s">
+      <c r="Q32" s="50"/>
+      <c r="R32" s="50"/>
+      <c r="S32" s="50"/>
+      <c r="T32" s="51"/>
+      <c r="U32" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V32" s="49"/>
-      <c r="W32" s="49"/>
-      <c r="X32" s="49"/>
-      <c r="Y32" s="50"/>
+      <c r="V32" s="50"/>
+      <c r="W32" s="50"/>
+      <c r="X32" s="50"/>
+      <c r="Y32" s="51"/>
       <c r="Z32" s="16">
         <v>0</v>
       </c>
@@ -3056,13 +3065,13 @@
       <c r="AB32" s="18">
         <v>1</v>
       </c>
-      <c r="AC32" s="48" t="s">
+      <c r="AC32" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD32" s="49"/>
-      <c r="AE32" s="49"/>
-      <c r="AF32" s="49"/>
-      <c r="AG32" s="50"/>
+      <c r="AD32" s="50"/>
+      <c r="AE32" s="50"/>
+      <c r="AF32" s="50"/>
+      <c r="AG32" s="51"/>
       <c r="AH32" s="32">
         <v>0</v>
       </c>
@@ -3084,10 +3093,10 @@
       <c r="AN32" s="36">
         <v>1</v>
       </c>
-      <c r="AP32" s="54" t="s">
+      <c r="AP32" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="AQ32" s="55"/>
+      <c r="AQ32" s="56"/>
       <c r="AR32" s="26">
         <v>0</v>
       </c>
@@ -3126,10 +3135,10 @@
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="52" t="s">
+      <c r="D33" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="52"/>
+      <c r="E33" s="53"/>
       <c r="F33" s="19" t="s">
         <v>27</v>
       </c>
@@ -3154,20 +3163,20 @@
       <c r="O33" s="34">
         <v>0</v>
       </c>
-      <c r="P33" s="48" t="s">
+      <c r="P33" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="50"/>
-      <c r="U33" s="48" t="s">
+      <c r="Q33" s="50"/>
+      <c r="R33" s="50"/>
+      <c r="S33" s="50"/>
+      <c r="T33" s="51"/>
+      <c r="U33" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V33" s="49"/>
-      <c r="W33" s="49"/>
-      <c r="X33" s="49"/>
-      <c r="Y33" s="50"/>
+      <c r="V33" s="50"/>
+      <c r="W33" s="50"/>
+      <c r="X33" s="50"/>
+      <c r="Y33" s="51"/>
       <c r="Z33" s="16">
         <v>1</v>
       </c>
@@ -3177,13 +3186,13 @@
       <c r="AB33" s="18">
         <v>1</v>
       </c>
-      <c r="AC33" s="48" t="s">
+      <c r="AC33" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD33" s="49"/>
-      <c r="AE33" s="49"/>
-      <c r="AF33" s="49"/>
-      <c r="AG33" s="50"/>
+      <c r="AD33" s="50"/>
+      <c r="AE33" s="50"/>
+      <c r="AF33" s="50"/>
+      <c r="AG33" s="51"/>
       <c r="AH33" s="32">
         <v>0</v>
       </c>
@@ -3205,10 +3214,10 @@
       <c r="AN33" s="36">
         <v>1</v>
       </c>
-      <c r="AP33" s="54" t="s">
+      <c r="AP33" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="AQ33" s="55"/>
+      <c r="AQ33" s="56"/>
       <c r="AR33" s="26">
         <v>1</v>
       </c>
@@ -3247,10 +3256,10 @@
       <c r="C34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="52" t="s">
+      <c r="D34" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="52"/>
+      <c r="E34" s="53"/>
       <c r="F34" s="19" t="s">
         <v>27</v>
       </c>
@@ -3275,20 +3284,20 @@
       <c r="O34" s="34">
         <v>0</v>
       </c>
-      <c r="P34" s="48" t="s">
+      <c r="P34" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="49"/>
-      <c r="S34" s="49"/>
-      <c r="T34" s="50"/>
-      <c r="U34" s="48" t="s">
+      <c r="Q34" s="50"/>
+      <c r="R34" s="50"/>
+      <c r="S34" s="50"/>
+      <c r="T34" s="51"/>
+      <c r="U34" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V34" s="49"/>
-      <c r="W34" s="49"/>
-      <c r="X34" s="49"/>
-      <c r="Y34" s="50"/>
+      <c r="V34" s="50"/>
+      <c r="W34" s="50"/>
+      <c r="X34" s="50"/>
+      <c r="Y34" s="51"/>
       <c r="Z34" s="16">
         <v>1</v>
       </c>
@@ -3298,13 +3307,13 @@
       <c r="AB34" s="18">
         <v>1</v>
       </c>
-      <c r="AC34" s="48" t="s">
+      <c r="AC34" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD34" s="49"/>
-      <c r="AE34" s="49"/>
-      <c r="AF34" s="49"/>
-      <c r="AG34" s="50"/>
+      <c r="AD34" s="50"/>
+      <c r="AE34" s="50"/>
+      <c r="AF34" s="50"/>
+      <c r="AG34" s="51"/>
       <c r="AH34" s="32">
         <v>0</v>
       </c>
@@ -3326,10 +3335,10 @@
       <c r="AN34" s="36">
         <v>1</v>
       </c>
-      <c r="AP34" s="54" t="s">
+      <c r="AP34" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="AQ34" s="55"/>
+      <c r="AQ34" s="56"/>
       <c r="AR34" s="26">
         <v>0</v>
       </c>
@@ -3368,10 +3377,10 @@
       <c r="C35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="52"/>
+      <c r="E35" s="53"/>
       <c r="F35" s="19" t="s">
         <v>27</v>
       </c>
@@ -3396,20 +3405,20 @@
       <c r="O35" s="34">
         <v>0</v>
       </c>
-      <c r="P35" s="48" t="s">
+      <c r="P35" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
-      <c r="T35" s="50"/>
-      <c r="U35" s="48" t="s">
+      <c r="Q35" s="50"/>
+      <c r="R35" s="50"/>
+      <c r="S35" s="50"/>
+      <c r="T35" s="51"/>
+      <c r="U35" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V35" s="49"/>
-      <c r="W35" s="49"/>
-      <c r="X35" s="49"/>
-      <c r="Y35" s="50"/>
+      <c r="V35" s="50"/>
+      <c r="W35" s="50"/>
+      <c r="X35" s="50"/>
+      <c r="Y35" s="51"/>
       <c r="Z35" s="16">
         <v>0</v>
       </c>
@@ -3419,13 +3428,13 @@
       <c r="AB35" s="18">
         <v>0</v>
       </c>
-      <c r="AC35" s="48" t="s">
+      <c r="AC35" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD35" s="49"/>
-      <c r="AE35" s="49"/>
-      <c r="AF35" s="49"/>
-      <c r="AG35" s="50"/>
+      <c r="AD35" s="50"/>
+      <c r="AE35" s="50"/>
+      <c r="AF35" s="50"/>
+      <c r="AG35" s="51"/>
       <c r="AH35" s="32">
         <v>0</v>
       </c>
@@ -3447,10 +3456,10 @@
       <c r="AN35" s="36">
         <v>1</v>
       </c>
-      <c r="AP35" s="54" t="s">
+      <c r="AP35" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="AQ35" s="55"/>
+      <c r="AQ35" s="56"/>
       <c r="AR35" s="26">
         <v>0</v>
       </c>
@@ -3489,10 +3498,10 @@
       <c r="C36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="52"/>
+      <c r="E36" s="53"/>
       <c r="F36" s="19" t="s">
         <v>27</v>
       </c>
@@ -3517,20 +3526,20 @@
       <c r="O36" s="34">
         <v>0</v>
       </c>
-      <c r="P36" s="48" t="s">
+      <c r="P36" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="49"/>
-      <c r="S36" s="49"/>
-      <c r="T36" s="50"/>
-      <c r="U36" s="48" t="s">
+      <c r="Q36" s="50"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V36" s="49"/>
-      <c r="W36" s="49"/>
-      <c r="X36" s="49"/>
-      <c r="Y36" s="50"/>
+      <c r="V36" s="50"/>
+      <c r="W36" s="50"/>
+      <c r="X36" s="50"/>
+      <c r="Y36" s="51"/>
       <c r="Z36" s="16">
         <v>0</v>
       </c>
@@ -3540,13 +3549,13 @@
       <c r="AB36" s="18">
         <v>1</v>
       </c>
-      <c r="AC36" s="48" t="s">
+      <c r="AC36" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD36" s="49"/>
-      <c r="AE36" s="49"/>
-      <c r="AF36" s="49"/>
-      <c r="AG36" s="50"/>
+      <c r="AD36" s="50"/>
+      <c r="AE36" s="50"/>
+      <c r="AF36" s="50"/>
+      <c r="AG36" s="51"/>
       <c r="AH36" s="32">
         <v>0</v>
       </c>
@@ -3568,10 +3577,10 @@
       <c r="AN36" s="36">
         <v>1</v>
       </c>
-      <c r="AP36" s="54" t="s">
+      <c r="AP36" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="AQ36" s="55"/>
+      <c r="AQ36" s="56"/>
       <c r="AR36" s="26">
         <v>1</v>
       </c>
@@ -3610,34 +3619,34 @@
       <c r="C37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="52" t="s">
+      <c r="D37" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="52"/>
+      <c r="E37" s="53"/>
       <c r="F37" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I37" s="53" t="s">
+      <c r="I37" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="49"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="49"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="50"/>
-      <c r="U37" s="48" t="s">
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+      <c r="Q37" s="50"/>
+      <c r="R37" s="50"/>
+      <c r="S37" s="50"/>
+      <c r="T37" s="51"/>
+      <c r="U37" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V37" s="49"/>
-      <c r="W37" s="49"/>
-      <c r="X37" s="49"/>
-      <c r="Y37" s="50"/>
+      <c r="V37" s="50"/>
+      <c r="W37" s="50"/>
+      <c r="X37" s="50"/>
+      <c r="Y37" s="51"/>
       <c r="Z37" s="16">
         <v>0</v>
       </c>
@@ -3647,13 +3656,13 @@
       <c r="AB37" s="18">
         <v>0</v>
       </c>
-      <c r="AC37" s="48" t="s">
+      <c r="AC37" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD37" s="49"/>
-      <c r="AE37" s="49"/>
-      <c r="AF37" s="49"/>
-      <c r="AG37" s="50"/>
+      <c r="AD37" s="50"/>
+      <c r="AE37" s="50"/>
+      <c r="AF37" s="50"/>
+      <c r="AG37" s="51"/>
       <c r="AH37" s="8">
         <v>0</v>
       </c>
@@ -3675,10 +3684,10 @@
       <c r="AN37" s="15">
         <v>1</v>
       </c>
-      <c r="AP37" s="51" t="s">
+      <c r="AP37" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ37" s="51"/>
+      <c r="AQ37" s="52"/>
       <c r="AR37" s="26">
         <v>0</v>
       </c>
@@ -3717,34 +3726,34 @@
       <c r="C38" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="52" t="s">
+      <c r="D38" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="52"/>
+      <c r="E38" s="53"/>
       <c r="F38" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="53" t="s">
+      <c r="I38" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="49"/>
-      <c r="P38" s="49"/>
-      <c r="Q38" s="49"/>
-      <c r="R38" s="49"/>
-      <c r="S38" s="49"/>
-      <c r="T38" s="50"/>
-      <c r="U38" s="48" t="s">
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="50"/>
+      <c r="R38" s="50"/>
+      <c r="S38" s="50"/>
+      <c r="T38" s="51"/>
+      <c r="U38" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V38" s="49"/>
-      <c r="W38" s="49"/>
-      <c r="X38" s="49"/>
-      <c r="Y38" s="50"/>
+      <c r="V38" s="50"/>
+      <c r="W38" s="50"/>
+      <c r="X38" s="50"/>
+      <c r="Y38" s="51"/>
       <c r="Z38" s="16">
         <v>1</v>
       </c>
@@ -3754,13 +3763,13 @@
       <c r="AB38" s="18">
         <v>0</v>
       </c>
-      <c r="AC38" s="48" t="s">
+      <c r="AC38" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD38" s="49"/>
-      <c r="AE38" s="49"/>
-      <c r="AF38" s="49"/>
-      <c r="AG38" s="50"/>
+      <c r="AD38" s="50"/>
+      <c r="AE38" s="50"/>
+      <c r="AF38" s="50"/>
+      <c r="AG38" s="51"/>
       <c r="AH38" s="32">
         <v>0</v>
       </c>
@@ -3782,10 +3791,10 @@
       <c r="AN38" s="36">
         <v>1</v>
       </c>
-      <c r="AP38" s="51" t="s">
+      <c r="AP38" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="AQ38" s="51"/>
+      <c r="AQ38" s="52"/>
       <c r="AR38" s="26">
         <v>0</v>
       </c>
@@ -3824,34 +3833,34 @@
       <c r="C39" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="52" t="s">
+      <c r="D39" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="52"/>
+      <c r="E39" s="53"/>
       <c r="F39" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="53" t="s">
+      <c r="I39" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="49"/>
-      <c r="S39" s="49"/>
-      <c r="T39" s="50"/>
-      <c r="U39" s="48" t="s">
+      <c r="J39" s="50"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="50"/>
+      <c r="Q39" s="50"/>
+      <c r="R39" s="50"/>
+      <c r="S39" s="50"/>
+      <c r="T39" s="51"/>
+      <c r="U39" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V39" s="49"/>
-      <c r="W39" s="49"/>
-      <c r="X39" s="49"/>
-      <c r="Y39" s="50"/>
+      <c r="V39" s="50"/>
+      <c r="W39" s="50"/>
+      <c r="X39" s="50"/>
+      <c r="Y39" s="51"/>
       <c r="Z39" s="16">
         <v>1</v>
       </c>
@@ -3861,13 +3870,13 @@
       <c r="AB39" s="18">
         <v>0</v>
       </c>
-      <c r="AC39" s="48" t="s">
+      <c r="AC39" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD39" s="49"/>
-      <c r="AE39" s="49"/>
-      <c r="AF39" s="49"/>
-      <c r="AG39" s="50"/>
+      <c r="AD39" s="50"/>
+      <c r="AE39" s="50"/>
+      <c r="AF39" s="50"/>
+      <c r="AG39" s="51"/>
       <c r="AH39" s="32">
         <v>0</v>
       </c>
@@ -3889,10 +3898,10 @@
       <c r="AN39" s="36">
         <v>1</v>
       </c>
-      <c r="AP39" s="51" t="s">
+      <c r="AP39" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="AQ39" s="51"/>
+      <c r="AQ39" s="52"/>
       <c r="AR39" s="26">
         <v>0</v>
       </c>
@@ -3931,34 +3940,34 @@
       <c r="C40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="52" t="s">
+      <c r="D40" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="52"/>
+      <c r="E40" s="53"/>
       <c r="F40" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I40" s="53" t="s">
+      <c r="I40" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="49"/>
-      <c r="O40" s="49"/>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="49"/>
-      <c r="R40" s="49"/>
-      <c r="S40" s="49"/>
-      <c r="T40" s="50"/>
-      <c r="U40" s="48" t="s">
+      <c r="J40" s="50"/>
+      <c r="K40" s="50"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="50"/>
+      <c r="P40" s="50"/>
+      <c r="Q40" s="50"/>
+      <c r="R40" s="50"/>
+      <c r="S40" s="50"/>
+      <c r="T40" s="51"/>
+      <c r="U40" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V40" s="49"/>
-      <c r="W40" s="49"/>
-      <c r="X40" s="49"/>
-      <c r="Y40" s="50"/>
+      <c r="V40" s="50"/>
+      <c r="W40" s="50"/>
+      <c r="X40" s="50"/>
+      <c r="Y40" s="51"/>
       <c r="Z40" s="16">
         <v>1</v>
       </c>
@@ -3968,13 +3977,13 @@
       <c r="AB40" s="18">
         <v>1</v>
       </c>
-      <c r="AC40" s="48" t="s">
+      <c r="AC40" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD40" s="49"/>
-      <c r="AE40" s="49"/>
-      <c r="AF40" s="49"/>
-      <c r="AG40" s="50"/>
+      <c r="AD40" s="50"/>
+      <c r="AE40" s="50"/>
+      <c r="AF40" s="50"/>
+      <c r="AG40" s="51"/>
       <c r="AH40" s="32">
         <v>0</v>
       </c>
@@ -3996,10 +4005,10 @@
       <c r="AN40" s="36">
         <v>1</v>
       </c>
-      <c r="AP40" s="51" t="s">
+      <c r="AP40" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="AQ40" s="51"/>
+      <c r="AQ40" s="52"/>
       <c r="AR40" s="26">
         <v>0</v>
       </c>
@@ -4038,10 +4047,10 @@
       <c r="C41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="52" t="s">
+      <c r="D41" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="E41" s="52"/>
+      <c r="E41" s="53"/>
       <c r="F41" s="12" t="s">
         <v>22</v>
       </c>
@@ -4066,20 +4075,20 @@
       <c r="O41" s="33">
         <v>0</v>
       </c>
-      <c r="P41" s="48" t="s">
+      <c r="P41" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
-      <c r="S41" s="49"/>
-      <c r="T41" s="50"/>
-      <c r="U41" s="49" t="s">
+      <c r="Q41" s="50"/>
+      <c r="R41" s="50"/>
+      <c r="S41" s="50"/>
+      <c r="T41" s="51"/>
+      <c r="U41" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V41" s="49"/>
-      <c r="W41" s="49"/>
-      <c r="X41" s="49"/>
-      <c r="Y41" s="50"/>
+      <c r="V41" s="50"/>
+      <c r="W41" s="50"/>
+      <c r="X41" s="50"/>
+      <c r="Y41" s="51"/>
       <c r="Z41" s="16">
         <v>0</v>
       </c>
@@ -4089,13 +4098,13 @@
       <c r="AB41" s="18">
         <v>1</v>
       </c>
-      <c r="AC41" s="48" t="s">
+      <c r="AC41" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD41" s="49"/>
-      <c r="AE41" s="49"/>
-      <c r="AF41" s="49"/>
-      <c r="AG41" s="50"/>
+      <c r="AD41" s="50"/>
+      <c r="AE41" s="50"/>
+      <c r="AF41" s="50"/>
+      <c r="AG41" s="51"/>
       <c r="AH41" s="32">
         <v>0</v>
       </c>
@@ -4117,10 +4126,10 @@
       <c r="AN41" s="36">
         <v>1</v>
       </c>
-      <c r="AP41" s="51" t="s">
+      <c r="AP41" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="AQ41" s="51"/>
+      <c r="AQ41" s="52"/>
       <c r="AR41" s="26">
         <v>0</v>
       </c>
@@ -4159,10 +4168,10 @@
       <c r="C42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="52" t="s">
+      <c r="D42" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="52"/>
+      <c r="E42" s="53"/>
       <c r="F42" s="12" t="s">
         <v>22</v>
       </c>
@@ -4187,20 +4196,20 @@
       <c r="O42" s="33">
         <v>0</v>
       </c>
-      <c r="P42" s="48" t="s">
+      <c r="P42" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="49"/>
-      <c r="S42" s="49"/>
-      <c r="T42" s="50"/>
-      <c r="U42" s="49" t="s">
+      <c r="Q42" s="50"/>
+      <c r="R42" s="50"/>
+      <c r="S42" s="50"/>
+      <c r="T42" s="51"/>
+      <c r="U42" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V42" s="49"/>
-      <c r="W42" s="49"/>
-      <c r="X42" s="49"/>
-      <c r="Y42" s="50"/>
+      <c r="V42" s="50"/>
+      <c r="W42" s="50"/>
+      <c r="X42" s="50"/>
+      <c r="Y42" s="51"/>
       <c r="Z42" s="16">
         <v>1</v>
       </c>
@@ -4210,13 +4219,13 @@
       <c r="AB42" s="18">
         <v>1</v>
       </c>
-      <c r="AC42" s="48" t="s">
+      <c r="AC42" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD42" s="49"/>
-      <c r="AE42" s="49"/>
-      <c r="AF42" s="49"/>
-      <c r="AG42" s="50"/>
+      <c r="AD42" s="50"/>
+      <c r="AE42" s="50"/>
+      <c r="AF42" s="50"/>
+      <c r="AG42" s="51"/>
       <c r="AH42" s="32">
         <v>0</v>
       </c>
@@ -4238,10 +4247,10 @@
       <c r="AN42" s="36">
         <v>1</v>
       </c>
-      <c r="AP42" s="51" t="s">
+      <c r="AP42" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="AQ42" s="51"/>
+      <c r="AQ42" s="52"/>
       <c r="AR42" s="26">
         <v>1</v>
       </c>
@@ -4280,10 +4289,10 @@
       <c r="C43" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="52" t="s">
+      <c r="D43" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="52"/>
+      <c r="E43" s="53"/>
       <c r="F43" s="12" t="s">
         <v>22</v>
       </c>
@@ -4308,20 +4317,20 @@
       <c r="O43" s="33">
         <v>0</v>
       </c>
-      <c r="P43" s="48" t="s">
+      <c r="P43" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="Q43" s="49"/>
-      <c r="R43" s="49"/>
-      <c r="S43" s="49"/>
-      <c r="T43" s="50"/>
-      <c r="U43" s="49" t="s">
+      <c r="Q43" s="50"/>
+      <c r="R43" s="50"/>
+      <c r="S43" s="50"/>
+      <c r="T43" s="51"/>
+      <c r="U43" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V43" s="49"/>
-      <c r="W43" s="49"/>
-      <c r="X43" s="49"/>
-      <c r="Y43" s="50"/>
+      <c r="V43" s="50"/>
+      <c r="W43" s="50"/>
+      <c r="X43" s="50"/>
+      <c r="Y43" s="51"/>
       <c r="Z43" s="16">
         <v>1</v>
       </c>
@@ -4331,13 +4340,13 @@
       <c r="AB43" s="18">
         <v>1</v>
       </c>
-      <c r="AC43" s="48" t="s">
+      <c r="AC43" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD43" s="49"/>
-      <c r="AE43" s="49"/>
-      <c r="AF43" s="49"/>
-      <c r="AG43" s="50"/>
+      <c r="AD43" s="50"/>
+      <c r="AE43" s="50"/>
+      <c r="AF43" s="50"/>
+      <c r="AG43" s="51"/>
       <c r="AH43" s="32">
         <v>0</v>
       </c>
@@ -4359,10 +4368,10 @@
       <c r="AN43" s="36">
         <v>1</v>
       </c>
-      <c r="AP43" s="51" t="s">
+      <c r="AP43" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="AQ43" s="51"/>
+      <c r="AQ43" s="52"/>
       <c r="AR43" s="26">
         <v>0</v>
       </c>
@@ -4401,34 +4410,34 @@
       <c r="C44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="52" t="s">
+      <c r="D44" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="52"/>
+      <c r="E44" s="53"/>
       <c r="F44" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I44" s="53" t="s">
+      <c r="I44" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J44" s="49"/>
-      <c r="K44" s="49"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="49"/>
-      <c r="O44" s="49"/>
-      <c r="P44" s="49"/>
-      <c r="Q44" s="49"/>
-      <c r="R44" s="49"/>
-      <c r="S44" s="49"/>
-      <c r="T44" s="50"/>
-      <c r="U44" s="48" t="s">
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+      <c r="R44" s="50"/>
+      <c r="S44" s="50"/>
+      <c r="T44" s="51"/>
+      <c r="U44" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V44" s="49"/>
-      <c r="W44" s="49"/>
-      <c r="X44" s="49"/>
-      <c r="Y44" s="50"/>
+      <c r="V44" s="50"/>
+      <c r="W44" s="50"/>
+      <c r="X44" s="50"/>
+      <c r="Y44" s="51"/>
       <c r="Z44" s="16">
         <v>0</v>
       </c>
@@ -4438,13 +4447,13 @@
       <c r="AB44" s="18">
         <v>0</v>
       </c>
-      <c r="AC44" s="48" t="s">
+      <c r="AC44" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD44" s="49"/>
-      <c r="AE44" s="49"/>
-      <c r="AF44" s="49"/>
-      <c r="AG44" s="50"/>
+      <c r="AD44" s="50"/>
+      <c r="AE44" s="50"/>
+      <c r="AF44" s="50"/>
+      <c r="AG44" s="51"/>
       <c r="AH44" s="32">
         <v>0</v>
       </c>
@@ -4466,10 +4475,10 @@
       <c r="AN44" s="36">
         <v>1</v>
       </c>
-      <c r="AP44" s="51" t="s">
+      <c r="AP44" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="AQ44" s="51"/>
+      <c r="AQ44" s="52"/>
       <c r="AR44" s="26">
         <v>0</v>
       </c>
@@ -4508,32 +4517,32 @@
       <c r="C45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="52" t="s">
+      <c r="D45" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="52"/>
+      <c r="E45" s="53"/>
       <c r="F45" s="12"/>
-      <c r="I45" s="53" t="s">
+      <c r="I45" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J45" s="49"/>
-      <c r="K45" s="49"/>
-      <c r="L45" s="49"/>
-      <c r="M45" s="49"/>
-      <c r="N45" s="49"/>
-      <c r="O45" s="49"/>
-      <c r="P45" s="49"/>
-      <c r="Q45" s="49"/>
-      <c r="R45" s="49"/>
-      <c r="S45" s="49"/>
-      <c r="T45" s="50"/>
-      <c r="U45" s="48" t="s">
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="50"/>
+      <c r="P45" s="50"/>
+      <c r="Q45" s="50"/>
+      <c r="R45" s="50"/>
+      <c r="S45" s="50"/>
+      <c r="T45" s="51"/>
+      <c r="U45" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V45" s="49"/>
-      <c r="W45" s="49"/>
-      <c r="X45" s="49"/>
-      <c r="Y45" s="50"/>
+      <c r="V45" s="50"/>
+      <c r="W45" s="50"/>
+      <c r="X45" s="50"/>
+      <c r="Y45" s="51"/>
       <c r="Z45" s="16">
         <v>0</v>
       </c>
@@ -4543,13 +4552,13 @@
       <c r="AB45" s="18">
         <v>1</v>
       </c>
-      <c r="AC45" s="48" t="s">
+      <c r="AC45" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD45" s="49"/>
-      <c r="AE45" s="49"/>
-      <c r="AF45" s="49"/>
-      <c r="AG45" s="50"/>
+      <c r="AD45" s="50"/>
+      <c r="AE45" s="50"/>
+      <c r="AF45" s="50"/>
+      <c r="AG45" s="51"/>
       <c r="AH45" s="32">
         <v>0</v>
       </c>
@@ -4571,11 +4580,11 @@
       <c r="AN45" s="36">
         <v>1</v>
       </c>
-      <c r="AP45" s="54" t="s">
+      <c r="AP45" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="AQ45" s="55"/>
-      <c r="AR45" s="46">
+      <c r="AQ45" s="56"/>
+      <c r="AR45" s="47">
         <v>1</v>
       </c>
       <c r="AS45" s="27">
@@ -4584,7 +4593,7 @@
       <c r="AT45" s="27">
         <v>0</v>
       </c>
-      <c r="AU45" s="47">
+      <c r="AU45" s="48">
         <v>1</v>
       </c>
       <c r="AW45" s="37">
@@ -4613,34 +4622,34 @@
       <c r="C46" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="52" t="s">
+      <c r="D46" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="E46" s="52"/>
+      <c r="E46" s="53"/>
       <c r="F46" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I46" s="53" t="s">
+      <c r="I46" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="49"/>
-      <c r="K46" s="49"/>
-      <c r="L46" s="49"/>
-      <c r="M46" s="49"/>
-      <c r="N46" s="49"/>
-      <c r="O46" s="49"/>
-      <c r="P46" s="49"/>
-      <c r="Q46" s="49"/>
-      <c r="R46" s="49"/>
-      <c r="S46" s="49"/>
-      <c r="T46" s="50"/>
-      <c r="U46" s="48" t="s">
+      <c r="J46" s="50"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="50"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="50"/>
+      <c r="R46" s="50"/>
+      <c r="S46" s="50"/>
+      <c r="T46" s="51"/>
+      <c r="U46" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V46" s="49"/>
-      <c r="W46" s="49"/>
-      <c r="X46" s="49"/>
-      <c r="Y46" s="50"/>
+      <c r="V46" s="50"/>
+      <c r="W46" s="50"/>
+      <c r="X46" s="50"/>
+      <c r="Y46" s="51"/>
       <c r="Z46" s="16">
         <v>0</v>
       </c>
@@ -4650,14 +4659,14 @@
       <c r="AB46" s="18">
         <v>0</v>
       </c>
-      <c r="AC46" s="48" t="s">
+      <c r="AC46" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD46" s="49"/>
-      <c r="AE46" s="49"/>
-      <c r="AF46" s="49"/>
-      <c r="AG46" s="50"/>
-      <c r="AH46" s="44">
+      <c r="AD46" s="50"/>
+      <c r="AE46" s="50"/>
+      <c r="AF46" s="50"/>
+      <c r="AG46" s="51"/>
+      <c r="AH46" s="45">
         <v>0</v>
       </c>
       <c r="AI46" s="43">
@@ -4675,14 +4684,14 @@
       <c r="AM46" s="43">
         <v>1</v>
       </c>
-      <c r="AN46" s="45">
-        <v>1</v>
-      </c>
-      <c r="AP46" s="51" t="s">
+      <c r="AN46" s="46">
+        <v>1</v>
+      </c>
+      <c r="AP46" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ46" s="51"/>
-      <c r="AR46" s="46">
+      <c r="AQ46" s="52"/>
+      <c r="AR46" s="47">
         <v>0</v>
       </c>
       <c r="AS46" s="27">
@@ -4691,7 +4700,7 @@
       <c r="AT46" s="27">
         <v>1</v>
       </c>
-      <c r="AU46" s="47">
+      <c r="AU46" s="48">
         <v>1</v>
       </c>
       <c r="AW46" s="42">
@@ -4720,34 +4729,34 @@
       <c r="C47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="52" t="s">
+      <c r="D47" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="E47" s="52"/>
+      <c r="E47" s="53"/>
       <c r="F47" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I47" s="53" t="s">
+      <c r="I47" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J47" s="49"/>
-      <c r="K47" s="49"/>
-      <c r="L47" s="49"/>
-      <c r="M47" s="49"/>
-      <c r="N47" s="49"/>
-      <c r="O47" s="49"/>
-      <c r="P47" s="49"/>
-      <c r="Q47" s="49"/>
-      <c r="R47" s="49"/>
-      <c r="S47" s="49"/>
-      <c r="T47" s="50"/>
-      <c r="U47" s="48" t="s">
+      <c r="J47" s="50"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="50"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="50"/>
+      <c r="P47" s="50"/>
+      <c r="Q47" s="50"/>
+      <c r="R47" s="50"/>
+      <c r="S47" s="50"/>
+      <c r="T47" s="51"/>
+      <c r="U47" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V47" s="49"/>
-      <c r="W47" s="49"/>
-      <c r="X47" s="49"/>
-      <c r="Y47" s="50"/>
+      <c r="V47" s="50"/>
+      <c r="W47" s="50"/>
+      <c r="X47" s="50"/>
+      <c r="Y47" s="51"/>
       <c r="Z47" s="16">
         <v>0</v>
       </c>
@@ -4757,14 +4766,14 @@
       <c r="AB47" s="18">
         <v>1</v>
       </c>
-      <c r="AC47" s="48" t="s">
+      <c r="AC47" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD47" s="49"/>
-      <c r="AE47" s="49"/>
-      <c r="AF47" s="49"/>
-      <c r="AG47" s="50"/>
-      <c r="AH47" s="44">
+      <c r="AD47" s="50"/>
+      <c r="AE47" s="50"/>
+      <c r="AF47" s="50"/>
+      <c r="AG47" s="51"/>
+      <c r="AH47" s="45">
         <v>0</v>
       </c>
       <c r="AI47" s="43">
@@ -4782,14 +4791,14 @@
       <c r="AM47" s="43">
         <v>1</v>
       </c>
-      <c r="AN47" s="45">
-        <v>1</v>
-      </c>
-      <c r="AP47" s="51" t="s">
+      <c r="AN47" s="46">
+        <v>1</v>
+      </c>
+      <c r="AP47" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ47" s="51"/>
-      <c r="AR47" s="46">
+      <c r="AQ47" s="52"/>
+      <c r="AR47" s="47">
         <v>0</v>
       </c>
       <c r="AS47" s="27">
@@ -4798,7 +4807,7 @@
       <c r="AT47" s="27">
         <v>1</v>
       </c>
-      <c r="AU47" s="47">
+      <c r="AU47" s="48">
         <v>1</v>
       </c>
       <c r="AW47" s="42">
@@ -4827,34 +4836,34 @@
       <c r="C48" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="52" t="s">
+      <c r="D48" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="E48" s="52"/>
+      <c r="E48" s="53"/>
       <c r="F48" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I48" s="53" t="s">
+      <c r="I48" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J48" s="49"/>
-      <c r="K48" s="49"/>
-      <c r="L48" s="49"/>
-      <c r="M48" s="49"/>
-      <c r="N48" s="49"/>
-      <c r="O48" s="49"/>
-      <c r="P48" s="49"/>
-      <c r="Q48" s="49"/>
-      <c r="R48" s="49"/>
-      <c r="S48" s="49"/>
-      <c r="T48" s="50"/>
-      <c r="U48" s="48" t="s">
+      <c r="J48" s="50"/>
+      <c r="K48" s="50"/>
+      <c r="L48" s="50"/>
+      <c r="M48" s="50"/>
+      <c r="N48" s="50"/>
+      <c r="O48" s="50"/>
+      <c r="P48" s="50"/>
+      <c r="Q48" s="50"/>
+      <c r="R48" s="50"/>
+      <c r="S48" s="50"/>
+      <c r="T48" s="51"/>
+      <c r="U48" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V48" s="49"/>
-      <c r="W48" s="49"/>
-      <c r="X48" s="49"/>
-      <c r="Y48" s="50"/>
+      <c r="V48" s="50"/>
+      <c r="W48" s="50"/>
+      <c r="X48" s="50"/>
+      <c r="Y48" s="51"/>
       <c r="Z48" s="16">
         <v>0</v>
       </c>
@@ -4864,13 +4873,13 @@
       <c r="AB48" s="18">
         <v>0</v>
       </c>
-      <c r="AC48" s="48" t="s">
+      <c r="AC48" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD48" s="49"/>
-      <c r="AE48" s="49"/>
-      <c r="AF48" s="49"/>
-      <c r="AG48" s="50"/>
+      <c r="AD48" s="50"/>
+      <c r="AE48" s="50"/>
+      <c r="AF48" s="50"/>
+      <c r="AG48" s="51"/>
       <c r="AH48" s="8">
         <v>0</v>
       </c>
@@ -4892,10 +4901,10 @@
       <c r="AN48" s="15">
         <v>1</v>
       </c>
-      <c r="AP48" s="51" t="s">
+      <c r="AP48" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ48" s="51"/>
+      <c r="AQ48" s="52"/>
       <c r="AR48" s="26">
         <v>0</v>
       </c>
@@ -4934,34 +4943,34 @@
       <c r="C49" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D49" s="52" t="s">
+      <c r="D49" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="52"/>
+      <c r="E49" s="53"/>
       <c r="F49" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I49" s="53" t="s">
+      <c r="I49" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J49" s="49"/>
-      <c r="K49" s="49"/>
-      <c r="L49" s="49"/>
-      <c r="M49" s="49"/>
-      <c r="N49" s="49"/>
-      <c r="O49" s="49"/>
-      <c r="P49" s="49"/>
-      <c r="Q49" s="49"/>
-      <c r="R49" s="49"/>
-      <c r="S49" s="49"/>
-      <c r="T49" s="50"/>
-      <c r="U49" s="48" t="s">
+      <c r="J49" s="50"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="50"/>
+      <c r="M49" s="50"/>
+      <c r="N49" s="50"/>
+      <c r="O49" s="50"/>
+      <c r="P49" s="50"/>
+      <c r="Q49" s="50"/>
+      <c r="R49" s="50"/>
+      <c r="S49" s="50"/>
+      <c r="T49" s="51"/>
+      <c r="U49" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V49" s="49"/>
-      <c r="W49" s="49"/>
-      <c r="X49" s="49"/>
-      <c r="Y49" s="50"/>
+      <c r="V49" s="50"/>
+      <c r="W49" s="50"/>
+      <c r="X49" s="50"/>
+      <c r="Y49" s="51"/>
       <c r="Z49" s="16">
         <v>1</v>
       </c>
@@ -4971,14 +4980,14 @@
       <c r="AB49" s="18">
         <v>0</v>
       </c>
-      <c r="AC49" s="48" t="s">
+      <c r="AC49" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD49" s="49"/>
-      <c r="AE49" s="49"/>
-      <c r="AF49" s="49"/>
-      <c r="AG49" s="50"/>
-      <c r="AH49" s="44">
+      <c r="AD49" s="50"/>
+      <c r="AE49" s="50"/>
+      <c r="AF49" s="50"/>
+      <c r="AG49" s="51"/>
+      <c r="AH49" s="45">
         <v>0</v>
       </c>
       <c r="AI49" s="43">
@@ -4996,14 +5005,14 @@
       <c r="AM49" s="43">
         <v>1</v>
       </c>
-      <c r="AN49" s="45">
-        <v>1</v>
-      </c>
-      <c r="AP49" s="51" t="s">
+      <c r="AN49" s="46">
+        <v>1</v>
+      </c>
+      <c r="AP49" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ49" s="51"/>
-      <c r="AR49" s="46">
+      <c r="AQ49" s="52"/>
+      <c r="AR49" s="47">
         <v>0</v>
       </c>
       <c r="AS49" s="27">
@@ -5012,7 +5021,7 @@
       <c r="AT49" s="27">
         <v>1</v>
       </c>
-      <c r="AU49" s="47">
+      <c r="AU49" s="48">
         <v>1</v>
       </c>
       <c r="AW49" s="42">
@@ -5041,34 +5050,34 @@
       <c r="C50" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="52" t="s">
+      <c r="D50" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="E50" s="52"/>
+      <c r="E50" s="53"/>
       <c r="F50" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I50" s="53" t="s">
+      <c r="I50" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="49"/>
-      <c r="N50" s="49"/>
-      <c r="O50" s="49"/>
-      <c r="P50" s="49"/>
-      <c r="Q50" s="49"/>
-      <c r="R50" s="49"/>
-      <c r="S50" s="49"/>
-      <c r="T50" s="50"/>
-      <c r="U50" s="48" t="s">
+      <c r="J50" s="50"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="50"/>
+      <c r="M50" s="50"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="50"/>
+      <c r="P50" s="50"/>
+      <c r="Q50" s="50"/>
+      <c r="R50" s="50"/>
+      <c r="S50" s="50"/>
+      <c r="T50" s="51"/>
+      <c r="U50" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V50" s="49"/>
-      <c r="W50" s="49"/>
-      <c r="X50" s="49"/>
-      <c r="Y50" s="50"/>
+      <c r="V50" s="50"/>
+      <c r="W50" s="50"/>
+      <c r="X50" s="50"/>
+      <c r="Y50" s="51"/>
       <c r="Z50" s="16">
         <v>1</v>
       </c>
@@ -5078,14 +5087,14 @@
       <c r="AB50" s="18">
         <v>1</v>
       </c>
-      <c r="AC50" s="48" t="s">
+      <c r="AC50" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD50" s="49"/>
-      <c r="AE50" s="49"/>
-      <c r="AF50" s="49"/>
-      <c r="AG50" s="50"/>
-      <c r="AH50" s="44">
+      <c r="AD50" s="50"/>
+      <c r="AE50" s="50"/>
+      <c r="AF50" s="50"/>
+      <c r="AG50" s="51"/>
+      <c r="AH50" s="45">
         <v>0</v>
       </c>
       <c r="AI50" s="43">
@@ -5103,14 +5112,14 @@
       <c r="AM50" s="43">
         <v>1</v>
       </c>
-      <c r="AN50" s="45">
-        <v>1</v>
-      </c>
-      <c r="AP50" s="51" t="s">
+      <c r="AN50" s="46">
+        <v>1</v>
+      </c>
+      <c r="AP50" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ50" s="51"/>
-      <c r="AR50" s="46">
+      <c r="AQ50" s="52"/>
+      <c r="AR50" s="47">
         <v>0</v>
       </c>
       <c r="AS50" s="27">
@@ -5119,7 +5128,7 @@
       <c r="AT50" s="27">
         <v>1</v>
       </c>
-      <c r="AU50" s="47">
+      <c r="AU50" s="48">
         <v>1</v>
       </c>
       <c r="AW50" s="42">
@@ -5148,34 +5157,34 @@
       <c r="C51" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="52" t="s">
+      <c r="D51" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="E51" s="52"/>
+      <c r="E51" s="53"/>
       <c r="F51" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I51" s="53" t="s">
+      <c r="I51" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J51" s="49"/>
-      <c r="K51" s="49"/>
-      <c r="L51" s="49"/>
-      <c r="M51" s="49"/>
-      <c r="N51" s="49"/>
-      <c r="O51" s="49"/>
-      <c r="P51" s="49"/>
-      <c r="Q51" s="49"/>
-      <c r="R51" s="49"/>
-      <c r="S51" s="49"/>
-      <c r="T51" s="50"/>
-      <c r="U51" s="48" t="s">
+      <c r="J51" s="50"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="50"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="50"/>
+      <c r="P51" s="50"/>
+      <c r="Q51" s="50"/>
+      <c r="R51" s="50"/>
+      <c r="S51" s="50"/>
+      <c r="T51" s="51"/>
+      <c r="U51" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V51" s="49"/>
-      <c r="W51" s="49"/>
-      <c r="X51" s="49"/>
-      <c r="Y51" s="50"/>
+      <c r="V51" s="50"/>
+      <c r="W51" s="50"/>
+      <c r="X51" s="50"/>
+      <c r="Y51" s="51"/>
       <c r="Z51" s="16">
         <v>0</v>
       </c>
@@ -5185,14 +5194,14 @@
       <c r="AB51" s="18">
         <v>0</v>
       </c>
-      <c r="AC51" s="48" t="s">
+      <c r="AC51" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="AD51" s="49"/>
-      <c r="AE51" s="49"/>
-      <c r="AF51" s="49"/>
-      <c r="AG51" s="50"/>
-      <c r="AH51" s="44">
+      <c r="AD51" s="50"/>
+      <c r="AE51" s="50"/>
+      <c r="AF51" s="50"/>
+      <c r="AG51" s="51"/>
+      <c r="AH51" s="45">
         <v>1</v>
       </c>
       <c r="AI51" s="43">
@@ -5210,14 +5219,14 @@
       <c r="AM51" s="43">
         <v>1</v>
       </c>
-      <c r="AN51" s="45">
-        <v>1</v>
-      </c>
-      <c r="AP51" s="51" t="s">
+      <c r="AN51" s="46">
+        <v>1</v>
+      </c>
+      <c r="AP51" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ51" s="51"/>
-      <c r="AR51" s="46">
+      <c r="AQ51" s="52"/>
+      <c r="AR51" s="47">
         <v>0</v>
       </c>
       <c r="AS51" s="27">
@@ -5226,7 +5235,7 @@
       <c r="AT51" s="27">
         <v>1</v>
       </c>
-      <c r="AU51" s="47">
+      <c r="AU51" s="48">
         <v>1</v>
       </c>
       <c r="AW51" s="42">
@@ -5244,89 +5253,89 @@
       <c r="BA51" s="42">
         <v>1</v>
       </c>
-      <c r="BB51" s="79" t="s">
+      <c r="BB51" s="80" t="s">
         <v>56</v>
       </c>
       <c r="BC51" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:55" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="E52" s="52"/>
+      <c r="D52" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" s="53"/>
       <c r="F52" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="53" t="s">
+      <c r="I52" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J52" s="49"/>
-      <c r="K52" s="49"/>
-      <c r="L52" s="49"/>
-      <c r="M52" s="49"/>
-      <c r="N52" s="49"/>
-      <c r="O52" s="50"/>
-      <c r="P52" s="48" t="s">
+      <c r="J52" s="50"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="50"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="50"/>
+      <c r="O52" s="51"/>
+      <c r="P52" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q52" s="49"/>
-      <c r="R52" s="49"/>
-      <c r="S52" s="49"/>
-      <c r="T52" s="50"/>
-      <c r="U52" s="48" t="s">
+      <c r="Q52" s="50"/>
+      <c r="R52" s="50"/>
+      <c r="S52" s="50"/>
+      <c r="T52" s="51"/>
+      <c r="U52" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V52" s="49"/>
-      <c r="W52" s="49"/>
-      <c r="X52" s="49"/>
-      <c r="Y52" s="50"/>
-      <c r="Z52" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA52" s="9">
-        <v>1</v>
-      </c>
-      <c r="AB52" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC52" s="48" t="s">
+      <c r="V52" s="50"/>
+      <c r="W52" s="50"/>
+      <c r="X52" s="50"/>
+      <c r="Y52" s="51"/>
+      <c r="Z52" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA52" s="43">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="44">
+        <v>1</v>
+      </c>
+      <c r="AC52" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="AD52" s="49"/>
-      <c r="AE52" s="49"/>
-      <c r="AF52" s="49"/>
-      <c r="AG52" s="50"/>
-      <c r="AH52" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI52" s="9">
-        <v>1</v>
-      </c>
-      <c r="AJ52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM52" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN52" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP52" s="51" t="s">
+      <c r="AD52" s="50"/>
+      <c r="AE52" s="50"/>
+      <c r="AF52" s="50"/>
+      <c r="AG52" s="51"/>
+      <c r="AH52" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI52" s="43">
+        <v>1</v>
+      </c>
+      <c r="AJ52" s="43">
+        <v>0</v>
+      </c>
+      <c r="AK52" s="43">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="43">
+        <v>0</v>
+      </c>
+      <c r="AM52" s="43">
+        <v>1</v>
+      </c>
+      <c r="AN52" s="46">
+        <v>1</v>
+      </c>
+      <c r="AP52" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ52" s="51"/>
-      <c r="AR52" s="26">
+      <c r="AQ52" s="52"/>
+      <c r="AR52" s="47">
         <v>0</v>
       </c>
       <c r="AS52" s="27">
@@ -5335,19 +5344,19 @@
       <c r="AT52" s="27">
         <v>1</v>
       </c>
-      <c r="AU52" s="28">
-        <v>1</v>
-      </c>
-      <c r="AW52" s="37">
-        <v>1</v>
-      </c>
-      <c r="AX52" s="37">
-        <v>0</v>
-      </c>
-      <c r="AY52" s="37">
-        <v>1</v>
-      </c>
-      <c r="AZ52" s="37">
+      <c r="AU52" s="48">
+        <v>1</v>
+      </c>
+      <c r="AW52" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX52" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY52" s="42">
+        <v>1</v>
+      </c>
+      <c r="AZ52" s="42">
         <v>1</v>
       </c>
       <c r="BA52" s="42">
@@ -5356,165 +5365,171 @@
       <c r="BB52" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC52" s="37" t="s">
+      <c r="BC52" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="52"/>
-      <c r="F53" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J53" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K53" s="49"/>
-      <c r="L53" s="49"/>
-      <c r="M53" s="49"/>
-      <c r="N53" s="49"/>
-      <c r="O53" s="50"/>
-      <c r="P53" s="48" t="s">
+    <row r="53" spans="3:55" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="E53" s="53"/>
+      <c r="F53" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I53" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="J53" s="50"/>
+      <c r="K53" s="50"/>
+      <c r="L53" s="50"/>
+      <c r="M53" s="50"/>
+      <c r="N53" s="50"/>
+      <c r="O53" s="51"/>
+      <c r="P53" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="Q53" s="49"/>
-      <c r="R53" s="49"/>
-      <c r="S53" s="49"/>
-      <c r="T53" s="50"/>
-      <c r="U53" s="48" t="s">
+      <c r="Q53" s="50"/>
+      <c r="R53" s="50"/>
+      <c r="S53" s="50"/>
+      <c r="T53" s="51"/>
+      <c r="U53" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="V53" s="49"/>
-      <c r="W53" s="49"/>
-      <c r="X53" s="49"/>
-      <c r="Y53" s="50"/>
-      <c r="Z53" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB53" s="10">
-        <v>0</v>
-      </c>
-      <c r="AC53" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD53" s="49"/>
-      <c r="AE53" s="49"/>
+      <c r="V53" s="50"/>
+      <c r="W53" s="50"/>
+      <c r="X53" s="50"/>
+      <c r="Y53" s="51"/>
+      <c r="Z53" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="43">
+        <v>1</v>
+      </c>
+      <c r="AB53" s="44">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD53" s="50"/>
+      <c r="AE53" s="50"/>
       <c r="AF53" s="50"/>
-      <c r="AG53" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH53" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI53" s="9">
-        <v>1</v>
-      </c>
-      <c r="AJ53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AM53" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN53" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP53" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="AQ53" s="51"/>
-      <c r="AR53" s="26">
+      <c r="AG53" s="51"/>
+      <c r="AH53" s="45">
+        <v>0</v>
+      </c>
+      <c r="AI53" s="43">
+        <v>1</v>
+      </c>
+      <c r="AJ53" s="43">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="43">
+        <v>0</v>
+      </c>
+      <c r="AL53" s="43">
+        <v>0</v>
+      </c>
+      <c r="AM53" s="43">
+        <v>1</v>
+      </c>
+      <c r="AN53" s="46">
+        <v>1</v>
+      </c>
+      <c r="AP53" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ53" s="52"/>
+      <c r="AR53" s="47">
         <v>0</v>
       </c>
       <c r="AS53" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT53" s="27">
-        <v>0</v>
-      </c>
-      <c r="AU53" s="28">
-        <v>0</v>
-      </c>
-      <c r="AW53" s="37">
-        <v>1</v>
-      </c>
-      <c r="AX53" s="37">
-        <v>0</v>
-      </c>
-      <c r="AY53" s="37">
-        <v>0</v>
-      </c>
-      <c r="AZ53" s="37">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AU53" s="48">
+        <v>1</v>
+      </c>
+      <c r="AW53" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX53" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY53" s="42">
+        <v>1</v>
+      </c>
+      <c r="AZ53" s="42">
+        <v>1</v>
       </c>
       <c r="BA53" s="42">
         <v>0</v>
       </c>
-      <c r="BB53" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC53" s="37" t="s">
-        <v>51</v>
+      <c r="BB53" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="BC53" s="42" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="E54" s="52"/>
-      <c r="F54" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="I54" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J54" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="K54" s="49"/>
-      <c r="L54" s="49"/>
-      <c r="M54" s="49"/>
-      <c r="N54" s="49"/>
-      <c r="O54" s="49"/>
-      <c r="P54" s="49"/>
-      <c r="Q54" s="49"/>
-      <c r="R54" s="49"/>
-      <c r="S54" s="49"/>
-      <c r="T54" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="U54" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="V54" s="49"/>
-      <c r="W54" s="49"/>
-      <c r="X54" s="49"/>
-      <c r="Y54" s="49"/>
-      <c r="Z54" s="49"/>
-      <c r="AA54" s="49"/>
-      <c r="AB54" s="50"/>
-      <c r="AC54" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD54" s="49"/>
-      <c r="AE54" s="49"/>
-      <c r="AF54" s="49"/>
-      <c r="AG54" s="50"/>
+      <c r="C54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="53"/>
+      <c r="F54" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I54" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="J54" s="50"/>
+      <c r="K54" s="50"/>
+      <c r="L54" s="50"/>
+      <c r="M54" s="50"/>
+      <c r="N54" s="50"/>
+      <c r="O54" s="51"/>
+      <c r="P54" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q54" s="50"/>
+      <c r="R54" s="50"/>
+      <c r="S54" s="50"/>
+      <c r="T54" s="51"/>
+      <c r="U54" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="V54" s="50"/>
+      <c r="W54" s="50"/>
+      <c r="X54" s="50"/>
+      <c r="Y54" s="51"/>
+      <c r="Z54" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA54" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB54" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD54" s="50"/>
+      <c r="AE54" s="50"/>
+      <c r="AF54" s="50"/>
+      <c r="AG54" s="51"/>
       <c r="AH54" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI54" s="9">
         <v>1</v>
@@ -5523,10 +5538,10 @@
         <v>0</v>
       </c>
       <c r="AK54" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL54" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM54" s="9">
         <v>1</v>
@@ -5534,10 +5549,10 @@
       <c r="AN54" s="15">
         <v>1</v>
       </c>
-      <c r="AP54" s="51" t="s">
+      <c r="AP54" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="AQ54" s="51"/>
+      <c r="AQ54" s="52"/>
       <c r="AR54" s="26">
         <v>0</v>
       </c>
@@ -5551,29 +5566,248 @@
         <v>1</v>
       </c>
       <c r="AW54" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX54" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY54" s="37">
         <v>1</v>
       </c>
       <c r="AZ54" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA54" s="42">
         <v>0</v>
       </c>
-      <c r="BB54" s="41" t="s">
-        <v>56</v>
+      <c r="BB54" s="40" t="s">
+        <v>54</v>
       </c>
       <c r="BC54" s="37" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="55" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" s="53"/>
+      <c r="F55" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J55" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="K55" s="50"/>
+      <c r="L55" s="50"/>
+      <c r="M55" s="50"/>
+      <c r="N55" s="50"/>
+      <c r="O55" s="51"/>
+      <c r="P55" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q55" s="50"/>
+      <c r="R55" s="50"/>
+      <c r="S55" s="50"/>
+      <c r="T55" s="51"/>
+      <c r="U55" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="V55" s="50"/>
+      <c r="W55" s="50"/>
+      <c r="X55" s="50"/>
+      <c r="Y55" s="51"/>
+      <c r="Z55" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA55" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB55" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC55" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD55" s="50"/>
+      <c r="AE55" s="50"/>
+      <c r="AF55" s="51"/>
+      <c r="AG55" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH55" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI55" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ55" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK55" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL55" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM55" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN55" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP55" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ55" s="52"/>
+      <c r="AR55" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS55" s="27">
+        <v>1</v>
+      </c>
+      <c r="AT55" s="27">
+        <v>0</v>
+      </c>
+      <c r="AU55" s="28">
+        <v>0</v>
+      </c>
+      <c r="AW55" s="37">
+        <v>1</v>
+      </c>
+      <c r="AX55" s="37">
+        <v>0</v>
+      </c>
+      <c r="AY55" s="37">
+        <v>0</v>
+      </c>
+      <c r="AZ55" s="37">
+        <v>0</v>
+      </c>
+      <c r="BA55" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB55" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC55" s="37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" s="53"/>
+      <c r="F56" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="K56" s="50"/>
+      <c r="L56" s="50"/>
+      <c r="M56" s="50"/>
+      <c r="N56" s="50"/>
+      <c r="O56" s="50"/>
+      <c r="P56" s="50"/>
+      <c r="Q56" s="50"/>
+      <c r="R56" s="50"/>
+      <c r="S56" s="50"/>
+      <c r="T56" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="U56" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="V56" s="50"/>
+      <c r="W56" s="50"/>
+      <c r="X56" s="50"/>
+      <c r="Y56" s="50"/>
+      <c r="Z56" s="50"/>
+      <c r="AA56" s="50"/>
+      <c r="AB56" s="51"/>
+      <c r="AC56" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD56" s="50"/>
+      <c r="AE56" s="50"/>
+      <c r="AF56" s="50"/>
+      <c r="AG56" s="51"/>
+      <c r="AH56" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI56" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ56" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK56" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL56" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM56" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN56" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP56" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ56" s="52"/>
+      <c r="AR56" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS56" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT56" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU56" s="28">
+        <v>1</v>
+      </c>
+      <c r="AW56" s="37">
+        <v>0</v>
+      </c>
+      <c r="AX56" s="37">
+        <v>1</v>
+      </c>
+      <c r="AY56" s="37">
+        <v>1</v>
+      </c>
+      <c r="AZ56" s="37">
+        <v>0</v>
+      </c>
+      <c r="BA56" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB56" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC56" s="37" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="191">
+  <mergeCells count="203">
+    <mergeCell ref="AP53:AQ53"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="I52:O52"/>
+    <mergeCell ref="P52:T52"/>
+    <mergeCell ref="U52:Y52"/>
+    <mergeCell ref="AC52:AG52"/>
+    <mergeCell ref="AP52:AQ52"/>
     <mergeCell ref="AP50:AQ50"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="I49:T49"/>
@@ -5596,9 +5830,9 @@
     <mergeCell ref="AP12:AQ12"/>
     <mergeCell ref="AP47:AQ47"/>
     <mergeCell ref="AP46:AQ46"/>
-    <mergeCell ref="AP52:AQ52"/>
-    <mergeCell ref="AP53:AQ53"/>
     <mergeCell ref="AP54:AQ54"/>
+    <mergeCell ref="AP55:AQ55"/>
+    <mergeCell ref="AP56:AQ56"/>
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="I8:O8"/>
     <mergeCell ref="P8:T8"/>
@@ -5668,7 +5902,7 @@
     <mergeCell ref="U28:Y28"/>
     <mergeCell ref="AC28:AG28"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D54:E54"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="I37:T37"/>
     <mergeCell ref="AC48:AG48"/>
@@ -5676,21 +5910,26 @@
     <mergeCell ref="I50:T50"/>
     <mergeCell ref="U50:Y50"/>
     <mergeCell ref="AC50:AG50"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="J54:S54"/>
-    <mergeCell ref="U54:AB54"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="I53:O53"/>
+    <mergeCell ref="P53:T53"/>
+    <mergeCell ref="U53:Y53"/>
+    <mergeCell ref="AC53:AG53"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="J56:S56"/>
+    <mergeCell ref="U56:AB56"/>
+    <mergeCell ref="AC56:AG56"/>
+    <mergeCell ref="I54:O54"/>
+    <mergeCell ref="P54:T54"/>
+    <mergeCell ref="U54:Y54"/>
     <mergeCell ref="AC54:AG54"/>
-    <mergeCell ref="I52:O52"/>
-    <mergeCell ref="P52:T52"/>
-    <mergeCell ref="U52:Y52"/>
-    <mergeCell ref="AC52:AG52"/>
     <mergeCell ref="I48:T48"/>
     <mergeCell ref="U48:Y48"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="P53:T53"/>
-    <mergeCell ref="U53:Y53"/>
-    <mergeCell ref="AC53:AF53"/>
-    <mergeCell ref="J53:O53"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="P55:T55"/>
+    <mergeCell ref="U55:Y55"/>
+    <mergeCell ref="AC55:AF55"/>
+    <mergeCell ref="J55:O55"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>

</xml_diff>

<commit_message>
added support for remaining B-Type instructions
</commit_message>
<xml_diff>
--- a/doc/decoding.xlsx
+++ b/doc/decoding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\SystemVerilog\FRiscV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD699D2-16BE-4546-AF92-23461508F52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA0ABE4-8DF5-4029-9845-00B393702DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29490" yWindow="1470" windowWidth="25965" windowHeight="14595" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
+    <workbookView xWindow="29205" yWindow="345" windowWidth="25965" windowHeight="14595" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,132 @@
         </r>
       </text>
     </comment>
-    <comment ref="D56" authorId="0" shapeId="0" xr:uid="{94E066D9-6740-478B-B1BE-00F56432855D}">
+    <comment ref="AW56" authorId="0" shapeId="0" xr:uid="{382EB2A2-9478-484D-8E75-908CA6135CC7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+if zero is 0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AW57" authorId="0" shapeId="0" xr:uid="{AF4AAD74-A0B1-4954-A93A-9B8D31C070C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+if lt is 1
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AW58" authorId="0" shapeId="0" xr:uid="{E14295BE-F230-4CBB-A96B-55B262588A8A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+if lt is 0 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AW59" authorId="0" shapeId="0" xr:uid="{D03D084B-C9A1-48B8-B35B-E6623C5F5D6D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+if lt is 1
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AW60" authorId="0" shapeId="0" xr:uid="{C250F179-A726-4849-B658-A37C0F1074CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+if lt is 0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D61" authorId="0" shapeId="0" xr:uid="{94E066D9-6740-478B-B1BE-00F56432855D}">
       <text>
         <r>
           <rPr>
@@ -118,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="83">
   <si>
     <t>R-TYPE</t>
   </si>
@@ -349,6 +474,24 @@
   </si>
   <si>
     <t>SH</t>
+  </si>
+  <si>
+    <t>BNE</t>
+  </si>
+  <si>
+    <t>BLT</t>
+  </si>
+  <si>
+    <t>BGE</t>
+  </si>
+  <si>
+    <t>BLTU</t>
+  </si>
+  <si>
+    <t>BGEU</t>
+  </si>
+  <si>
+    <t>Uses  LT?</t>
   </si>
 </sst>
 </file>
@@ -454,7 +597,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -637,15 +780,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -757,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -881,6 +1015,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -959,9 +1096,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -971,10 +1105,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -983,13 +1117,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1309,13 +1440,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA95D64-5055-4174-A4D5-0BDBECB18FB0}">
-  <dimension ref="C1:BC56"/>
+  <dimension ref="C1:BD61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="7" ySplit="23" topLeftCell="H36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="23" topLeftCell="H45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="C54" sqref="C54"/>
+      <selection pane="bottomRight" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -1336,25 +1467,26 @@
     <col min="53" max="53" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="56" max="16384" width="4.7109375" style="3"/>
+    <col min="56" max="56" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="16384" width="4.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:47" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP2" s="70" t="s">
+      <c r="AP2" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="AQ2" s="71"/>
-      <c r="AR2" s="71"/>
-      <c r="AS2" s="71"/>
-      <c r="AT2" s="71"/>
-      <c r="AU2" s="72"/>
+      <c r="AQ2" s="70"/>
+      <c r="AR2" s="70"/>
+      <c r="AS2" s="70"/>
+      <c r="AT2" s="70"/>
+      <c r="AU2" s="71"/>
     </row>
     <row r="3" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP3" s="73" t="s">
+      <c r="AP3" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="58"/>
+      <c r="AQ3" s="59"/>
       <c r="AR3" s="21">
         <v>0</v>
       </c>
@@ -1364,15 +1496,15 @@
       <c r="AT3" s="21">
         <v>0</v>
       </c>
-      <c r="AU3" s="74">
+      <c r="AU3" s="73">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="4:47" ht="15" x14ac:dyDescent="0.2">
-      <c r="AP4" s="75" t="s">
+      <c r="AP4" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="AQ4" s="57"/>
+      <c r="AQ4" s="58"/>
       <c r="AR4" s="21">
         <v>0</v>
       </c>
@@ -1382,7 +1514,7 @@
       <c r="AT4" s="21">
         <v>0</v>
       </c>
-      <c r="AU4" s="74">
+      <c r="AU4" s="73">
         <v>1</v>
       </c>
     </row>
@@ -1483,10 +1615,10 @@
       <c r="AN5" s="2">
         <v>0</v>
       </c>
-      <c r="AP5" s="75" t="s">
+      <c r="AP5" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="AQ5" s="57"/>
+      <c r="AQ5" s="58"/>
       <c r="AR5" s="21">
         <v>0</v>
       </c>
@@ -1496,7 +1628,7 @@
       <c r="AT5" s="21">
         <v>1</v>
       </c>
-      <c r="AU5" s="74">
+      <c r="AU5" s="73">
         <v>0</v>
       </c>
     </row>
@@ -1533,10 +1665,10 @@
       <c r="AL6" s="2"/>
       <c r="AM6" s="2"/>
       <c r="AN6" s="2"/>
-      <c r="AP6" s="75" t="s">
+      <c r="AP6" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="AQ6" s="57"/>
+      <c r="AQ6" s="58"/>
       <c r="AR6" s="21">
         <v>0</v>
       </c>
@@ -1546,7 +1678,7 @@
       <c r="AT6" s="21">
         <v>1</v>
       </c>
-      <c r="AU6" s="74">
+      <c r="AU6" s="73">
         <v>1</v>
       </c>
     </row>
@@ -1587,10 +1719,10 @@
       <c r="AN7" s="3">
         <v>0</v>
       </c>
-      <c r="AP7" s="75" t="s">
+      <c r="AP7" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="AQ7" s="57"/>
+      <c r="AQ7" s="58"/>
       <c r="AR7" s="21">
         <v>0</v>
       </c>
@@ -1600,65 +1732,65 @@
       <c r="AT7" s="21">
         <v>0</v>
       </c>
-      <c r="AU7" s="74">
+      <c r="AU7" s="73">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="I8" s="54" t="s">
+      <c r="D8" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="I8" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="49" t="s">
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="49" t="s">
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V8" s="50"/>
-      <c r="W8" s="50"/>
-      <c r="X8" s="50"/>
-      <c r="Y8" s="51"/>
-      <c r="Z8" s="49" t="s">
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="51"/>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="50"/>
-      <c r="AB8" s="51"/>
-      <c r="AC8" s="49" t="s">
+      <c r="AA8" s="51"/>
+      <c r="AB8" s="52"/>
+      <c r="AC8" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD8" s="50"/>
-      <c r="AE8" s="50"/>
-      <c r="AF8" s="50"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="49" t="s">
+      <c r="AD8" s="51"/>
+      <c r="AE8" s="51"/>
+      <c r="AF8" s="51"/>
+      <c r="AG8" s="52"/>
+      <c r="AH8" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AI8" s="50"/>
-      <c r="AJ8" s="50"/>
-      <c r="AK8" s="50"/>
-      <c r="AL8" s="50"/>
-      <c r="AM8" s="50"/>
-      <c r="AN8" s="61"/>
-      <c r="AP8" s="75" t="s">
+      <c r="AI8" s="51"/>
+      <c r="AJ8" s="51"/>
+      <c r="AK8" s="51"/>
+      <c r="AL8" s="51"/>
+      <c r="AM8" s="51"/>
+      <c r="AN8" s="62"/>
+      <c r="AP8" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="AQ8" s="57"/>
+      <c r="AQ8" s="58"/>
       <c r="AR8" s="21">
         <v>0</v>
       </c>
@@ -1668,7 +1800,7 @@
       <c r="AT8" s="21">
         <v>0</v>
       </c>
-      <c r="AU8" s="74">
+      <c r="AU8" s="73">
         <v>1</v>
       </c>
     </row>
@@ -1709,10 +1841,10 @@
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
-      <c r="AP9" s="75" t="s">
+      <c r="AP9" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="AQ9" s="57"/>
+      <c r="AQ9" s="58"/>
       <c r="AR9" s="21">
         <v>0</v>
       </c>
@@ -1722,7 +1854,7 @@
       <c r="AT9" s="21">
         <v>1</v>
       </c>
-      <c r="AU9" s="74">
+      <c r="AU9" s="73">
         <v>0</v>
       </c>
     </row>
@@ -1761,10 +1893,10 @@
       <c r="AN10" s="3">
         <v>0</v>
       </c>
-      <c r="AP10" s="75" t="s">
+      <c r="AP10" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="AQ10" s="57"/>
+      <c r="AQ10" s="58"/>
       <c r="AR10" s="21">
         <v>0</v>
       </c>
@@ -1774,77 +1906,77 @@
       <c r="AT10" s="21">
         <v>1</v>
       </c>
-      <c r="AU10" s="74">
+      <c r="AU10" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="I11" s="54" t="s">
+      <c r="D11" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="I11" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="50"/>
-      <c r="T11" s="51"/>
-      <c r="U11" s="49" t="s">
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="52"/>
+      <c r="U11" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V11" s="50"/>
-      <c r="W11" s="50"/>
-      <c r="X11" s="50"/>
-      <c r="Y11" s="51"/>
-      <c r="Z11" s="49" t="s">
+      <c r="V11" s="51"/>
+      <c r="W11" s="51"/>
+      <c r="X11" s="51"/>
+      <c r="Y11" s="52"/>
+      <c r="Z11" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="AA11" s="50"/>
-      <c r="AB11" s="51"/>
-      <c r="AC11" s="49" t="s">
+      <c r="AA11" s="51"/>
+      <c r="AB11" s="52"/>
+      <c r="AC11" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD11" s="50"/>
-      <c r="AE11" s="50"/>
-      <c r="AF11" s="50"/>
-      <c r="AG11" s="51"/>
-      <c r="AH11" s="49" t="s">
+      <c r="AD11" s="51"/>
+      <c r="AE11" s="51"/>
+      <c r="AF11" s="51"/>
+      <c r="AG11" s="52"/>
+      <c r="AH11" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AI11" s="50"/>
-      <c r="AJ11" s="50"/>
-      <c r="AK11" s="50"/>
-      <c r="AL11" s="50"/>
-      <c r="AM11" s="50"/>
-      <c r="AN11" s="61"/>
-      <c r="AP11" s="76" t="s">
+      <c r="AI11" s="51"/>
+      <c r="AJ11" s="51"/>
+      <c r="AK11" s="51"/>
+      <c r="AL11" s="51"/>
+      <c r="AM11" s="51"/>
+      <c r="AN11" s="62"/>
+      <c r="AP11" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="AQ11" s="77"/>
-      <c r="AR11" s="78">
-        <v>1</v>
-      </c>
-      <c r="AS11" s="78">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="78">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="79">
+      <c r="AQ11" s="58"/>
+      <c r="AR11" s="21">
+        <v>1</v>
+      </c>
+      <c r="AS11" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="21">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="73">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:47" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -1881,12 +2013,22 @@
       <c r="AL12" s="4"/>
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
-      <c r="AP12" s="68"/>
-      <c r="AQ12" s="68"/>
-      <c r="AR12" s="69"/>
-      <c r="AS12" s="69"/>
-      <c r="AT12" s="69"/>
-      <c r="AU12" s="69"/>
+      <c r="AP12" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ12" s="76"/>
+      <c r="AR12" s="77">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="77">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="77">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="78">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="4:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="5"/>
@@ -1931,56 +2073,56 @@
       </c>
     </row>
     <row r="14" spans="4:47" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="I14" s="54" t="s">
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="I14" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="49" t="s">
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="50"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="49" t="s">
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V14" s="50"/>
-      <c r="W14" s="50"/>
-      <c r="X14" s="50"/>
-      <c r="Y14" s="51"/>
-      <c r="Z14" s="49" t="s">
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="52"/>
+      <c r="Z14" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="AA14" s="50"/>
-      <c r="AB14" s="51"/>
-      <c r="AC14" s="49" t="s">
+      <c r="AA14" s="51"/>
+      <c r="AB14" s="52"/>
+      <c r="AC14" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="AD14" s="50"/>
-      <c r="AE14" s="50"/>
-      <c r="AF14" s="50"/>
-      <c r="AG14" s="51"/>
-      <c r="AH14" s="49" t="s">
+      <c r="AD14" s="51"/>
+      <c r="AE14" s="51"/>
+      <c r="AF14" s="51"/>
+      <c r="AG14" s="52"/>
+      <c r="AH14" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AI14" s="50"/>
-      <c r="AJ14" s="50"/>
-      <c r="AK14" s="50"/>
-      <c r="AL14" s="50"/>
-      <c r="AM14" s="50"/>
-      <c r="AN14" s="61"/>
+      <c r="AI14" s="51"/>
+      <c r="AJ14" s="51"/>
+      <c r="AK14" s="51"/>
+      <c r="AL14" s="51"/>
+      <c r="AM14" s="51"/>
+      <c r="AN14" s="62"/>
     </row>
     <row r="15" spans="4:47" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="5"/>
@@ -2065,63 +2207,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:55" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="65" t="s">
+    <row r="17" spans="3:56" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
       <c r="I17" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="54" t="s">
+      <c r="J17" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="49" t="s">
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q17" s="50"/>
-      <c r="R17" s="50"/>
-      <c r="S17" s="50"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="49" t="s">
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="52"/>
+      <c r="U17" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V17" s="50"/>
-      <c r="W17" s="50"/>
-      <c r="X17" s="50"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="49" t="s">
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51"/>
+      <c r="Y17" s="52"/>
+      <c r="Z17" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="AA17" s="50"/>
-      <c r="AB17" s="51"/>
-      <c r="AC17" s="49" t="s">
+      <c r="AA17" s="51"/>
+      <c r="AB17" s="52"/>
+      <c r="AC17" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="AD17" s="50"/>
-      <c r="AE17" s="50"/>
-      <c r="AF17" s="51"/>
+      <c r="AD17" s="51"/>
+      <c r="AE17" s="51"/>
+      <c r="AF17" s="52"/>
       <c r="AG17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AH17" s="49" t="s">
+      <c r="AH17" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AI17" s="50"/>
-      <c r="AJ17" s="50"/>
-      <c r="AK17" s="50"/>
-      <c r="AL17" s="50"/>
-      <c r="AM17" s="50"/>
-      <c r="AN17" s="61"/>
+      <c r="AI17" s="51"/>
+      <c r="AJ17" s="51"/>
+      <c r="AK17" s="51"/>
+      <c r="AL17" s="51"/>
+      <c r="AM17" s="51"/>
+      <c r="AN17" s="62"/>
     </row>
-    <row r="18" spans="3:55" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:56" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -2159,7 +2301,7 @@
       <c r="AM18" s="4"/>
       <c r="AN18" s="4"/>
     </row>
-    <row r="19" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -2183,53 +2325,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:55" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="62" t="s">
+    <row r="20" spans="3:56" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="I20" s="54" t="s">
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="I20" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="50"/>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="50"/>
-      <c r="S20" s="50"/>
-      <c r="T20" s="50"/>
-      <c r="U20" s="50"/>
-      <c r="V20" s="50"/>
-      <c r="W20" s="50"/>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="50"/>
-      <c r="Z20" s="50"/>
-      <c r="AA20" s="50"/>
-      <c r="AB20" s="51"/>
-      <c r="AC20" s="49" t="s">
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+      <c r="AB20" s="52"/>
+      <c r="AC20" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD20" s="50"/>
-      <c r="AE20" s="50"/>
-      <c r="AF20" s="50"/>
-      <c r="AG20" s="51"/>
-      <c r="AH20" s="49" t="s">
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51"/>
+      <c r="AF20" s="51"/>
+      <c r="AG20" s="52"/>
+      <c r="AH20" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AI20" s="50"/>
-      <c r="AJ20" s="50"/>
-      <c r="AK20" s="50"/>
-      <c r="AL20" s="50"/>
-      <c r="AM20" s="50"/>
-      <c r="AN20" s="61"/>
+      <c r="AI20" s="51"/>
+      <c r="AJ20" s="51"/>
+      <c r="AK20" s="51"/>
+      <c r="AL20" s="51"/>
+      <c r="AM20" s="51"/>
+      <c r="AN20" s="62"/>
     </row>
-    <row r="21" spans="3:55" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:56" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -2267,7 +2409,7 @@
       <c r="AM21" s="4"/>
       <c r="AN21" s="4"/>
     </row>
-    <row r="22" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -2309,78 +2451,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:55" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="63" t="s">
+    <row r="23" spans="3:56" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
       <c r="I23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="49" t="s">
+      <c r="J23" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="50"/>
-      <c r="S23" s="50"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
+      <c r="S23" s="51"/>
       <c r="T23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U23" s="49" t="s">
+      <c r="U23" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="V23" s="50"/>
-      <c r="W23" s="50"/>
-      <c r="X23" s="50"/>
-      <c r="Y23" s="50"/>
-      <c r="Z23" s="50"/>
-      <c r="AA23" s="50"/>
-      <c r="AB23" s="51"/>
-      <c r="AC23" s="49" t="s">
+      <c r="V23" s="51"/>
+      <c r="W23" s="51"/>
+      <c r="X23" s="51"/>
+      <c r="Y23" s="51"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="51"/>
+      <c r="AB23" s="52"/>
+      <c r="AC23" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD23" s="50"/>
-      <c r="AE23" s="50"/>
-      <c r="AF23" s="50"/>
-      <c r="AG23" s="51"/>
-      <c r="AH23" s="49" t="s">
+      <c r="AD23" s="51"/>
+      <c r="AE23" s="51"/>
+      <c r="AF23" s="51"/>
+      <c r="AG23" s="52"/>
+      <c r="AH23" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AI23" s="50"/>
-      <c r="AJ23" s="50"/>
-      <c r="AK23" s="50"/>
-      <c r="AL23" s="50"/>
-      <c r="AM23" s="50"/>
-      <c r="AN23" s="61"/>
+      <c r="AI23" s="51"/>
+      <c r="AJ23" s="51"/>
+      <c r="AK23" s="51"/>
+      <c r="AL23" s="51"/>
+      <c r="AM23" s="51"/>
+      <c r="AN23" s="62"/>
     </row>
-    <row r="25" spans="3:55" ht="15" x14ac:dyDescent="0.25">
-      <c r="AW25" s="66" t="s">
+    <row r="25" spans="3:56" ht="15" x14ac:dyDescent="0.25">
+      <c r="AW25" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="AX25" s="66"/>
-      <c r="AY25" s="66"/>
-      <c r="AZ25" s="66"/>
-      <c r="BA25" s="66"/>
-      <c r="BB25" s="66"/>
+      <c r="AX25" s="67"/>
+      <c r="AY25" s="67"/>
+      <c r="AZ25" s="67"/>
+      <c r="BA25" s="67"/>
+      <c r="BB25" s="67"/>
     </row>
-    <row r="26" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="AP26" s="67" t="s">
+      <c r="AP26" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="AQ26" s="67"/>
-      <c r="AR26" s="67"/>
-      <c r="AS26" s="67"/>
+      <c r="AQ26" s="68"/>
+      <c r="AR26" s="68"/>
+      <c r="AS26" s="68"/>
       <c r="AT26" s="22"/>
       <c r="AU26" s="22"/>
       <c r="AW26" s="38" t="s">
@@ -2404,15 +2546,18 @@
       <c r="BC26" s="39" t="s">
         <v>53</v>
       </c>
+      <c r="BD26" s="39" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="27" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="53" t="s">
+      <c r="D27" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="53"/>
+      <c r="E27" s="54"/>
       <c r="F27" s="19" t="s">
         <v>27</v>
       </c>
@@ -2437,20 +2582,20 @@
       <c r="O27" s="10">
         <v>0</v>
       </c>
-      <c r="P27" s="49" t="s">
+      <c r="P27" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="50"/>
-      <c r="T27" s="51"/>
-      <c r="U27" s="49" t="s">
+      <c r="Q27" s="51"/>
+      <c r="R27" s="51"/>
+      <c r="S27" s="51"/>
+      <c r="T27" s="52"/>
+      <c r="U27" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V27" s="50"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="50"/>
-      <c r="Y27" s="51"/>
+      <c r="V27" s="51"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="51"/>
+      <c r="Y27" s="52"/>
       <c r="Z27" s="16">
         <v>0</v>
       </c>
@@ -2460,13 +2605,13 @@
       <c r="AB27" s="18">
         <v>0</v>
       </c>
-      <c r="AC27" s="49" t="s">
+      <c r="AC27" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD27" s="50"/>
-      <c r="AE27" s="50"/>
-      <c r="AF27" s="50"/>
-      <c r="AG27" s="51"/>
+      <c r="AD27" s="51"/>
+      <c r="AE27" s="51"/>
+      <c r="AF27" s="51"/>
+      <c r="AG27" s="52"/>
       <c r="AH27" s="8">
         <v>0</v>
       </c>
@@ -2488,10 +2633,10 @@
       <c r="AN27" s="15">
         <v>1</v>
       </c>
-      <c r="AP27" s="52" t="s">
+      <c r="AP27" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ27" s="52"/>
+      <c r="AQ27" s="53"/>
       <c r="AR27" s="23">
         <v>0</v>
       </c>
@@ -2525,15 +2670,18 @@
       <c r="BC27" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD27" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="28" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="53" t="s">
+      <c r="D28" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="53"/>
+      <c r="E28" s="54"/>
       <c r="F28" s="19" t="s">
         <v>27</v>
       </c>
@@ -2558,20 +2706,20 @@
       <c r="O28" s="10">
         <v>0</v>
       </c>
-      <c r="P28" s="49" t="s">
+      <c r="P28" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="50"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="49" t="s">
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="52"/>
+      <c r="U28" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V28" s="50"/>
-      <c r="W28" s="50"/>
-      <c r="X28" s="50"/>
-      <c r="Y28" s="51"/>
+      <c r="V28" s="51"/>
+      <c r="W28" s="51"/>
+      <c r="X28" s="51"/>
+      <c r="Y28" s="52"/>
       <c r="Z28" s="16">
         <v>0</v>
       </c>
@@ -2581,13 +2729,13 @@
       <c r="AB28" s="18">
         <v>0</v>
       </c>
-      <c r="AC28" s="49" t="s">
+      <c r="AC28" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD28" s="50"/>
-      <c r="AE28" s="50"/>
-      <c r="AF28" s="50"/>
-      <c r="AG28" s="51"/>
+      <c r="AD28" s="51"/>
+      <c r="AE28" s="51"/>
+      <c r="AF28" s="51"/>
+      <c r="AG28" s="52"/>
       <c r="AH28" s="8">
         <v>0</v>
       </c>
@@ -2609,10 +2757,10 @@
       <c r="AN28" s="15">
         <v>1</v>
       </c>
-      <c r="AP28" s="52" t="s">
+      <c r="AP28" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="AQ28" s="52"/>
+      <c r="AQ28" s="53"/>
       <c r="AR28" s="26">
         <v>0</v>
       </c>
@@ -2646,15 +2794,18 @@
       <c r="BC28" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD28" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="29" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="53" t="s">
+      <c r="D29" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="53"/>
+      <c r="E29" s="54"/>
       <c r="F29" s="19" t="s">
         <v>27</v>
       </c>
@@ -2679,20 +2830,20 @@
       <c r="O29" s="34">
         <v>0</v>
       </c>
-      <c r="P29" s="49" t="s">
+      <c r="P29" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q29" s="50"/>
-      <c r="R29" s="50"/>
-      <c r="S29" s="50"/>
-      <c r="T29" s="51"/>
-      <c r="U29" s="49" t="s">
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
+      <c r="T29" s="52"/>
+      <c r="U29" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V29" s="50"/>
-      <c r="W29" s="50"/>
-      <c r="X29" s="50"/>
-      <c r="Y29" s="51"/>
+      <c r="V29" s="51"/>
+      <c r="W29" s="51"/>
+      <c r="X29" s="51"/>
+      <c r="Y29" s="52"/>
       <c r="Z29" s="16">
         <v>1</v>
       </c>
@@ -2702,13 +2853,13 @@
       <c r="AB29" s="18">
         <v>0</v>
       </c>
-      <c r="AC29" s="49" t="s">
+      <c r="AC29" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD29" s="50"/>
-      <c r="AE29" s="50"/>
-      <c r="AF29" s="50"/>
-      <c r="AG29" s="51"/>
+      <c r="AD29" s="51"/>
+      <c r="AE29" s="51"/>
+      <c r="AF29" s="51"/>
+      <c r="AG29" s="52"/>
       <c r="AH29" s="32">
         <v>0</v>
       </c>
@@ -2730,10 +2881,10 @@
       <c r="AN29" s="36">
         <v>1</v>
       </c>
-      <c r="AP29" s="55" t="s">
+      <c r="AP29" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="AQ29" s="56"/>
+      <c r="AQ29" s="57"/>
       <c r="AR29" s="26">
         <v>0</v>
       </c>
@@ -2767,15 +2918,18 @@
       <c r="BC29" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD29" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="30" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="53" t="s">
+      <c r="D30" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="53"/>
+      <c r="E30" s="54"/>
       <c r="F30" s="19" t="s">
         <v>27</v>
       </c>
@@ -2800,20 +2954,20 @@
       <c r="O30" s="34">
         <v>0</v>
       </c>
-      <c r="P30" s="49" t="s">
+      <c r="P30" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q30" s="50"/>
-      <c r="R30" s="50"/>
-      <c r="S30" s="50"/>
-      <c r="T30" s="51"/>
-      <c r="U30" s="49" t="s">
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
+      <c r="T30" s="52"/>
+      <c r="U30" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V30" s="50"/>
-      <c r="W30" s="50"/>
-      <c r="X30" s="50"/>
-      <c r="Y30" s="51"/>
+      <c r="V30" s="51"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
+      <c r="Y30" s="52"/>
       <c r="Z30" s="16">
         <v>1</v>
       </c>
@@ -2823,13 +2977,13 @@
       <c r="AB30" s="18">
         <v>0</v>
       </c>
-      <c r="AC30" s="49" t="s">
+      <c r="AC30" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD30" s="50"/>
-      <c r="AE30" s="50"/>
-      <c r="AF30" s="50"/>
-      <c r="AG30" s="51"/>
+      <c r="AD30" s="51"/>
+      <c r="AE30" s="51"/>
+      <c r="AF30" s="51"/>
+      <c r="AG30" s="52"/>
       <c r="AH30" s="32">
         <v>0</v>
       </c>
@@ -2851,10 +3005,10 @@
       <c r="AN30" s="36">
         <v>1</v>
       </c>
-      <c r="AP30" s="55" t="s">
+      <c r="AP30" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="AQ30" s="56"/>
+      <c r="AQ30" s="57"/>
       <c r="AR30" s="26">
         <v>0</v>
       </c>
@@ -2888,15 +3042,18 @@
       <c r="BC30" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD30" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="31" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="53" t="s">
+      <c r="D31" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="53"/>
+      <c r="E31" s="54"/>
       <c r="F31" s="19" t="s">
         <v>27</v>
       </c>
@@ -2921,20 +3078,20 @@
       <c r="O31" s="34">
         <v>0</v>
       </c>
-      <c r="P31" s="49" t="s">
+      <c r="P31" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q31" s="50"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="50"/>
-      <c r="T31" s="51"/>
-      <c r="U31" s="49" t="s">
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
+      <c r="T31" s="52"/>
+      <c r="U31" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V31" s="50"/>
-      <c r="W31" s="50"/>
-      <c r="X31" s="50"/>
-      <c r="Y31" s="51"/>
+      <c r="V31" s="51"/>
+      <c r="W31" s="51"/>
+      <c r="X31" s="51"/>
+      <c r="Y31" s="52"/>
       <c r="Z31" s="16">
         <v>1</v>
       </c>
@@ -2944,13 +3101,13 @@
       <c r="AB31" s="18">
         <v>1</v>
       </c>
-      <c r="AC31" s="49" t="s">
+      <c r="AC31" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD31" s="50"/>
-      <c r="AE31" s="50"/>
-      <c r="AF31" s="50"/>
-      <c r="AG31" s="51"/>
+      <c r="AD31" s="51"/>
+      <c r="AE31" s="51"/>
+      <c r="AF31" s="51"/>
+      <c r="AG31" s="52"/>
       <c r="AH31" s="32">
         <v>0</v>
       </c>
@@ -2972,10 +3129,10 @@
       <c r="AN31" s="36">
         <v>1</v>
       </c>
-      <c r="AP31" s="55" t="s">
+      <c r="AP31" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="AQ31" s="56"/>
+      <c r="AQ31" s="57"/>
       <c r="AR31" s="26">
         <v>0</v>
       </c>
@@ -3009,15 +3166,18 @@
       <c r="BC31" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD31" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="32" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="53" t="s">
+      <c r="D32" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="53"/>
+      <c r="E32" s="54"/>
       <c r="F32" s="19" t="s">
         <v>27</v>
       </c>
@@ -3042,20 +3202,20 @@
       <c r="O32" s="34">
         <v>0</v>
       </c>
-      <c r="P32" s="49" t="s">
+      <c r="P32" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q32" s="50"/>
-      <c r="R32" s="50"/>
-      <c r="S32" s="50"/>
-      <c r="T32" s="51"/>
-      <c r="U32" s="49" t="s">
+      <c r="Q32" s="51"/>
+      <c r="R32" s="51"/>
+      <c r="S32" s="51"/>
+      <c r="T32" s="52"/>
+      <c r="U32" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V32" s="50"/>
-      <c r="W32" s="50"/>
-      <c r="X32" s="50"/>
-      <c r="Y32" s="51"/>
+      <c r="V32" s="51"/>
+      <c r="W32" s="51"/>
+      <c r="X32" s="51"/>
+      <c r="Y32" s="52"/>
       <c r="Z32" s="16">
         <v>0</v>
       </c>
@@ -3065,13 +3225,13 @@
       <c r="AB32" s="18">
         <v>1</v>
       </c>
-      <c r="AC32" s="49" t="s">
+      <c r="AC32" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD32" s="50"/>
-      <c r="AE32" s="50"/>
-      <c r="AF32" s="50"/>
-      <c r="AG32" s="51"/>
+      <c r="AD32" s="51"/>
+      <c r="AE32" s="51"/>
+      <c r="AF32" s="51"/>
+      <c r="AG32" s="52"/>
       <c r="AH32" s="32">
         <v>0</v>
       </c>
@@ -3093,10 +3253,10 @@
       <c r="AN32" s="36">
         <v>1</v>
       </c>
-      <c r="AP32" s="55" t="s">
+      <c r="AP32" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="AQ32" s="56"/>
+      <c r="AQ32" s="57"/>
       <c r="AR32" s="26">
         <v>0</v>
       </c>
@@ -3130,15 +3290,18 @@
       <c r="BC32" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD32" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="33" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="53" t="s">
+      <c r="D33" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="53"/>
+      <c r="E33" s="54"/>
       <c r="F33" s="19" t="s">
         <v>27</v>
       </c>
@@ -3163,20 +3326,20 @@
       <c r="O33" s="34">
         <v>0</v>
       </c>
-      <c r="P33" s="49" t="s">
+      <c r="P33" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q33" s="50"/>
-      <c r="R33" s="50"/>
-      <c r="S33" s="50"/>
-      <c r="T33" s="51"/>
-      <c r="U33" s="49" t="s">
+      <c r="Q33" s="51"/>
+      <c r="R33" s="51"/>
+      <c r="S33" s="51"/>
+      <c r="T33" s="52"/>
+      <c r="U33" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V33" s="50"/>
-      <c r="W33" s="50"/>
-      <c r="X33" s="50"/>
-      <c r="Y33" s="51"/>
+      <c r="V33" s="51"/>
+      <c r="W33" s="51"/>
+      <c r="X33" s="51"/>
+      <c r="Y33" s="52"/>
       <c r="Z33" s="16">
         <v>1</v>
       </c>
@@ -3186,13 +3349,13 @@
       <c r="AB33" s="18">
         <v>1</v>
       </c>
-      <c r="AC33" s="49" t="s">
+      <c r="AC33" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD33" s="50"/>
-      <c r="AE33" s="50"/>
-      <c r="AF33" s="50"/>
-      <c r="AG33" s="51"/>
+      <c r="AD33" s="51"/>
+      <c r="AE33" s="51"/>
+      <c r="AF33" s="51"/>
+      <c r="AG33" s="52"/>
       <c r="AH33" s="32">
         <v>0</v>
       </c>
@@ -3214,10 +3377,10 @@
       <c r="AN33" s="36">
         <v>1</v>
       </c>
-      <c r="AP33" s="55" t="s">
+      <c r="AP33" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="AQ33" s="56"/>
+      <c r="AQ33" s="57"/>
       <c r="AR33" s="26">
         <v>1</v>
       </c>
@@ -3251,15 +3414,18 @@
       <c r="BC33" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD33" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="34" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="53" t="s">
+      <c r="D34" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="53"/>
+      <c r="E34" s="54"/>
       <c r="F34" s="19" t="s">
         <v>27</v>
       </c>
@@ -3284,20 +3450,20 @@
       <c r="O34" s="34">
         <v>0</v>
       </c>
-      <c r="P34" s="49" t="s">
+      <c r="P34" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q34" s="50"/>
-      <c r="R34" s="50"/>
-      <c r="S34" s="50"/>
-      <c r="T34" s="51"/>
-      <c r="U34" s="49" t="s">
+      <c r="Q34" s="51"/>
+      <c r="R34" s="51"/>
+      <c r="S34" s="51"/>
+      <c r="T34" s="52"/>
+      <c r="U34" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V34" s="50"/>
-      <c r="W34" s="50"/>
-      <c r="X34" s="50"/>
-      <c r="Y34" s="51"/>
+      <c r="V34" s="51"/>
+      <c r="W34" s="51"/>
+      <c r="X34" s="51"/>
+      <c r="Y34" s="52"/>
       <c r="Z34" s="16">
         <v>1</v>
       </c>
@@ -3307,13 +3473,13 @@
       <c r="AB34" s="18">
         <v>1</v>
       </c>
-      <c r="AC34" s="49" t="s">
+      <c r="AC34" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD34" s="50"/>
-      <c r="AE34" s="50"/>
-      <c r="AF34" s="50"/>
-      <c r="AG34" s="51"/>
+      <c r="AD34" s="51"/>
+      <c r="AE34" s="51"/>
+      <c r="AF34" s="51"/>
+      <c r="AG34" s="52"/>
       <c r="AH34" s="32">
         <v>0</v>
       </c>
@@ -3335,10 +3501,10 @@
       <c r="AN34" s="36">
         <v>1</v>
       </c>
-      <c r="AP34" s="55" t="s">
+      <c r="AP34" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="AQ34" s="56"/>
+      <c r="AQ34" s="57"/>
       <c r="AR34" s="26">
         <v>0</v>
       </c>
@@ -3372,15 +3538,18 @@
       <c r="BC34" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD34" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="35" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="53" t="s">
+      <c r="D35" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="53"/>
+      <c r="E35" s="54"/>
       <c r="F35" s="19" t="s">
         <v>27</v>
       </c>
@@ -3405,20 +3574,20 @@
       <c r="O35" s="34">
         <v>0</v>
       </c>
-      <c r="P35" s="49" t="s">
+      <c r="P35" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q35" s="50"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="50"/>
-      <c r="T35" s="51"/>
-      <c r="U35" s="49" t="s">
+      <c r="Q35" s="51"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="51"/>
+      <c r="T35" s="52"/>
+      <c r="U35" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V35" s="50"/>
-      <c r="W35" s="50"/>
-      <c r="X35" s="50"/>
-      <c r="Y35" s="51"/>
+      <c r="V35" s="51"/>
+      <c r="W35" s="51"/>
+      <c r="X35" s="51"/>
+      <c r="Y35" s="52"/>
       <c r="Z35" s="16">
         <v>0</v>
       </c>
@@ -3428,13 +3597,13 @@
       <c r="AB35" s="18">
         <v>0</v>
       </c>
-      <c r="AC35" s="49" t="s">
+      <c r="AC35" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD35" s="50"/>
-      <c r="AE35" s="50"/>
-      <c r="AF35" s="50"/>
-      <c r="AG35" s="51"/>
+      <c r="AD35" s="51"/>
+      <c r="AE35" s="51"/>
+      <c r="AF35" s="51"/>
+      <c r="AG35" s="52"/>
       <c r="AH35" s="32">
         <v>0</v>
       </c>
@@ -3456,10 +3625,10 @@
       <c r="AN35" s="36">
         <v>1</v>
       </c>
-      <c r="AP35" s="55" t="s">
+      <c r="AP35" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="AQ35" s="56"/>
+      <c r="AQ35" s="57"/>
       <c r="AR35" s="26">
         <v>0</v>
       </c>
@@ -3493,15 +3662,18 @@
       <c r="BC35" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD35" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="36" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="53" t="s">
+      <c r="D36" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="53"/>
+      <c r="E36" s="54"/>
       <c r="F36" s="19" t="s">
         <v>27</v>
       </c>
@@ -3526,20 +3698,20 @@
       <c r="O36" s="34">
         <v>0</v>
       </c>
-      <c r="P36" s="49" t="s">
+      <c r="P36" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q36" s="50"/>
-      <c r="R36" s="50"/>
-      <c r="S36" s="50"/>
-      <c r="T36" s="51"/>
-      <c r="U36" s="49" t="s">
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="52"/>
+      <c r="U36" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V36" s="50"/>
-      <c r="W36" s="50"/>
-      <c r="X36" s="50"/>
-      <c r="Y36" s="51"/>
+      <c r="V36" s="51"/>
+      <c r="W36" s="51"/>
+      <c r="X36" s="51"/>
+      <c r="Y36" s="52"/>
       <c r="Z36" s="16">
         <v>0</v>
       </c>
@@ -3549,13 +3721,13 @@
       <c r="AB36" s="18">
         <v>1</v>
       </c>
-      <c r="AC36" s="49" t="s">
+      <c r="AC36" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD36" s="50"/>
-      <c r="AE36" s="50"/>
-      <c r="AF36" s="50"/>
-      <c r="AG36" s="51"/>
+      <c r="AD36" s="51"/>
+      <c r="AE36" s="51"/>
+      <c r="AF36" s="51"/>
+      <c r="AG36" s="52"/>
       <c r="AH36" s="32">
         <v>0</v>
       </c>
@@ -3577,10 +3749,10 @@
       <c r="AN36" s="36">
         <v>1</v>
       </c>
-      <c r="AP36" s="55" t="s">
+      <c r="AP36" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="AQ36" s="56"/>
+      <c r="AQ36" s="57"/>
       <c r="AR36" s="26">
         <v>1</v>
       </c>
@@ -3614,39 +3786,42 @@
       <c r="BC36" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD36" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="37" spans="3:55" ht="15.75" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:56" ht="15.75" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="53" t="s">
+      <c r="D37" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="53"/>
+      <c r="E37" s="54"/>
       <c r="F37" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I37" s="54" t="s">
+      <c r="I37" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="50"/>
-      <c r="O37" s="50"/>
-      <c r="P37" s="50"/>
-      <c r="Q37" s="50"/>
-      <c r="R37" s="50"/>
-      <c r="S37" s="50"/>
-      <c r="T37" s="51"/>
-      <c r="U37" s="49" t="s">
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="51"/>
+      <c r="R37" s="51"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="52"/>
+      <c r="U37" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V37" s="50"/>
-      <c r="W37" s="50"/>
-      <c r="X37" s="50"/>
-      <c r="Y37" s="51"/>
+      <c r="V37" s="51"/>
+      <c r="W37" s="51"/>
+      <c r="X37" s="51"/>
+      <c r="Y37" s="52"/>
       <c r="Z37" s="16">
         <v>0</v>
       </c>
@@ -3656,13 +3831,13 @@
       <c r="AB37" s="18">
         <v>0</v>
       </c>
-      <c r="AC37" s="49" t="s">
+      <c r="AC37" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD37" s="50"/>
-      <c r="AE37" s="50"/>
-      <c r="AF37" s="50"/>
-      <c r="AG37" s="51"/>
+      <c r="AD37" s="51"/>
+      <c r="AE37" s="51"/>
+      <c r="AF37" s="51"/>
+      <c r="AG37" s="52"/>
       <c r="AH37" s="8">
         <v>0</v>
       </c>
@@ -3684,10 +3859,10 @@
       <c r="AN37" s="15">
         <v>1</v>
       </c>
-      <c r="AP37" s="52" t="s">
+      <c r="AP37" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ37" s="52"/>
+      <c r="AQ37" s="53"/>
       <c r="AR37" s="26">
         <v>0</v>
       </c>
@@ -3721,39 +3896,42 @@
       <c r="BC37" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD37" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="38" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="53" t="s">
+      <c r="D38" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="E38" s="53"/>
+      <c r="E38" s="54"/>
       <c r="F38" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="54" t="s">
+      <c r="I38" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="50"/>
-      <c r="K38" s="50"/>
-      <c r="L38" s="50"/>
-      <c r="M38" s="50"/>
-      <c r="N38" s="50"/>
-      <c r="O38" s="50"/>
-      <c r="P38" s="50"/>
-      <c r="Q38" s="50"/>
-      <c r="R38" s="50"/>
-      <c r="S38" s="50"/>
-      <c r="T38" s="51"/>
-      <c r="U38" s="49" t="s">
+      <c r="J38" s="51"/>
+      <c r="K38" s="51"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="51"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="51"/>
+      <c r="R38" s="51"/>
+      <c r="S38" s="51"/>
+      <c r="T38" s="52"/>
+      <c r="U38" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V38" s="50"/>
-      <c r="W38" s="50"/>
-      <c r="X38" s="50"/>
-      <c r="Y38" s="51"/>
+      <c r="V38" s="51"/>
+      <c r="W38" s="51"/>
+      <c r="X38" s="51"/>
+      <c r="Y38" s="52"/>
       <c r="Z38" s="16">
         <v>1</v>
       </c>
@@ -3763,13 +3941,13 @@
       <c r="AB38" s="18">
         <v>0</v>
       </c>
-      <c r="AC38" s="49" t="s">
+      <c r="AC38" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD38" s="50"/>
-      <c r="AE38" s="50"/>
-      <c r="AF38" s="50"/>
-      <c r="AG38" s="51"/>
+      <c r="AD38" s="51"/>
+      <c r="AE38" s="51"/>
+      <c r="AF38" s="51"/>
+      <c r="AG38" s="52"/>
       <c r="AH38" s="32">
         <v>0</v>
       </c>
@@ -3791,10 +3969,10 @@
       <c r="AN38" s="36">
         <v>1</v>
       </c>
-      <c r="AP38" s="52" t="s">
+      <c r="AP38" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="AQ38" s="52"/>
+      <c r="AQ38" s="53"/>
       <c r="AR38" s="26">
         <v>0</v>
       </c>
@@ -3828,39 +4006,42 @@
       <c r="BC38" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD38" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="39" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="53" t="s">
+      <c r="D39" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E39" s="53"/>
+      <c r="E39" s="54"/>
       <c r="F39" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="54" t="s">
+      <c r="I39" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="50"/>
-      <c r="K39" s="50"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="50"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="50"/>
-      <c r="P39" s="50"/>
-      <c r="Q39" s="50"/>
-      <c r="R39" s="50"/>
-      <c r="S39" s="50"/>
-      <c r="T39" s="51"/>
-      <c r="U39" s="49" t="s">
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
+      <c r="T39" s="52"/>
+      <c r="U39" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V39" s="50"/>
-      <c r="W39" s="50"/>
-      <c r="X39" s="50"/>
-      <c r="Y39" s="51"/>
+      <c r="V39" s="51"/>
+      <c r="W39" s="51"/>
+      <c r="X39" s="51"/>
+      <c r="Y39" s="52"/>
       <c r="Z39" s="16">
         <v>1</v>
       </c>
@@ -3870,13 +4051,13 @@
       <c r="AB39" s="18">
         <v>0</v>
       </c>
-      <c r="AC39" s="49" t="s">
+      <c r="AC39" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD39" s="50"/>
-      <c r="AE39" s="50"/>
-      <c r="AF39" s="50"/>
-      <c r="AG39" s="51"/>
+      <c r="AD39" s="51"/>
+      <c r="AE39" s="51"/>
+      <c r="AF39" s="51"/>
+      <c r="AG39" s="52"/>
       <c r="AH39" s="32">
         <v>0</v>
       </c>
@@ -3898,10 +4079,10 @@
       <c r="AN39" s="36">
         <v>1</v>
       </c>
-      <c r="AP39" s="52" t="s">
+      <c r="AP39" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="AQ39" s="52"/>
+      <c r="AQ39" s="53"/>
       <c r="AR39" s="26">
         <v>0</v>
       </c>
@@ -3935,39 +4116,42 @@
       <c r="BC39" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD39" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="40" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="53" t="s">
+      <c r="D40" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="53"/>
+      <c r="E40" s="54"/>
       <c r="F40" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I40" s="54" t="s">
+      <c r="I40" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J40" s="50"/>
-      <c r="K40" s="50"/>
-      <c r="L40" s="50"/>
-      <c r="M40" s="50"/>
-      <c r="N40" s="50"/>
-      <c r="O40" s="50"/>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="50"/>
-      <c r="R40" s="50"/>
-      <c r="S40" s="50"/>
-      <c r="T40" s="51"/>
-      <c r="U40" s="49" t="s">
+      <c r="J40" s="51"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="51"/>
+      <c r="O40" s="51"/>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="51"/>
+      <c r="R40" s="51"/>
+      <c r="S40" s="51"/>
+      <c r="T40" s="52"/>
+      <c r="U40" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V40" s="50"/>
-      <c r="W40" s="50"/>
-      <c r="X40" s="50"/>
-      <c r="Y40" s="51"/>
+      <c r="V40" s="51"/>
+      <c r="W40" s="51"/>
+      <c r="X40" s="51"/>
+      <c r="Y40" s="52"/>
       <c r="Z40" s="16">
         <v>1</v>
       </c>
@@ -3977,13 +4161,13 @@
       <c r="AB40" s="18">
         <v>1</v>
       </c>
-      <c r="AC40" s="49" t="s">
+      <c r="AC40" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD40" s="50"/>
-      <c r="AE40" s="50"/>
-      <c r="AF40" s="50"/>
-      <c r="AG40" s="51"/>
+      <c r="AD40" s="51"/>
+      <c r="AE40" s="51"/>
+      <c r="AF40" s="51"/>
+      <c r="AG40" s="52"/>
       <c r="AH40" s="32">
         <v>0</v>
       </c>
@@ -4005,10 +4189,10 @@
       <c r="AN40" s="36">
         <v>1</v>
       </c>
-      <c r="AP40" s="52" t="s">
+      <c r="AP40" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="AQ40" s="52"/>
+      <c r="AQ40" s="53"/>
       <c r="AR40" s="26">
         <v>0</v>
       </c>
@@ -4042,15 +4226,18 @@
       <c r="BC40" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD40" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="41" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="53" t="s">
+      <c r="D41" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="E41" s="53"/>
+      <c r="E41" s="54"/>
       <c r="F41" s="12" t="s">
         <v>22</v>
       </c>
@@ -4075,20 +4262,20 @@
       <c r="O41" s="33">
         <v>0</v>
       </c>
-      <c r="P41" s="49" t="s">
+      <c r="P41" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Q41" s="50"/>
-      <c r="R41" s="50"/>
-      <c r="S41" s="50"/>
-      <c r="T41" s="51"/>
-      <c r="U41" s="50" t="s">
+      <c r="Q41" s="51"/>
+      <c r="R41" s="51"/>
+      <c r="S41" s="51"/>
+      <c r="T41" s="52"/>
+      <c r="U41" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V41" s="50"/>
-      <c r="W41" s="50"/>
-      <c r="X41" s="50"/>
-      <c r="Y41" s="51"/>
+      <c r="V41" s="51"/>
+      <c r="W41" s="51"/>
+      <c r="X41" s="51"/>
+      <c r="Y41" s="52"/>
       <c r="Z41" s="16">
         <v>0</v>
       </c>
@@ -4098,13 +4285,13 @@
       <c r="AB41" s="18">
         <v>1</v>
       </c>
-      <c r="AC41" s="49" t="s">
+      <c r="AC41" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD41" s="50"/>
-      <c r="AE41" s="50"/>
-      <c r="AF41" s="50"/>
-      <c r="AG41" s="51"/>
+      <c r="AD41" s="51"/>
+      <c r="AE41" s="51"/>
+      <c r="AF41" s="51"/>
+      <c r="AG41" s="52"/>
       <c r="AH41" s="32">
         <v>0</v>
       </c>
@@ -4126,10 +4313,10 @@
       <c r="AN41" s="36">
         <v>1</v>
       </c>
-      <c r="AP41" s="52" t="s">
+      <c r="AP41" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="AQ41" s="52"/>
+      <c r="AQ41" s="53"/>
       <c r="AR41" s="26">
         <v>0</v>
       </c>
@@ -4163,15 +4350,18 @@
       <c r="BC41" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD41" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="42" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="53" t="s">
+      <c r="D42" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="53"/>
+      <c r="E42" s="54"/>
       <c r="F42" s="12" t="s">
         <v>22</v>
       </c>
@@ -4196,20 +4386,20 @@
       <c r="O42" s="33">
         <v>0</v>
       </c>
-      <c r="P42" s="49" t="s">
+      <c r="P42" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Q42" s="50"/>
-      <c r="R42" s="50"/>
-      <c r="S42" s="50"/>
-      <c r="T42" s="51"/>
-      <c r="U42" s="50" t="s">
+      <c r="Q42" s="51"/>
+      <c r="R42" s="51"/>
+      <c r="S42" s="51"/>
+      <c r="T42" s="52"/>
+      <c r="U42" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V42" s="50"/>
-      <c r="W42" s="50"/>
-      <c r="X42" s="50"/>
-      <c r="Y42" s="51"/>
+      <c r="V42" s="51"/>
+      <c r="W42" s="51"/>
+      <c r="X42" s="51"/>
+      <c r="Y42" s="52"/>
       <c r="Z42" s="16">
         <v>1</v>
       </c>
@@ -4219,13 +4409,13 @@
       <c r="AB42" s="18">
         <v>1</v>
       </c>
-      <c r="AC42" s="49" t="s">
+      <c r="AC42" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD42" s="50"/>
-      <c r="AE42" s="50"/>
-      <c r="AF42" s="50"/>
-      <c r="AG42" s="51"/>
+      <c r="AD42" s="51"/>
+      <c r="AE42" s="51"/>
+      <c r="AF42" s="51"/>
+      <c r="AG42" s="52"/>
       <c r="AH42" s="32">
         <v>0</v>
       </c>
@@ -4247,10 +4437,10 @@
       <c r="AN42" s="36">
         <v>1</v>
       </c>
-      <c r="AP42" s="52" t="s">
+      <c r="AP42" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="AQ42" s="52"/>
+      <c r="AQ42" s="53"/>
       <c r="AR42" s="26">
         <v>1</v>
       </c>
@@ -4284,15 +4474,18 @@
       <c r="BC42" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD42" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="43" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="53" t="s">
+      <c r="D43" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="53"/>
+      <c r="E43" s="54"/>
       <c r="F43" s="12" t="s">
         <v>22</v>
       </c>
@@ -4317,20 +4510,20 @@
       <c r="O43" s="33">
         <v>0</v>
       </c>
-      <c r="P43" s="49" t="s">
+      <c r="P43" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Q43" s="50"/>
-      <c r="R43" s="50"/>
-      <c r="S43" s="50"/>
-      <c r="T43" s="51"/>
-      <c r="U43" s="50" t="s">
+      <c r="Q43" s="51"/>
+      <c r="R43" s="51"/>
+      <c r="S43" s="51"/>
+      <c r="T43" s="52"/>
+      <c r="U43" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="V43" s="50"/>
-      <c r="W43" s="50"/>
-      <c r="X43" s="50"/>
-      <c r="Y43" s="51"/>
+      <c r="V43" s="51"/>
+      <c r="W43" s="51"/>
+      <c r="X43" s="51"/>
+      <c r="Y43" s="52"/>
       <c r="Z43" s="16">
         <v>1</v>
       </c>
@@ -4340,13 +4533,13 @@
       <c r="AB43" s="18">
         <v>1</v>
       </c>
-      <c r="AC43" s="49" t="s">
+      <c r="AC43" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD43" s="50"/>
-      <c r="AE43" s="50"/>
-      <c r="AF43" s="50"/>
-      <c r="AG43" s="51"/>
+      <c r="AD43" s="51"/>
+      <c r="AE43" s="51"/>
+      <c r="AF43" s="51"/>
+      <c r="AG43" s="52"/>
       <c r="AH43" s="32">
         <v>0</v>
       </c>
@@ -4368,10 +4561,10 @@
       <c r="AN43" s="36">
         <v>1</v>
       </c>
-      <c r="AP43" s="52" t="s">
+      <c r="AP43" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="AQ43" s="52"/>
+      <c r="AQ43" s="53"/>
       <c r="AR43" s="26">
         <v>0</v>
       </c>
@@ -4405,39 +4598,42 @@
       <c r="BC43" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD43" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="44" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="53" t="s">
+      <c r="D44" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="53"/>
+      <c r="E44" s="54"/>
       <c r="F44" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I44" s="54" t="s">
+      <c r="I44" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J44" s="50"/>
-      <c r="K44" s="50"/>
-      <c r="L44" s="50"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="50"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="50"/>
-      <c r="R44" s="50"/>
-      <c r="S44" s="50"/>
-      <c r="T44" s="51"/>
-      <c r="U44" s="49" t="s">
+      <c r="J44" s="51"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="51"/>
+      <c r="O44" s="51"/>
+      <c r="P44" s="51"/>
+      <c r="Q44" s="51"/>
+      <c r="R44" s="51"/>
+      <c r="S44" s="51"/>
+      <c r="T44" s="52"/>
+      <c r="U44" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V44" s="50"/>
-      <c r="W44" s="50"/>
-      <c r="X44" s="50"/>
-      <c r="Y44" s="51"/>
+      <c r="V44" s="51"/>
+      <c r="W44" s="51"/>
+      <c r="X44" s="51"/>
+      <c r="Y44" s="52"/>
       <c r="Z44" s="16">
         <v>0</v>
       </c>
@@ -4447,13 +4643,13 @@
       <c r="AB44" s="18">
         <v>0</v>
       </c>
-      <c r="AC44" s="49" t="s">
+      <c r="AC44" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD44" s="50"/>
-      <c r="AE44" s="50"/>
-      <c r="AF44" s="50"/>
-      <c r="AG44" s="51"/>
+      <c r="AD44" s="51"/>
+      <c r="AE44" s="51"/>
+      <c r="AF44" s="51"/>
+      <c r="AG44" s="52"/>
       <c r="AH44" s="32">
         <v>0</v>
       </c>
@@ -4475,10 +4671,10 @@
       <c r="AN44" s="36">
         <v>1</v>
       </c>
-      <c r="AP44" s="52" t="s">
+      <c r="AP44" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="AQ44" s="52"/>
+      <c r="AQ44" s="53"/>
       <c r="AR44" s="26">
         <v>0</v>
       </c>
@@ -4512,37 +4708,40 @@
       <c r="BC44" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD44" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="45" spans="3:55" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="53" t="s">
+      <c r="D45" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="53"/>
+      <c r="E45" s="54"/>
       <c r="F45" s="12"/>
-      <c r="I45" s="54" t="s">
+      <c r="I45" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="50"/>
-      <c r="M45" s="50"/>
-      <c r="N45" s="50"/>
-      <c r="O45" s="50"/>
-      <c r="P45" s="50"/>
-      <c r="Q45" s="50"/>
-      <c r="R45" s="50"/>
-      <c r="S45" s="50"/>
-      <c r="T45" s="51"/>
-      <c r="U45" s="49" t="s">
+      <c r="J45" s="51"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="51"/>
+      <c r="M45" s="51"/>
+      <c r="N45" s="51"/>
+      <c r="O45" s="51"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="51"/>
+      <c r="R45" s="51"/>
+      <c r="S45" s="51"/>
+      <c r="T45" s="52"/>
+      <c r="U45" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V45" s="50"/>
-      <c r="W45" s="50"/>
-      <c r="X45" s="50"/>
-      <c r="Y45" s="51"/>
+      <c r="V45" s="51"/>
+      <c r="W45" s="51"/>
+      <c r="X45" s="51"/>
+      <c r="Y45" s="52"/>
       <c r="Z45" s="16">
         <v>0</v>
       </c>
@@ -4552,13 +4751,13 @@
       <c r="AB45" s="18">
         <v>1</v>
       </c>
-      <c r="AC45" s="49" t="s">
+      <c r="AC45" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD45" s="50"/>
-      <c r="AE45" s="50"/>
-      <c r="AF45" s="50"/>
-      <c r="AG45" s="51"/>
+      <c r="AD45" s="51"/>
+      <c r="AE45" s="51"/>
+      <c r="AF45" s="51"/>
+      <c r="AG45" s="52"/>
       <c r="AH45" s="32">
         <v>0</v>
       </c>
@@ -4580,11 +4779,11 @@
       <c r="AN45" s="36">
         <v>1</v>
       </c>
-      <c r="AP45" s="55" t="s">
+      <c r="AP45" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="AQ45" s="56"/>
-      <c r="AR45" s="47">
+      <c r="AQ45" s="57"/>
+      <c r="AR45" s="48">
         <v>1</v>
       </c>
       <c r="AS45" s="27">
@@ -4593,7 +4792,7 @@
       <c r="AT45" s="27">
         <v>0</v>
       </c>
-      <c r="AU45" s="48">
+      <c r="AU45" s="49">
         <v>1</v>
       </c>
       <c r="AW45" s="37">
@@ -4617,39 +4816,42 @@
       <c r="BC45" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD45" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="46" spans="3:55" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:56" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="53" t="s">
+      <c r="D46" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="E46" s="53"/>
+      <c r="E46" s="54"/>
       <c r="F46" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I46" s="54" t="s">
+      <c r="I46" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-      <c r="L46" s="50"/>
-      <c r="M46" s="50"/>
-      <c r="N46" s="50"/>
-      <c r="O46" s="50"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="50"/>
-      <c r="R46" s="50"/>
-      <c r="S46" s="50"/>
-      <c r="T46" s="51"/>
-      <c r="U46" s="49" t="s">
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
+      <c r="M46" s="51"/>
+      <c r="N46" s="51"/>
+      <c r="O46" s="51"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="51"/>
+      <c r="R46" s="51"/>
+      <c r="S46" s="51"/>
+      <c r="T46" s="52"/>
+      <c r="U46" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V46" s="50"/>
-      <c r="W46" s="50"/>
-      <c r="X46" s="50"/>
-      <c r="Y46" s="51"/>
+      <c r="V46" s="51"/>
+      <c r="W46" s="51"/>
+      <c r="X46" s="51"/>
+      <c r="Y46" s="52"/>
       <c r="Z46" s="16">
         <v>0</v>
       </c>
@@ -4659,39 +4861,39 @@
       <c r="AB46" s="18">
         <v>0</v>
       </c>
-      <c r="AC46" s="49" t="s">
+      <c r="AC46" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD46" s="50"/>
-      <c r="AE46" s="50"/>
-      <c r="AF46" s="50"/>
-      <c r="AG46" s="51"/>
-      <c r="AH46" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI46" s="43">
-        <v>0</v>
-      </c>
-      <c r="AJ46" s="43">
-        <v>0</v>
-      </c>
-      <c r="AK46" s="43">
-        <v>0</v>
-      </c>
-      <c r="AL46" s="43">
-        <v>0</v>
-      </c>
-      <c r="AM46" s="43">
-        <v>1</v>
-      </c>
-      <c r="AN46" s="46">
-        <v>1</v>
-      </c>
-      <c r="AP46" s="52" t="s">
+      <c r="AD46" s="51"/>
+      <c r="AE46" s="51"/>
+      <c r="AF46" s="51"/>
+      <c r="AG46" s="52"/>
+      <c r="AH46" s="46">
+        <v>0</v>
+      </c>
+      <c r="AI46" s="44">
+        <v>0</v>
+      </c>
+      <c r="AJ46" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL46" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM46" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN46" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP46" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ46" s="52"/>
-      <c r="AR46" s="47">
+      <c r="AQ46" s="53"/>
+      <c r="AR46" s="48">
         <v>0</v>
       </c>
       <c r="AS46" s="27">
@@ -4700,7 +4902,7 @@
       <c r="AT46" s="27">
         <v>1</v>
       </c>
-      <c r="AU46" s="48">
+      <c r="AU46" s="49">
         <v>1</v>
       </c>
       <c r="AW46" s="42">
@@ -4724,39 +4926,42 @@
       <c r="BC46" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BD46" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="47" spans="3:55" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:56" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="53" t="s">
+      <c r="D47" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="E47" s="53"/>
+      <c r="E47" s="54"/>
       <c r="F47" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I47" s="54" t="s">
+      <c r="I47" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J47" s="50"/>
-      <c r="K47" s="50"/>
-      <c r="L47" s="50"/>
-      <c r="M47" s="50"/>
-      <c r="N47" s="50"/>
-      <c r="O47" s="50"/>
-      <c r="P47" s="50"/>
-      <c r="Q47" s="50"/>
-      <c r="R47" s="50"/>
-      <c r="S47" s="50"/>
-      <c r="T47" s="51"/>
-      <c r="U47" s="49" t="s">
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="51"/>
+      <c r="R47" s="51"/>
+      <c r="S47" s="51"/>
+      <c r="T47" s="52"/>
+      <c r="U47" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V47" s="50"/>
-      <c r="W47" s="50"/>
-      <c r="X47" s="50"/>
-      <c r="Y47" s="51"/>
+      <c r="V47" s="51"/>
+      <c r="W47" s="51"/>
+      <c r="X47" s="51"/>
+      <c r="Y47" s="52"/>
       <c r="Z47" s="16">
         <v>0</v>
       </c>
@@ -4766,39 +4971,39 @@
       <c r="AB47" s="18">
         <v>1</v>
       </c>
-      <c r="AC47" s="49" t="s">
+      <c r="AC47" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD47" s="50"/>
-      <c r="AE47" s="50"/>
-      <c r="AF47" s="50"/>
-      <c r="AG47" s="51"/>
-      <c r="AH47" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI47" s="43">
-        <v>0</v>
-      </c>
-      <c r="AJ47" s="43">
-        <v>0</v>
-      </c>
-      <c r="AK47" s="43">
-        <v>0</v>
-      </c>
-      <c r="AL47" s="43">
-        <v>0</v>
-      </c>
-      <c r="AM47" s="43">
-        <v>1</v>
-      </c>
-      <c r="AN47" s="46">
-        <v>1</v>
-      </c>
-      <c r="AP47" s="52" t="s">
+      <c r="AD47" s="51"/>
+      <c r="AE47" s="51"/>
+      <c r="AF47" s="51"/>
+      <c r="AG47" s="52"/>
+      <c r="AH47" s="46">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="44">
+        <v>0</v>
+      </c>
+      <c r="AJ47" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL47" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM47" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN47" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP47" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ47" s="52"/>
-      <c r="AR47" s="47">
+      <c r="AQ47" s="53"/>
+      <c r="AR47" s="48">
         <v>0</v>
       </c>
       <c r="AS47" s="27">
@@ -4807,7 +5012,7 @@
       <c r="AT47" s="27">
         <v>1</v>
       </c>
-      <c r="AU47" s="48">
+      <c r="AU47" s="49">
         <v>1</v>
       </c>
       <c r="AW47" s="42">
@@ -4831,39 +5036,42 @@
       <c r="BC47" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BD47" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="48" spans="3:55" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:56" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="53" t="s">
+      <c r="D48" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="E48" s="53"/>
+      <c r="E48" s="54"/>
       <c r="F48" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I48" s="54" t="s">
+      <c r="I48" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J48" s="50"/>
-      <c r="K48" s="50"/>
-      <c r="L48" s="50"/>
-      <c r="M48" s="50"/>
-      <c r="N48" s="50"/>
-      <c r="O48" s="50"/>
-      <c r="P48" s="50"/>
-      <c r="Q48" s="50"/>
-      <c r="R48" s="50"/>
-      <c r="S48" s="50"/>
-      <c r="T48" s="51"/>
-      <c r="U48" s="49" t="s">
+      <c r="J48" s="51"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="51"/>
+      <c r="N48" s="51"/>
+      <c r="O48" s="51"/>
+      <c r="P48" s="51"/>
+      <c r="Q48" s="51"/>
+      <c r="R48" s="51"/>
+      <c r="S48" s="51"/>
+      <c r="T48" s="52"/>
+      <c r="U48" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V48" s="50"/>
-      <c r="W48" s="50"/>
-      <c r="X48" s="50"/>
-      <c r="Y48" s="51"/>
+      <c r="V48" s="51"/>
+      <c r="W48" s="51"/>
+      <c r="X48" s="51"/>
+      <c r="Y48" s="52"/>
       <c r="Z48" s="16">
         <v>0</v>
       </c>
@@ -4873,13 +5081,13 @@
       <c r="AB48" s="18">
         <v>0</v>
       </c>
-      <c r="AC48" s="49" t="s">
+      <c r="AC48" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD48" s="50"/>
-      <c r="AE48" s="50"/>
-      <c r="AF48" s="50"/>
-      <c r="AG48" s="51"/>
+      <c r="AD48" s="51"/>
+      <c r="AE48" s="51"/>
+      <c r="AF48" s="51"/>
+      <c r="AG48" s="52"/>
       <c r="AH48" s="8">
         <v>0</v>
       </c>
@@ -4901,10 +5109,10 @@
       <c r="AN48" s="15">
         <v>1</v>
       </c>
-      <c r="AP48" s="52" t="s">
+      <c r="AP48" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ48" s="52"/>
+      <c r="AQ48" s="53"/>
       <c r="AR48" s="26">
         <v>0</v>
       </c>
@@ -4938,39 +5146,42 @@
       <c r="BC48" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD48" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="49" spans="3:55" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:56" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D49" s="53" t="s">
+      <c r="D49" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="53"/>
+      <c r="E49" s="54"/>
       <c r="F49" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I49" s="54" t="s">
+      <c r="I49" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J49" s="50"/>
-      <c r="K49" s="50"/>
-      <c r="L49" s="50"/>
-      <c r="M49" s="50"/>
-      <c r="N49" s="50"/>
-      <c r="O49" s="50"/>
-      <c r="P49" s="50"/>
-      <c r="Q49" s="50"/>
-      <c r="R49" s="50"/>
-      <c r="S49" s="50"/>
-      <c r="T49" s="51"/>
-      <c r="U49" s="49" t="s">
+      <c r="J49" s="51"/>
+      <c r="K49" s="51"/>
+      <c r="L49" s="51"/>
+      <c r="M49" s="51"/>
+      <c r="N49" s="51"/>
+      <c r="O49" s="51"/>
+      <c r="P49" s="51"/>
+      <c r="Q49" s="51"/>
+      <c r="R49" s="51"/>
+      <c r="S49" s="51"/>
+      <c r="T49" s="52"/>
+      <c r="U49" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V49" s="50"/>
-      <c r="W49" s="50"/>
-      <c r="X49" s="50"/>
-      <c r="Y49" s="51"/>
+      <c r="V49" s="51"/>
+      <c r="W49" s="51"/>
+      <c r="X49" s="51"/>
+      <c r="Y49" s="52"/>
       <c r="Z49" s="16">
         <v>1</v>
       </c>
@@ -4980,39 +5191,39 @@
       <c r="AB49" s="18">
         <v>0</v>
       </c>
-      <c r="AC49" s="49" t="s">
+      <c r="AC49" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD49" s="50"/>
-      <c r="AE49" s="50"/>
-      <c r="AF49" s="50"/>
-      <c r="AG49" s="51"/>
-      <c r="AH49" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI49" s="43">
-        <v>0</v>
-      </c>
-      <c r="AJ49" s="43">
-        <v>0</v>
-      </c>
-      <c r="AK49" s="43">
-        <v>0</v>
-      </c>
-      <c r="AL49" s="43">
-        <v>0</v>
-      </c>
-      <c r="AM49" s="43">
-        <v>1</v>
-      </c>
-      <c r="AN49" s="46">
-        <v>1</v>
-      </c>
-      <c r="AP49" s="52" t="s">
+      <c r="AD49" s="51"/>
+      <c r="AE49" s="51"/>
+      <c r="AF49" s="51"/>
+      <c r="AG49" s="52"/>
+      <c r="AH49" s="46">
+        <v>0</v>
+      </c>
+      <c r="AI49" s="44">
+        <v>0</v>
+      </c>
+      <c r="AJ49" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK49" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL49" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM49" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN49" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP49" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ49" s="52"/>
-      <c r="AR49" s="47">
+      <c r="AQ49" s="53"/>
+      <c r="AR49" s="48">
         <v>0</v>
       </c>
       <c r="AS49" s="27">
@@ -5021,7 +5232,7 @@
       <c r="AT49" s="27">
         <v>1</v>
       </c>
-      <c r="AU49" s="48">
+      <c r="AU49" s="49">
         <v>1</v>
       </c>
       <c r="AW49" s="42">
@@ -5045,39 +5256,42 @@
       <c r="BC49" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BD49" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="50" spans="3:55" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:56" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="53" t="s">
+      <c r="D50" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="E50" s="53"/>
+      <c r="E50" s="54"/>
       <c r="F50" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I50" s="54" t="s">
+      <c r="I50" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J50" s="50"/>
-      <c r="K50" s="50"/>
-      <c r="L50" s="50"/>
-      <c r="M50" s="50"/>
-      <c r="N50" s="50"/>
-      <c r="O50" s="50"/>
-      <c r="P50" s="50"/>
-      <c r="Q50" s="50"/>
-      <c r="R50" s="50"/>
-      <c r="S50" s="50"/>
-      <c r="T50" s="51"/>
-      <c r="U50" s="49" t="s">
+      <c r="J50" s="51"/>
+      <c r="K50" s="51"/>
+      <c r="L50" s="51"/>
+      <c r="M50" s="51"/>
+      <c r="N50" s="51"/>
+      <c r="O50" s="51"/>
+      <c r="P50" s="51"/>
+      <c r="Q50" s="51"/>
+      <c r="R50" s="51"/>
+      <c r="S50" s="51"/>
+      <c r="T50" s="52"/>
+      <c r="U50" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V50" s="50"/>
-      <c r="W50" s="50"/>
-      <c r="X50" s="50"/>
-      <c r="Y50" s="51"/>
+      <c r="V50" s="51"/>
+      <c r="W50" s="51"/>
+      <c r="X50" s="51"/>
+      <c r="Y50" s="52"/>
       <c r="Z50" s="16">
         <v>1</v>
       </c>
@@ -5087,39 +5301,39 @@
       <c r="AB50" s="18">
         <v>1</v>
       </c>
-      <c r="AC50" s="49" t="s">
+      <c r="AC50" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD50" s="50"/>
-      <c r="AE50" s="50"/>
-      <c r="AF50" s="50"/>
-      <c r="AG50" s="51"/>
-      <c r="AH50" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI50" s="43">
-        <v>0</v>
-      </c>
-      <c r="AJ50" s="43">
-        <v>0</v>
-      </c>
-      <c r="AK50" s="43">
-        <v>0</v>
-      </c>
-      <c r="AL50" s="43">
-        <v>0</v>
-      </c>
-      <c r="AM50" s="43">
-        <v>1</v>
-      </c>
-      <c r="AN50" s="46">
-        <v>1</v>
-      </c>
-      <c r="AP50" s="52" t="s">
+      <c r="AD50" s="51"/>
+      <c r="AE50" s="51"/>
+      <c r="AF50" s="51"/>
+      <c r="AG50" s="52"/>
+      <c r="AH50" s="46">
+        <v>0</v>
+      </c>
+      <c r="AI50" s="44">
+        <v>0</v>
+      </c>
+      <c r="AJ50" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK50" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL50" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM50" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN50" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP50" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ50" s="52"/>
-      <c r="AR50" s="47">
+      <c r="AQ50" s="53"/>
+      <c r="AR50" s="48">
         <v>0</v>
       </c>
       <c r="AS50" s="27">
@@ -5128,7 +5342,7 @@
       <c r="AT50" s="27">
         <v>1</v>
       </c>
-      <c r="AU50" s="48">
+      <c r="AU50" s="49">
         <v>1</v>
       </c>
       <c r="AW50" s="42">
@@ -5152,39 +5366,42 @@
       <c r="BC50" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BD50" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="51" spans="3:55" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="53" t="s">
+      <c r="D51" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="E51" s="53"/>
+      <c r="E51" s="54"/>
       <c r="F51" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I51" s="54" t="s">
+      <c r="I51" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J51" s="50"/>
-      <c r="K51" s="50"/>
-      <c r="L51" s="50"/>
-      <c r="M51" s="50"/>
-      <c r="N51" s="50"/>
-      <c r="O51" s="50"/>
-      <c r="P51" s="50"/>
-      <c r="Q51" s="50"/>
-      <c r="R51" s="50"/>
-      <c r="S51" s="50"/>
-      <c r="T51" s="51"/>
-      <c r="U51" s="49" t="s">
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="51"/>
+      <c r="O51" s="51"/>
+      <c r="P51" s="51"/>
+      <c r="Q51" s="51"/>
+      <c r="R51" s="51"/>
+      <c r="S51" s="51"/>
+      <c r="T51" s="52"/>
+      <c r="U51" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V51" s="50"/>
-      <c r="W51" s="50"/>
-      <c r="X51" s="50"/>
-      <c r="Y51" s="51"/>
+      <c r="V51" s="51"/>
+      <c r="W51" s="51"/>
+      <c r="X51" s="51"/>
+      <c r="Y51" s="52"/>
       <c r="Z51" s="16">
         <v>0</v>
       </c>
@@ -5194,39 +5411,39 @@
       <c r="AB51" s="18">
         <v>0</v>
       </c>
-      <c r="AC51" s="49" t="s">
+      <c r="AC51" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD51" s="50"/>
-      <c r="AE51" s="50"/>
-      <c r="AF51" s="50"/>
-      <c r="AG51" s="51"/>
-      <c r="AH51" s="45">
-        <v>1</v>
-      </c>
-      <c r="AI51" s="43">
-        <v>1</v>
-      </c>
-      <c r="AJ51" s="43">
-        <v>0</v>
-      </c>
-      <c r="AK51" s="43">
-        <v>0</v>
-      </c>
-      <c r="AL51" s="43">
-        <v>1</v>
-      </c>
-      <c r="AM51" s="43">
-        <v>1</v>
-      </c>
-      <c r="AN51" s="46">
-        <v>1</v>
-      </c>
-      <c r="AP51" s="52" t="s">
+      <c r="AD51" s="51"/>
+      <c r="AE51" s="51"/>
+      <c r="AF51" s="51"/>
+      <c r="AG51" s="52"/>
+      <c r="AH51" s="46">
+        <v>1</v>
+      </c>
+      <c r="AI51" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ51" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK51" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL51" s="44">
+        <v>1</v>
+      </c>
+      <c r="AM51" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN51" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP51" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ51" s="52"/>
-      <c r="AR51" s="47">
+      <c r="AQ51" s="53"/>
+      <c r="AR51" s="48">
         <v>0</v>
       </c>
       <c r="AS51" s="27">
@@ -5235,7 +5452,7 @@
       <c r="AT51" s="27">
         <v>1</v>
       </c>
-      <c r="AU51" s="48">
+      <c r="AU51" s="49">
         <v>1</v>
       </c>
       <c r="AW51" s="42">
@@ -5253,89 +5470,92 @@
       <c r="BA51" s="42">
         <v>1</v>
       </c>
-      <c r="BB51" s="80" t="s">
+      <c r="BB51" s="79" t="s">
         <v>56</v>
       </c>
       <c r="BC51" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BD51" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="52" spans="3:55" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="53" t="s">
+      <c r="D52" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="E52" s="53"/>
+      <c r="E52" s="54"/>
       <c r="F52" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="54" t="s">
+      <c r="I52" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J52" s="50"/>
-      <c r="K52" s="50"/>
-      <c r="L52" s="50"/>
-      <c r="M52" s="50"/>
-      <c r="N52" s="50"/>
-      <c r="O52" s="51"/>
-      <c r="P52" s="49" t="s">
+      <c r="J52" s="51"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="51"/>
+      <c r="O52" s="52"/>
+      <c r="P52" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q52" s="50"/>
-      <c r="R52" s="50"/>
-      <c r="S52" s="50"/>
-      <c r="T52" s="51"/>
-      <c r="U52" s="49" t="s">
+      <c r="Q52" s="51"/>
+      <c r="R52" s="51"/>
+      <c r="S52" s="51"/>
+      <c r="T52" s="52"/>
+      <c r="U52" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V52" s="50"/>
-      <c r="W52" s="50"/>
-      <c r="X52" s="50"/>
-      <c r="Y52" s="51"/>
-      <c r="Z52" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA52" s="43">
-        <v>0</v>
-      </c>
-      <c r="AB52" s="44">
-        <v>1</v>
-      </c>
-      <c r="AC52" s="49" t="s">
+      <c r="V52" s="51"/>
+      <c r="W52" s="51"/>
+      <c r="X52" s="51"/>
+      <c r="Y52" s="52"/>
+      <c r="Z52" s="46">
+        <v>0</v>
+      </c>
+      <c r="AA52" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="45">
+        <v>1</v>
+      </c>
+      <c r="AC52" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="AD52" s="50"/>
-      <c r="AE52" s="50"/>
-      <c r="AF52" s="50"/>
-      <c r="AG52" s="51"/>
-      <c r="AH52" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI52" s="43">
-        <v>1</v>
-      </c>
-      <c r="AJ52" s="43">
-        <v>0</v>
-      </c>
-      <c r="AK52" s="43">
-        <v>0</v>
-      </c>
-      <c r="AL52" s="43">
-        <v>0</v>
-      </c>
-      <c r="AM52" s="43">
-        <v>1</v>
-      </c>
-      <c r="AN52" s="46">
-        <v>1</v>
-      </c>
-      <c r="AP52" s="52" t="s">
+      <c r="AD52" s="51"/>
+      <c r="AE52" s="51"/>
+      <c r="AF52" s="51"/>
+      <c r="AG52" s="52"/>
+      <c r="AH52" s="46">
+        <v>0</v>
+      </c>
+      <c r="AI52" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ52" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK52" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM52" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN52" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP52" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ52" s="52"/>
-      <c r="AR52" s="47">
+      <c r="AQ52" s="53"/>
+      <c r="AR52" s="48">
         <v>0</v>
       </c>
       <c r="AS52" s="27">
@@ -5344,7 +5564,7 @@
       <c r="AT52" s="27">
         <v>1</v>
       </c>
-      <c r="AU52" s="48">
+      <c r="AU52" s="49">
         <v>1</v>
       </c>
       <c r="AW52" s="42">
@@ -5368,83 +5588,86 @@
       <c r="BC52" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BD52" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="53" spans="3:55" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="53" t="s">
+      <c r="D53" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="E53" s="53"/>
+      <c r="E53" s="54"/>
       <c r="F53" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I53" s="54" t="s">
+      <c r="I53" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J53" s="50"/>
-      <c r="K53" s="50"/>
-      <c r="L53" s="50"/>
-      <c r="M53" s="50"/>
-      <c r="N53" s="50"/>
-      <c r="O53" s="51"/>
-      <c r="P53" s="49" t="s">
+      <c r="J53" s="51"/>
+      <c r="K53" s="51"/>
+      <c r="L53" s="51"/>
+      <c r="M53" s="51"/>
+      <c r="N53" s="51"/>
+      <c r="O53" s="52"/>
+      <c r="P53" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q53" s="50"/>
-      <c r="R53" s="50"/>
-      <c r="S53" s="50"/>
-      <c r="T53" s="51"/>
-      <c r="U53" s="49" t="s">
+      <c r="Q53" s="51"/>
+      <c r="R53" s="51"/>
+      <c r="S53" s="51"/>
+      <c r="T53" s="52"/>
+      <c r="U53" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V53" s="50"/>
-      <c r="W53" s="50"/>
-      <c r="X53" s="50"/>
-      <c r="Y53" s="51"/>
-      <c r="Z53" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA53" s="43">
-        <v>1</v>
-      </c>
-      <c r="AB53" s="44">
-        <v>0</v>
-      </c>
-      <c r="AC53" s="49" t="s">
+      <c r="V53" s="51"/>
+      <c r="W53" s="51"/>
+      <c r="X53" s="51"/>
+      <c r="Y53" s="52"/>
+      <c r="Z53" s="46">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="44">
+        <v>1</v>
+      </c>
+      <c r="AB53" s="45">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="AD53" s="50"/>
-      <c r="AE53" s="50"/>
-      <c r="AF53" s="50"/>
-      <c r="AG53" s="51"/>
-      <c r="AH53" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI53" s="43">
-        <v>1</v>
-      </c>
-      <c r="AJ53" s="43">
-        <v>0</v>
-      </c>
-      <c r="AK53" s="43">
-        <v>0</v>
-      </c>
-      <c r="AL53" s="43">
-        <v>0</v>
-      </c>
-      <c r="AM53" s="43">
-        <v>1</v>
-      </c>
-      <c r="AN53" s="46">
-        <v>1</v>
-      </c>
-      <c r="AP53" s="52" t="s">
+      <c r="AD53" s="51"/>
+      <c r="AE53" s="51"/>
+      <c r="AF53" s="51"/>
+      <c r="AG53" s="52"/>
+      <c r="AH53" s="46">
+        <v>0</v>
+      </c>
+      <c r="AI53" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ53" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL53" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM53" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN53" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP53" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ53" s="52"/>
-      <c r="AR53" s="47">
+      <c r="AQ53" s="53"/>
+      <c r="AR53" s="48">
         <v>0</v>
       </c>
       <c r="AS53" s="27">
@@ -5453,7 +5676,7 @@
       <c r="AT53" s="27">
         <v>1</v>
       </c>
-      <c r="AU53" s="48">
+      <c r="AU53" s="49">
         <v>1</v>
       </c>
       <c r="AW53" s="42">
@@ -5477,41 +5700,44 @@
       <c r="BC53" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BD53" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="54" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="53" t="s">
+      <c r="D54" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="E54" s="53"/>
+      <c r="E54" s="54"/>
       <c r="F54" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I54" s="54" t="s">
+      <c r="I54" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="J54" s="50"/>
-      <c r="K54" s="50"/>
-      <c r="L54" s="50"/>
-      <c r="M54" s="50"/>
-      <c r="N54" s="50"/>
-      <c r="O54" s="51"/>
-      <c r="P54" s="49" t="s">
+      <c r="J54" s="51"/>
+      <c r="K54" s="51"/>
+      <c r="L54" s="51"/>
+      <c r="M54" s="51"/>
+      <c r="N54" s="51"/>
+      <c r="O54" s="52"/>
+      <c r="P54" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q54" s="50"/>
-      <c r="R54" s="50"/>
-      <c r="S54" s="50"/>
-      <c r="T54" s="51"/>
-      <c r="U54" s="49" t="s">
+      <c r="Q54" s="51"/>
+      <c r="R54" s="51"/>
+      <c r="S54" s="51"/>
+      <c r="T54" s="52"/>
+      <c r="U54" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V54" s="50"/>
-      <c r="W54" s="50"/>
-      <c r="X54" s="50"/>
-      <c r="Y54" s="51"/>
+      <c r="V54" s="51"/>
+      <c r="W54" s="51"/>
+      <c r="X54" s="51"/>
+      <c r="Y54" s="52"/>
       <c r="Z54" s="8">
         <v>0</v>
       </c>
@@ -5521,13 +5747,13 @@
       <c r="AB54" s="10">
         <v>0</v>
       </c>
-      <c r="AC54" s="49" t="s">
+      <c r="AC54" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="AD54" s="50"/>
-      <c r="AE54" s="50"/>
-      <c r="AF54" s="50"/>
-      <c r="AG54" s="51"/>
+      <c r="AD54" s="51"/>
+      <c r="AE54" s="51"/>
+      <c r="AF54" s="51"/>
+      <c r="AG54" s="52"/>
       <c r="AH54" s="8">
         <v>0</v>
       </c>
@@ -5549,10 +5775,10 @@
       <c r="AN54" s="15">
         <v>1</v>
       </c>
-      <c r="AP54" s="52" t="s">
+      <c r="AP54" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ54" s="52"/>
+      <c r="AQ54" s="53"/>
       <c r="AR54" s="26">
         <v>0</v>
       </c>
@@ -5586,40 +5812,46 @@
       <c r="BC54" s="37" t="s">
         <v>50</v>
       </c>
+      <c r="BD54" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="55" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="53" t="s">
+    <row r="55" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="E55" s="53"/>
+      <c r="E55" s="54"/>
       <c r="F55" s="29" t="s">
         <v>37</v>
       </c>
       <c r="I55" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J55" s="54" t="s">
+      <c r="J55" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="K55" s="50"/>
-      <c r="L55" s="50"/>
-      <c r="M55" s="50"/>
-      <c r="N55" s="50"/>
-      <c r="O55" s="51"/>
-      <c r="P55" s="49" t="s">
+      <c r="K55" s="51"/>
+      <c r="L55" s="51"/>
+      <c r="M55" s="51"/>
+      <c r="N55" s="51"/>
+      <c r="O55" s="52"/>
+      <c r="P55" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="Q55" s="50"/>
-      <c r="R55" s="50"/>
-      <c r="S55" s="50"/>
-      <c r="T55" s="51"/>
-      <c r="U55" s="49" t="s">
+      <c r="Q55" s="51"/>
+      <c r="R55" s="51"/>
+      <c r="S55" s="51"/>
+      <c r="T55" s="52"/>
+      <c r="U55" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="V55" s="50"/>
-      <c r="W55" s="50"/>
-      <c r="X55" s="50"/>
-      <c r="Y55" s="51"/>
+      <c r="V55" s="51"/>
+      <c r="W55" s="51"/>
+      <c r="X55" s="51"/>
+      <c r="Y55" s="52"/>
       <c r="Z55" s="8">
         <v>0</v>
       </c>
@@ -5629,12 +5861,12 @@
       <c r="AB55" s="10">
         <v>0</v>
       </c>
-      <c r="AC55" s="49" t="s">
+      <c r="AC55" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="AD55" s="50"/>
-      <c r="AE55" s="50"/>
-      <c r="AF55" s="51"/>
+      <c r="AD55" s="51"/>
+      <c r="AE55" s="51"/>
+      <c r="AF55" s="52"/>
       <c r="AG55" s="10" t="s">
         <v>15</v>
       </c>
@@ -5659,10 +5891,10 @@
       <c r="AN55" s="15">
         <v>1</v>
       </c>
-      <c r="AP55" s="52" t="s">
+      <c r="AP55" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="AQ55" s="52"/>
+      <c r="AQ55" s="53"/>
       <c r="AR55" s="26">
         <v>0</v>
       </c>
@@ -5696,111 +5928,715 @@
       <c r="BC55" s="37" t="s">
         <v>51</v>
       </c>
+      <c r="BD55" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="56" spans="3:55" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="53" t="s">
+    <row r="56" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" s="54"/>
+      <c r="F56" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I56" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="J56" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="K56" s="51"/>
+      <c r="L56" s="51"/>
+      <c r="M56" s="51"/>
+      <c r="N56" s="51"/>
+      <c r="O56" s="52"/>
+      <c r="P56" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q56" s="51"/>
+      <c r="R56" s="51"/>
+      <c r="S56" s="51"/>
+      <c r="T56" s="52"/>
+      <c r="U56" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="V56" s="51"/>
+      <c r="W56" s="51"/>
+      <c r="X56" s="51"/>
+      <c r="Y56" s="52"/>
+      <c r="Z56" s="46">
+        <v>0</v>
+      </c>
+      <c r="AA56" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB56" s="45">
+        <v>1</v>
+      </c>
+      <c r="AC56" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD56" s="51"/>
+      <c r="AE56" s="51"/>
+      <c r="AF56" s="52"/>
+      <c r="AG56" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH56" s="46">
+        <v>1</v>
+      </c>
+      <c r="AI56" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ56" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK56" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL56" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM56" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN56" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP56" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ56" s="57"/>
+      <c r="AR56" s="48">
+        <v>0</v>
+      </c>
+      <c r="AS56" s="27">
+        <v>1</v>
+      </c>
+      <c r="AT56" s="27">
+        <v>0</v>
+      </c>
+      <c r="AU56" s="49">
+        <v>0</v>
+      </c>
+      <c r="AW56" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX56" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY56" s="42">
+        <v>0</v>
+      </c>
+      <c r="AZ56" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA56" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB56" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC56" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="BD56" s="42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="54"/>
+      <c r="F57" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I57" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="J57" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="K57" s="51"/>
+      <c r="L57" s="51"/>
+      <c r="M57" s="51"/>
+      <c r="N57" s="51"/>
+      <c r="O57" s="52"/>
+      <c r="P57" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q57" s="51"/>
+      <c r="R57" s="51"/>
+      <c r="S57" s="51"/>
+      <c r="T57" s="52"/>
+      <c r="U57" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="V57" s="51"/>
+      <c r="W57" s="51"/>
+      <c r="X57" s="51"/>
+      <c r="Y57" s="52"/>
+      <c r="Z57" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA57" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="45">
+        <v>0</v>
+      </c>
+      <c r="AC57" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD57" s="51"/>
+      <c r="AE57" s="51"/>
+      <c r="AF57" s="52"/>
+      <c r="AG57" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH57" s="46">
+        <v>1</v>
+      </c>
+      <c r="AI57" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ57" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK57" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL57" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM57" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN57" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP57" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ57" s="53"/>
+      <c r="AR57" s="48">
+        <v>0</v>
+      </c>
+      <c r="AS57" s="27">
+        <v>1</v>
+      </c>
+      <c r="AT57" s="27">
+        <v>0</v>
+      </c>
+      <c r="AU57" s="49">
+        <v>1</v>
+      </c>
+      <c r="AW57" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX57" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY57" s="42">
+        <v>0</v>
+      </c>
+      <c r="AZ57" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA57" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB57" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC57" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD57" s="42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D58" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" s="54"/>
+      <c r="F58" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I58" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="J58" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="K58" s="51"/>
+      <c r="L58" s="51"/>
+      <c r="M58" s="51"/>
+      <c r="N58" s="51"/>
+      <c r="O58" s="52"/>
+      <c r="P58" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q58" s="51"/>
+      <c r="R58" s="51"/>
+      <c r="S58" s="51"/>
+      <c r="T58" s="52"/>
+      <c r="U58" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="V58" s="51"/>
+      <c r="W58" s="51"/>
+      <c r="X58" s="51"/>
+      <c r="Y58" s="52"/>
+      <c r="Z58" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA58" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB58" s="45">
+        <v>1</v>
+      </c>
+      <c r="AC58" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD58" s="51"/>
+      <c r="AE58" s="51"/>
+      <c r="AF58" s="52"/>
+      <c r="AG58" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH58" s="46">
+        <v>1</v>
+      </c>
+      <c r="AI58" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ58" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK58" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL58" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM58" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN58" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP58" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ58" s="53"/>
+      <c r="AR58" s="48">
+        <v>0</v>
+      </c>
+      <c r="AS58" s="27">
+        <v>1</v>
+      </c>
+      <c r="AT58" s="27">
+        <v>0</v>
+      </c>
+      <c r="AU58" s="49">
+        <v>1</v>
+      </c>
+      <c r="AW58" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX58" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY58" s="42">
+        <v>0</v>
+      </c>
+      <c r="AZ58" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA58" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB58" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC58" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD58" s="42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" s="54"/>
+      <c r="F59" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I59" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="J59" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="K59" s="51"/>
+      <c r="L59" s="51"/>
+      <c r="M59" s="51"/>
+      <c r="N59" s="51"/>
+      <c r="O59" s="52"/>
+      <c r="P59" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q59" s="51"/>
+      <c r="R59" s="51"/>
+      <c r="S59" s="51"/>
+      <c r="T59" s="52"/>
+      <c r="U59" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="V59" s="51"/>
+      <c r="W59" s="51"/>
+      <c r="X59" s="51"/>
+      <c r="Y59" s="52"/>
+      <c r="Z59" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA59" s="44">
+        <v>1</v>
+      </c>
+      <c r="AB59" s="45">
+        <v>0</v>
+      </c>
+      <c r="AC59" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD59" s="51"/>
+      <c r="AE59" s="51"/>
+      <c r="AF59" s="52"/>
+      <c r="AG59" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH59" s="46">
+        <v>1</v>
+      </c>
+      <c r="AI59" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ59" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK59" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL59" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM59" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN59" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP59" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ59" s="57"/>
+      <c r="AR59" s="48">
+        <v>1</v>
+      </c>
+      <c r="AS59" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT59" s="27">
+        <v>0</v>
+      </c>
+      <c r="AU59" s="49">
+        <v>1</v>
+      </c>
+      <c r="AW59" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX59" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY59" s="42">
+        <v>0</v>
+      </c>
+      <c r="AZ59" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA59" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB59" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC59" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD59" s="42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="54"/>
+      <c r="F60" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I60" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="J60" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="K60" s="51"/>
+      <c r="L60" s="51"/>
+      <c r="M60" s="51"/>
+      <c r="N60" s="51"/>
+      <c r="O60" s="52"/>
+      <c r="P60" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q60" s="51"/>
+      <c r="R60" s="51"/>
+      <c r="S60" s="51"/>
+      <c r="T60" s="52"/>
+      <c r="U60" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="V60" s="51"/>
+      <c r="W60" s="51"/>
+      <c r="X60" s="51"/>
+      <c r="Y60" s="52"/>
+      <c r="Z60" s="46">
+        <v>1</v>
+      </c>
+      <c r="AA60" s="44">
+        <v>1</v>
+      </c>
+      <c r="AB60" s="45">
+        <v>1</v>
+      </c>
+      <c r="AC60" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD60" s="51"/>
+      <c r="AE60" s="51"/>
+      <c r="AF60" s="52"/>
+      <c r="AG60" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH60" s="46">
+        <v>1</v>
+      </c>
+      <c r="AI60" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ60" s="44">
+        <v>0</v>
+      </c>
+      <c r="AK60" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL60" s="44">
+        <v>0</v>
+      </c>
+      <c r="AM60" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN60" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP60" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ60" s="57"/>
+      <c r="AR60" s="48">
+        <v>1</v>
+      </c>
+      <c r="AS60" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT60" s="27">
+        <v>0</v>
+      </c>
+      <c r="AU60" s="49">
+        <v>1</v>
+      </c>
+      <c r="AW60" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX60" s="42">
+        <v>0</v>
+      </c>
+      <c r="AY60" s="42">
+        <v>0</v>
+      </c>
+      <c r="AZ60" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA60" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB60" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC60" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD60" s="42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D61" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="E56" s="53"/>
-      <c r="F56" s="30" t="s">
+      <c r="E61" s="54"/>
+      <c r="F61" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="I56" s="6" t="s">
+      <c r="I61" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J56" s="49" t="s">
+      <c r="J61" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="K56" s="50"/>
-      <c r="L56" s="50"/>
-      <c r="M56" s="50"/>
-      <c r="N56" s="50"/>
-      <c r="O56" s="50"/>
-      <c r="P56" s="50"/>
-      <c r="Q56" s="50"/>
-      <c r="R56" s="50"/>
-      <c r="S56" s="50"/>
-      <c r="T56" s="7" t="s">
+      <c r="K61" s="51"/>
+      <c r="L61" s="51"/>
+      <c r="M61" s="51"/>
+      <c r="N61" s="51"/>
+      <c r="O61" s="51"/>
+      <c r="P61" s="51"/>
+      <c r="Q61" s="51"/>
+      <c r="R61" s="51"/>
+      <c r="S61" s="51"/>
+      <c r="T61" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="U56" s="49" t="s">
+      <c r="U61" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="V56" s="50"/>
-      <c r="W56" s="50"/>
-      <c r="X56" s="50"/>
-      <c r="Y56" s="50"/>
-      <c r="Z56" s="50"/>
-      <c r="AA56" s="50"/>
-      <c r="AB56" s="51"/>
-      <c r="AC56" s="49" t="s">
+      <c r="V61" s="51"/>
+      <c r="W61" s="51"/>
+      <c r="X61" s="51"/>
+      <c r="Y61" s="51"/>
+      <c r="Z61" s="51"/>
+      <c r="AA61" s="51"/>
+      <c r="AB61" s="52"/>
+      <c r="AC61" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="AD56" s="50"/>
-      <c r="AE56" s="50"/>
-      <c r="AF56" s="50"/>
-      <c r="AG56" s="51"/>
-      <c r="AH56" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI56" s="9">
-        <v>1</v>
-      </c>
-      <c r="AJ56" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK56" s="9">
-        <v>1</v>
-      </c>
-      <c r="AL56" s="9">
-        <v>1</v>
-      </c>
-      <c r="AM56" s="9">
-        <v>1</v>
-      </c>
-      <c r="AN56" s="15">
-        <v>1</v>
-      </c>
-      <c r="AP56" s="52" t="s">
+      <c r="AD61" s="51"/>
+      <c r="AE61" s="51"/>
+      <c r="AF61" s="51"/>
+      <c r="AG61" s="52"/>
+      <c r="AH61" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI61" s="9">
+        <v>1</v>
+      </c>
+      <c r="AJ61" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK61" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL61" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM61" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN61" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP61" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="AQ56" s="52"/>
-      <c r="AR56" s="26">
-        <v>0</v>
-      </c>
-      <c r="AS56" s="27">
-        <v>0</v>
-      </c>
-      <c r="AT56" s="27">
-        <v>1</v>
-      </c>
-      <c r="AU56" s="28">
-        <v>1</v>
-      </c>
-      <c r="AW56" s="37">
-        <v>0</v>
-      </c>
-      <c r="AX56" s="37">
-        <v>1</v>
-      </c>
-      <c r="AY56" s="37">
-        <v>1</v>
-      </c>
-      <c r="AZ56" s="37">
-        <v>0</v>
-      </c>
-      <c r="BA56" s="42">
-        <v>0</v>
-      </c>
-      <c r="BB56" s="41" t="s">
+      <c r="AQ61" s="53"/>
+      <c r="AR61" s="26">
+        <v>0</v>
+      </c>
+      <c r="AS61" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT61" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU61" s="28">
+        <v>1</v>
+      </c>
+      <c r="AW61" s="37">
+        <v>0</v>
+      </c>
+      <c r="AX61" s="37">
+        <v>1</v>
+      </c>
+      <c r="AY61" s="37">
+        <v>1</v>
+      </c>
+      <c r="AZ61" s="37">
+        <v>0</v>
+      </c>
+      <c r="BA61" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB61" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="BC56" s="37" t="s">
+      <c r="BC61" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD61" s="42" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="203">
+  <mergeCells count="233">
+    <mergeCell ref="AC60:AF60"/>
+    <mergeCell ref="AP60:AQ60"/>
+    <mergeCell ref="AP57:AQ57"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="J59:O59"/>
+    <mergeCell ref="P59:T59"/>
+    <mergeCell ref="U59:Y59"/>
+    <mergeCell ref="AC59:AF59"/>
+    <mergeCell ref="AP59:AQ59"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="J58:O58"/>
+    <mergeCell ref="P58:T58"/>
+    <mergeCell ref="U58:Y58"/>
+    <mergeCell ref="AC58:AF58"/>
+    <mergeCell ref="AP58:AQ58"/>
     <mergeCell ref="AP53:AQ53"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="I52:O52"/>
@@ -5808,6 +6644,12 @@
     <mergeCell ref="U52:Y52"/>
     <mergeCell ref="AC52:AG52"/>
     <mergeCell ref="AP52:AQ52"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="J56:O56"/>
+    <mergeCell ref="P56:T56"/>
+    <mergeCell ref="U56:Y56"/>
+    <mergeCell ref="AC56:AF56"/>
+    <mergeCell ref="AP56:AQ56"/>
     <mergeCell ref="AP50:AQ50"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="I49:T49"/>
@@ -5832,7 +6674,7 @@
     <mergeCell ref="AP46:AQ46"/>
     <mergeCell ref="AP54:AQ54"/>
     <mergeCell ref="AP55:AQ55"/>
-    <mergeCell ref="AP56:AQ56"/>
+    <mergeCell ref="AP61:AQ61"/>
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="I8:O8"/>
     <mergeCell ref="P8:T8"/>
@@ -5915,10 +6757,10 @@
     <mergeCell ref="P53:T53"/>
     <mergeCell ref="U53:Y53"/>
     <mergeCell ref="AC53:AG53"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="J56:S56"/>
-    <mergeCell ref="U56:AB56"/>
-    <mergeCell ref="AC56:AG56"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="J61:S61"/>
+    <mergeCell ref="U61:AB61"/>
+    <mergeCell ref="AC61:AG61"/>
     <mergeCell ref="I54:O54"/>
     <mergeCell ref="P54:T54"/>
     <mergeCell ref="U54:Y54"/>
@@ -5930,6 +6772,15 @@
     <mergeCell ref="U55:Y55"/>
     <mergeCell ref="AC55:AF55"/>
     <mergeCell ref="J55:O55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="J57:O57"/>
+    <mergeCell ref="P57:T57"/>
+    <mergeCell ref="U57:Y57"/>
+    <mergeCell ref="AC57:AF57"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="J60:O60"/>
+    <mergeCell ref="P60:T60"/>
+    <mergeCell ref="U60:Y60"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D32:E32"/>

</xml_diff>

<commit_message>
all instructions implemented (barring env related calls) and added elab schematic from Vivado
</commit_message>
<xml_diff>
--- a/doc/decoding.xlsx
+++ b/doc/decoding.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\SystemVerilog\FRiscV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA0ABE4-8DF5-4029-9845-00B393702DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099E24FC-E29E-4688-9CF3-D5AA25210C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29205" yWindow="345" windowWidth="25965" windowHeight="14595" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
+    <workbookView xWindow="28215" yWindow="2565" windowWidth="25965" windowHeight="14595" xr2:uid="{D316FFA2-481E-4588-99DB-346029B926A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$27:$BC$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$27:$BD$36</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -243,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="87">
   <si>
     <t>R-TYPE</t>
   </si>
@@ -492,6 +492,18 @@
   </si>
   <si>
     <t>Uses  LT?</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>LUI</t>
+  </si>
+  <si>
+    <t>AUIPC</t>
+  </si>
+  <si>
+    <t>auipc</t>
   </si>
 </sst>
 </file>
@@ -547,7 +559,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -593,6 +605,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -891,7 +909,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1124,6 +1142,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1440,13 +1461,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA95D64-5055-4174-A4D5-0BDBECB18FB0}">
-  <dimension ref="C1:BD61"/>
+  <dimension ref="C1:BE63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="7" ySplit="23" topLeftCell="H45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="23" topLeftCell="H47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
-      <selection pane="bottomRight" activeCell="C62" sqref="C62"/>
+      <selection pane="bottomRight" activeCell="BD65" sqref="BD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="14.25" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -1465,10 +1486,11 @@
     <col min="51" max="51" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="57" max="16384" width="4.7109375" style="3"/>
+    <col min="54" max="54" width="8.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="58" max="16384" width="4.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:47" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -2207,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:56" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:57" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="66" t="s">
         <v>3</v>
       </c>
@@ -2263,7 +2285,7 @@
       <c r="AM17" s="51"/>
       <c r="AN17" s="62"/>
     </row>
-    <row r="18" spans="3:56" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:57" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -2301,7 +2323,7 @@
       <c r="AM18" s="4"/>
       <c r="AN18" s="4"/>
     </row>
-    <row r="19" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -2325,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:56" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:57" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D20" s="63" t="s">
         <v>4</v>
       </c>
@@ -2371,7 +2393,7 @@
       <c r="AM20" s="51"/>
       <c r="AN20" s="62"/>
     </row>
-    <row r="21" spans="3:56" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:57" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -2409,7 +2431,7 @@
       <c r="AM21" s="4"/>
       <c r="AN21" s="4"/>
     </row>
-    <row r="22" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -2451,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:56" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:57" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="64" t="s">
         <v>5</v>
       </c>
@@ -2503,7 +2525,7 @@
       <c r="AM23" s="51"/>
       <c r="AN23" s="62"/>
     </row>
-    <row r="25" spans="3:56" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:57" ht="15" x14ac:dyDescent="0.25">
       <c r="AW25" s="67" t="s">
         <v>48</v>
       </c>
@@ -2512,8 +2534,9 @@
       <c r="AZ25" s="67"/>
       <c r="BA25" s="67"/>
       <c r="BB25" s="67"/>
+      <c r="BC25" s="67"/>
     </row>
-    <row r="26" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="31" t="s">
         <v>57</v>
       </c>
@@ -2540,17 +2563,20 @@
       <c r="BA26" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="BB26" s="39" t="s">
+      <c r="BB26" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC26" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="BC26" s="39" t="s">
+      <c r="BD26" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="BD26" s="39" t="s">
+      <c r="BE26" s="39" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
@@ -2664,17 +2690,20 @@
       <c r="BA27" s="42">
         <v>0</v>
       </c>
-      <c r="BB27" s="40" t="s">
+      <c r="BB27" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC27" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC27" s="37" t="s">
+      <c r="BD27" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD27" s="42" t="s">
+      <c r="BE27" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
         <v>51</v>
       </c>
@@ -2788,17 +2817,20 @@
       <c r="BA28" s="42">
         <v>0</v>
       </c>
-      <c r="BB28" s="40" t="s">
+      <c r="BB28" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC28" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC28" s="37" t="s">
+      <c r="BD28" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD28" s="42" t="s">
+      <c r="BE28" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="3" t="s">
         <v>51</v>
       </c>
@@ -2912,17 +2944,20 @@
       <c r="BA29" s="42">
         <v>0</v>
       </c>
-      <c r="BB29" s="40" t="s">
+      <c r="BB29" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC29" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC29" s="37" t="s">
+      <c r="BD29" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD29" s="42" t="s">
+      <c r="BE29" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
         <v>51</v>
       </c>
@@ -3036,17 +3071,20 @@
       <c r="BA30" s="42">
         <v>0</v>
       </c>
-      <c r="BB30" s="40" t="s">
+      <c r="BB30" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC30" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC30" s="37" t="s">
+      <c r="BD30" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD30" s="42" t="s">
+      <c r="BE30" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
         <v>51</v>
       </c>
@@ -3160,17 +3198,20 @@
       <c r="BA31" s="42">
         <v>0</v>
       </c>
-      <c r="BB31" s="40" t="s">
+      <c r="BB31" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC31" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC31" s="37" t="s">
+      <c r="BD31" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD31" s="42" t="s">
+      <c r="BE31" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3" t="s">
         <v>51</v>
       </c>
@@ -3284,17 +3325,20 @@
       <c r="BA32" s="42">
         <v>0</v>
       </c>
-      <c r="BB32" s="40" t="s">
+      <c r="BB32" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC32" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC32" s="37" t="s">
+      <c r="BD32" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD32" s="42" t="s">
+      <c r="BE32" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
@@ -3408,17 +3452,20 @@
       <c r="BA33" s="42">
         <v>0</v>
       </c>
-      <c r="BB33" s="40" t="s">
+      <c r="BB33" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC33" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC33" s="37" t="s">
+      <c r="BD33" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD33" s="42" t="s">
+      <c r="BE33" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3" t="s">
         <v>51</v>
       </c>
@@ -3532,17 +3579,20 @@
       <c r="BA34" s="42">
         <v>0</v>
       </c>
-      <c r="BB34" s="40" t="s">
+      <c r="BB34" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC34" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC34" s="37" t="s">
+      <c r="BD34" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD34" s="42" t="s">
+      <c r="BE34" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
         <v>51</v>
       </c>
@@ -3656,17 +3706,20 @@
       <c r="BA35" s="42">
         <v>0</v>
       </c>
-      <c r="BB35" s="40" t="s">
+      <c r="BB35" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC35" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC35" s="37" t="s">
+      <c r="BD35" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD35" s="42" t="s">
+      <c r="BE35" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="3" t="s">
         <v>51</v>
       </c>
@@ -3780,17 +3833,20 @@
       <c r="BA36" s="42">
         <v>0</v>
       </c>
-      <c r="BB36" s="40" t="s">
+      <c r="BB36" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC36" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC36" s="37" t="s">
+      <c r="BD36" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD36" s="42" t="s">
+      <c r="BE36" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="3:56" ht="15.75" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:57" ht="15.75" outlineLevel="1" collapsed="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="3" t="s">
         <v>51</v>
       </c>
@@ -3890,17 +3946,20 @@
       <c r="BA37" s="42">
         <v>0</v>
       </c>
-      <c r="BB37" s="40" t="s">
+      <c r="BB37" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC37" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC37" s="37" t="s">
+      <c r="BD37" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD37" s="42" t="s">
+      <c r="BE37" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="3" t="s">
         <v>51</v>
       </c>
@@ -4000,17 +4059,20 @@
       <c r="BA38" s="42">
         <v>0</v>
       </c>
-      <c r="BB38" s="40" t="s">
+      <c r="BB38" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC38" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC38" s="37" t="s">
+      <c r="BD38" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD38" s="42" t="s">
+      <c r="BE38" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="3" t="s">
         <v>51</v>
       </c>
@@ -4110,17 +4172,20 @@
       <c r="BA39" s="42">
         <v>0</v>
       </c>
-      <c r="BB39" s="40" t="s">
+      <c r="BB39" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC39" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC39" s="37" t="s">
+      <c r="BD39" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD39" s="42" t="s">
+      <c r="BE39" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="3" t="s">
         <v>51</v>
       </c>
@@ -4220,17 +4285,20 @@
       <c r="BA40" s="42">
         <v>0</v>
       </c>
-      <c r="BB40" s="40" t="s">
+      <c r="BB40" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC40" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC40" s="37" t="s">
+      <c r="BD40" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD40" s="42" t="s">
+      <c r="BE40" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="3" t="s">
         <v>51</v>
       </c>
@@ -4344,17 +4412,20 @@
       <c r="BA41" s="42">
         <v>0</v>
       </c>
-      <c r="BB41" s="40" t="s">
+      <c r="BB41" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC41" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC41" s="37" t="s">
+      <c r="BD41" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD41" s="42" t="s">
+      <c r="BE41" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="3" t="s">
         <v>51</v>
       </c>
@@ -4468,17 +4539,20 @@
       <c r="BA42" s="42">
         <v>0</v>
       </c>
-      <c r="BB42" s="40" t="s">
+      <c r="BB42" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC42" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC42" s="37" t="s">
+      <c r="BD42" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD42" s="42" t="s">
+      <c r="BE42" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="3" t="s">
         <v>51</v>
       </c>
@@ -4592,17 +4666,20 @@
       <c r="BA43" s="42">
         <v>0</v>
       </c>
-      <c r="BB43" s="40" t="s">
+      <c r="BB43" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC43" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC43" s="37" t="s">
+      <c r="BD43" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD43" s="42" t="s">
+      <c r="BE43" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="3" t="s">
         <v>51</v>
       </c>
@@ -4702,17 +4779,20 @@
       <c r="BA44" s="42">
         <v>0</v>
       </c>
-      <c r="BB44" s="40" t="s">
+      <c r="BB44" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC44" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC44" s="37" t="s">
+      <c r="BD44" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD44" s="42" t="s">
+      <c r="BE44" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="3:56" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:57" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="3" t="s">
         <v>51</v>
       </c>
@@ -4810,17 +4890,20 @@
       <c r="BA45" s="42">
         <v>0</v>
       </c>
-      <c r="BB45" s="40" t="s">
+      <c r="BB45" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC45" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC45" s="37" t="s">
+      <c r="BD45" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD45" s="42" t="s">
+      <c r="BE45" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="3:56" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:57" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="3" t="s">
         <v>51</v>
       </c>
@@ -4920,17 +5003,20 @@
       <c r="BA46" s="42">
         <v>0</v>
       </c>
-      <c r="BB46" s="40" t="s">
+      <c r="BB46" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC46" s="40" t="s">
         <v>55</v>
-      </c>
-      <c r="BC46" s="42" t="s">
-        <v>50</v>
       </c>
       <c r="BD46" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BE46" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="47" spans="3:56" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:57" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="3" t="s">
         <v>51</v>
       </c>
@@ -5030,17 +5116,20 @@
       <c r="BA47" s="42">
         <v>0</v>
       </c>
-      <c r="BB47" s="40" t="s">
+      <c r="BB47" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC47" s="40" t="s">
         <v>55</v>
-      </c>
-      <c r="BC47" s="42" t="s">
-        <v>50</v>
       </c>
       <c r="BD47" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BE47" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="48" spans="3:56" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:57" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="3" t="s">
         <v>51</v>
       </c>
@@ -5140,17 +5229,20 @@
       <c r="BA48" s="42">
         <v>0</v>
       </c>
-      <c r="BB48" s="40" t="s">
+      <c r="BB48" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC48" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="BC48" s="37" t="s">
+      <c r="BD48" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD48" s="42" t="s">
+      <c r="BE48" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="3:56" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:57" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="3" t="s">
         <v>51</v>
       </c>
@@ -5250,17 +5342,20 @@
       <c r="BA49" s="42">
         <v>0</v>
       </c>
-      <c r="BB49" s="40" t="s">
+      <c r="BB49" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC49" s="40" t="s">
         <v>55</v>
-      </c>
-      <c r="BC49" s="42" t="s">
-        <v>50</v>
       </c>
       <c r="BD49" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BE49" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="50" spans="3:56" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:57" ht="15.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="3" t="s">
         <v>51</v>
       </c>
@@ -5360,17 +5455,20 @@
       <c r="BA50" s="42">
         <v>0</v>
       </c>
-      <c r="BB50" s="40" t="s">
+      <c r="BB50" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC50" s="40" t="s">
         <v>55</v>
-      </c>
-      <c r="BC50" s="42" t="s">
-        <v>50</v>
       </c>
       <c r="BD50" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BE50" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="51" spans="3:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:57" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="3" t="s">
         <v>51</v>
       </c>
@@ -5470,17 +5568,20 @@
       <c r="BA51" s="42">
         <v>1</v>
       </c>
-      <c r="BB51" s="79" t="s">
+      <c r="BB51" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC51" s="79" t="s">
         <v>56</v>
-      </c>
-      <c r="BC51" s="42" t="s">
-        <v>50</v>
       </c>
       <c r="BD51" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BE51" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="52" spans="3:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:57" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="3" t="s">
         <v>51</v>
       </c>
@@ -5582,17 +5683,20 @@
       <c r="BA52" s="42">
         <v>0</v>
       </c>
-      <c r="BB52" s="40" t="s">
+      <c r="BB52" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC52" s="40" t="s">
         <v>54</v>
-      </c>
-      <c r="BC52" s="42" t="s">
-        <v>50</v>
       </c>
       <c r="BD52" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BE52" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="53" spans="3:56" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:57" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="3" t="s">
         <v>51</v>
       </c>
@@ -5694,17 +5798,20 @@
       <c r="BA53" s="42">
         <v>0</v>
       </c>
-      <c r="BB53" s="40" t="s">
+      <c r="BB53" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC53" s="40" t="s">
         <v>54</v>
-      </c>
-      <c r="BC53" s="42" t="s">
-        <v>50</v>
       </c>
       <c r="BD53" s="42" t="s">
         <v>50</v>
       </c>
+      <c r="BE53" s="42" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="54" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="3" t="s">
         <v>51</v>
       </c>
@@ -5806,17 +5913,20 @@
       <c r="BA54" s="42">
         <v>0</v>
       </c>
-      <c r="BB54" s="40" t="s">
+      <c r="BB54" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC54" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="BC54" s="37" t="s">
+      <c r="BD54" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD54" s="42" t="s">
+      <c r="BE54" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="3" t="s">
         <v>51</v>
       </c>
@@ -5922,17 +6032,20 @@
       <c r="BA55" s="42">
         <v>0</v>
       </c>
-      <c r="BB55" s="37" t="s">
+      <c r="BB55" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC55" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="BC55" s="37" t="s">
+      <c r="BD55" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="BD55" s="42" t="s">
+      <c r="BE55" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="3" t="s">
         <v>51</v>
       </c>
@@ -6038,17 +6151,20 @@
       <c r="BA56" s="42">
         <v>0</v>
       </c>
-      <c r="BB56" s="42" t="s">
+      <c r="BB56" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC56" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="BC56" s="42" t="s">
+      <c r="BD56" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="BD56" s="42" t="s">
+      <c r="BE56" s="42" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="3" t="s">
         <v>51</v>
       </c>
@@ -6154,17 +6270,20 @@
       <c r="BA57" s="42">
         <v>0</v>
       </c>
-      <c r="BB57" s="42" t="s">
+      <c r="BB57" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC57" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="BC57" s="42" t="s">
+      <c r="BD57" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="BD57" s="42" t="s">
+      <c r="BE57" s="42" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
         <v>51</v>
       </c>
@@ -6270,17 +6389,20 @@
       <c r="BA58" s="42">
         <v>0</v>
       </c>
-      <c r="BB58" s="42" t="s">
+      <c r="BB58" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC58" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="BC58" s="42" t="s">
+      <c r="BD58" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="BD58" s="42" t="s">
+      <c r="BE58" s="42" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="3" t="s">
         <v>51</v>
       </c>
@@ -6386,17 +6508,20 @@
       <c r="BA59" s="42">
         <v>0</v>
       </c>
-      <c r="BB59" s="42" t="s">
+      <c r="BB59" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC59" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="BC59" s="42" t="s">
+      <c r="BD59" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="BD59" s="42" t="s">
+      <c r="BE59" s="42" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="3" t="s">
         <v>51</v>
       </c>
@@ -6502,17 +6627,20 @@
       <c r="BA60" s="42">
         <v>0</v>
       </c>
-      <c r="BB60" s="42" t="s">
+      <c r="BB60" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC60" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="BC60" s="42" t="s">
+      <c r="BD60" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="BD60" s="42" t="s">
+      <c r="BE60" s="42" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="3" t="s">
         <v>51</v>
       </c>
@@ -6610,20 +6738,238 @@
       <c r="BA61" s="42">
         <v>0</v>
       </c>
-      <c r="BB61" s="41" t="s">
+      <c r="BB61" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC61" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="BC61" s="37" t="s">
+      <c r="BD61" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="BD61" s="42" t="s">
+      <c r="BE61" s="42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D62" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="E62" s="54"/>
+      <c r="F62" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="I62" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="J62" s="51"/>
+      <c r="K62" s="51"/>
+      <c r="L62" s="51"/>
+      <c r="M62" s="51"/>
+      <c r="N62" s="51"/>
+      <c r="O62" s="51"/>
+      <c r="P62" s="51"/>
+      <c r="Q62" s="51"/>
+      <c r="R62" s="51"/>
+      <c r="S62" s="51"/>
+      <c r="T62" s="51"/>
+      <c r="U62" s="51"/>
+      <c r="V62" s="51"/>
+      <c r="W62" s="51"/>
+      <c r="X62" s="51"/>
+      <c r="Y62" s="51"/>
+      <c r="Z62" s="51"/>
+      <c r="AA62" s="51"/>
+      <c r="AB62" s="52"/>
+      <c r="AC62" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD62" s="51"/>
+      <c r="AE62" s="51"/>
+      <c r="AF62" s="51"/>
+      <c r="AG62" s="52"/>
+      <c r="AH62" s="46">
+        <v>0</v>
+      </c>
+      <c r="AI62" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ62" s="44">
+        <v>1</v>
+      </c>
+      <c r="AK62" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL62" s="44">
+        <v>1</v>
+      </c>
+      <c r="AM62" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN62" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP62" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ62" s="53"/>
+      <c r="AR62" s="48">
+        <v>0</v>
+      </c>
+      <c r="AS62" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT62" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU62" s="49">
+        <v>1</v>
+      </c>
+      <c r="AW62" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX62" s="42">
+        <v>1</v>
+      </c>
+      <c r="AY62" s="42">
+        <v>1</v>
+      </c>
+      <c r="AZ62" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA62" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB62" s="42">
+        <v>0</v>
+      </c>
+      <c r="BC62" s="41">
+        <v>0</v>
+      </c>
+      <c r="BD62" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="BE62" s="42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="3:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D63" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="E63" s="54"/>
+      <c r="F63" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="I63" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="J63" s="51"/>
+      <c r="K63" s="51"/>
+      <c r="L63" s="51"/>
+      <c r="M63" s="51"/>
+      <c r="N63" s="51"/>
+      <c r="O63" s="51"/>
+      <c r="P63" s="51"/>
+      <c r="Q63" s="51"/>
+      <c r="R63" s="51"/>
+      <c r="S63" s="51"/>
+      <c r="T63" s="51"/>
+      <c r="U63" s="51"/>
+      <c r="V63" s="51"/>
+      <c r="W63" s="51"/>
+      <c r="X63" s="51"/>
+      <c r="Y63" s="51"/>
+      <c r="Z63" s="51"/>
+      <c r="AA63" s="51"/>
+      <c r="AB63" s="52"/>
+      <c r="AC63" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD63" s="51"/>
+      <c r="AE63" s="51"/>
+      <c r="AF63" s="51"/>
+      <c r="AG63" s="52"/>
+      <c r="AH63" s="46">
+        <v>0</v>
+      </c>
+      <c r="AI63" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ63" s="44">
+        <v>1</v>
+      </c>
+      <c r="AK63" s="44">
+        <v>0</v>
+      </c>
+      <c r="AL63" s="44">
+        <v>1</v>
+      </c>
+      <c r="AM63" s="44">
+        <v>1</v>
+      </c>
+      <c r="AN63" s="47">
+        <v>1</v>
+      </c>
+      <c r="AP63" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ63" s="53"/>
+      <c r="AR63" s="48">
+        <v>0</v>
+      </c>
+      <c r="AS63" s="27">
+        <v>0</v>
+      </c>
+      <c r="AT63" s="27">
+        <v>1</v>
+      </c>
+      <c r="AU63" s="49">
+        <v>1</v>
+      </c>
+      <c r="AW63" s="42">
+        <v>1</v>
+      </c>
+      <c r="AX63" s="42">
+        <v>1</v>
+      </c>
+      <c r="AY63" s="42">
+        <v>1</v>
+      </c>
+      <c r="AZ63" s="42">
+        <v>0</v>
+      </c>
+      <c r="BA63" s="42">
+        <v>0</v>
+      </c>
+      <c r="BB63" s="42">
+        <v>1</v>
+      </c>
+      <c r="BC63" s="41">
+        <v>10</v>
+      </c>
+      <c r="BD63" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="BE63" s="42" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="233">
+  <mergeCells count="241">
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="I63:AB63"/>
+    <mergeCell ref="AC63:AG63"/>
+    <mergeCell ref="AP63:AQ63"/>
     <mergeCell ref="AC60:AF60"/>
     <mergeCell ref="AP60:AQ60"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="AC62:AG62"/>
+    <mergeCell ref="AP62:AQ62"/>
+    <mergeCell ref="I62:AB62"/>
     <mergeCell ref="AP57:AQ57"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="J59:O59"/>
@@ -6661,7 +7007,7 @@
     <mergeCell ref="U51:Y51"/>
     <mergeCell ref="AC51:AG51"/>
     <mergeCell ref="AP51:AQ51"/>
-    <mergeCell ref="AW25:BB25"/>
+    <mergeCell ref="AW25:BC25"/>
     <mergeCell ref="AP27:AQ27"/>
     <mergeCell ref="AP28:AQ28"/>
     <mergeCell ref="AP37:AQ37"/>

</xml_diff>